<commit_message>
Creato VEICOLI9.xlsx per coprire tutte le zone (nessun veicolo ha più di 1 zona associata)
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,7 +512,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>250866</v>
+        <v>251129</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -520,10 +520,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D2" t="n">
-        <v>104.4081632653061</v>
+        <v>146.7959183673469</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -532,21 +532,21 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-04-10 09:00:00</t>
+          <t>2025-04-10 09:05:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-04-10 09:00:00</t>
+          <t>2025-04-10 09:05:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-04-10 10:44:24</t>
+          <t>2025-04-10 11:31:47</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>5116</v>
+        <v>7193</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -555,17 +555,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L2" t="n">
+        <v>5</v>
+      </c>
+      <c r="M2" t="n">
+        <v>76</v>
+      </c>
+      <c r="N2" t="n">
         <v>6</v>
-      </c>
-      <c r="M2" t="n">
-        <v>70</v>
-      </c>
-      <c r="N2" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -628,7 +628,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>243569</v>
+        <v>243335</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -636,10 +636,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D4" t="n">
-        <v>40.640625</v>
+        <v>515.6875</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -648,21 +648,21 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-04-10 09:59:00</t>
+          <t>2025-04-10 10:16:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-04-10 09:59:00</t>
+          <t>2025-04-10 10:16:00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-04-10 10:39:38</t>
+          <t>2025-04-11 10:51:41</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2601</v>
+        <v>33004</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -675,52 +675,52 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M4" t="n">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="N4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251088</v>
+        <v>243569</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D5" t="n">
-        <v>89.6376811594203</v>
+        <v>36.63380281690141</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-10 10:31:19</t>
+          <t>2025-04-10 10:00:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-04-10 11:06:19</t>
+          <t>2025-04-10 10:48:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-04-10 11:06:19</t>
+          <t>2025-04-10 10:48:00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-04-10 12:35:57</t>
+          <t>2025-04-10 11:24:38</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>6185</v>
+        <v>2601</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -729,14 +729,14 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L5" t="n">
         <v>3</v>
       </c>
       <c r="M5" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N5" t="n">
         <v>4</v>
@@ -744,41 +744,41 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251204</v>
+        <v>251025</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D6" t="n">
-        <v>119.734375</v>
+        <v>60.39130434782609</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-04-10 10:39:38</t>
+          <t>2025-04-10 10:31:19</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-04-10 11:11:38</t>
+          <t>2025-04-10 11:06:19</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-04-10 11:11:38</t>
+          <t>2025-04-10 11:06:19</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-04-10 13:11:22</t>
+          <t>2025-04-10 12:06:42</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>7663</v>
+        <v>4167</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -791,18 +791,18 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" t="n">
         <v>70</v>
       </c>
       <c r="N6" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251346</v>
+        <v>251033</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -813,7 +813,7 @@
         <v>36.5</v>
       </c>
       <c r="D7" t="n">
-        <v>70.16363636363636</v>
+        <v>111.7454545454545</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -832,11 +832,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-04-10 12:27:39</t>
+          <t>2025-04-10 13:09:14</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>3859</v>
+        <v>6146</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -849,52 +849,52 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
       </c>
       <c r="N7" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251550</v>
+        <v>251094</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D8" t="n">
-        <v>727.5714285714286</v>
+        <v>190.0985915492958</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-04-10 10:44:24</t>
+          <t>2025-04-10 11:24:38</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-04-10 11:34:24</t>
+          <t>2025-04-10 11:56:38</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-04-10 11:34:24</t>
+          <t>2025-04-10 11:56:38</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-04-14 07:41:58</t>
+          <t>2025-04-11 07:06:43</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>35651</v>
+        <v>13497</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -903,56 +903,56 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M8" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251109</v>
+        <v>250866</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="D9" t="n">
-        <v>266.5915492957747</v>
+        <v>104.4081632653061</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-04-10 13:25:00</t>
+          <t>2025-04-10 11:31:47</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-04-11 07:17:00</t>
+          <t>2025-04-10 12:13:47</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-04-11 07:17:00</t>
+          <t>2025-04-10 12:13:47</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-04-11 11:43:35</t>
+          <t>2025-04-10 13:58:12</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>18928</v>
+        <v>5116</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -961,17 +961,829 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
       <c r="N9" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>251088</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>R9</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>25</v>
+      </c>
+      <c r="D10" t="n">
+        <v>89.6376811594203</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-04-10 12:06:42</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-04-10 12:31:42</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-04-10 12:31:42</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:01:20</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>6185</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M10" t="n">
+        <v>70</v>
+      </c>
+      <c r="N10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>251204</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CASON</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>139.3272727272727</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-04-10 13:09:14</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-04-10 13:39:44</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-04-10 13:39:44</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025-04-11 07:59:04</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>7663</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>2</v>
+      </c>
+      <c r="M11" t="n">
+        <v>70</v>
+      </c>
+      <c r="N11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>251100</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>52</v>
+      </c>
+      <c r="D12" t="n">
+        <v>65.64788732394366</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-04-10 13:25:00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:17:00</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:17:00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025-04-11 07:22:38</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>4661</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>4</v>
+      </c>
+      <c r="M12" t="n">
+        <v>70</v>
+      </c>
+      <c r="N12" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>251097</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>50</v>
+      </c>
+      <c r="D13" t="n">
+        <v>354.3061224489796</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-04-10 13:58:12</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:48:12</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:48:12</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2025-04-11 12:42:30</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>17361</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>3</v>
+      </c>
+      <c r="M13" t="n">
+        <v>70</v>
+      </c>
+      <c r="N13" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>251327</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R9</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" t="n">
+        <v>242.6666666666667</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:01:20</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:31:20</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:31:20</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2025-04-11 10:34:00</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>16744</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>4</v>
+      </c>
+      <c r="M14" t="n">
+        <v>70</v>
+      </c>
+      <c r="N14" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>251346</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BIMEC 4</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>39</v>
+      </c>
+      <c r="D15" t="n">
+        <v>63.26229508196721</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:16:00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:55:00</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:55:00</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2025-04-11 07:58:15</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>3859</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>8</v>
+      </c>
+      <c r="M15" t="n">
+        <v>70</v>
+      </c>
+      <c r="N15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>250780</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BIMEC 5</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>40</v>
+      </c>
+      <c r="D16" t="n">
+        <v>368.056338028169</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:19:00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:59:00</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:59:00</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2025-04-11 13:07:03</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>26132</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>10</v>
+      </c>
+      <c r="M16" t="n">
+        <v>70</v>
+      </c>
+      <c r="N16" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>251550</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>R10</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>125</v>
+      </c>
+      <c r="D17" t="n">
+        <v>584.4426229508197</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2025-04-10 14:33:00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-04-11 08:38:00</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-04-11 08:38:00</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2025-04-14 10:22:26</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>35651</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>3</v>
+      </c>
+      <c r="M17" t="n">
+        <v>70</v>
+      </c>
+      <c r="N17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>251281</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>50</v>
+      </c>
+      <c r="D18" t="n">
+        <v>230.1408450704225</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2025-04-11 07:22:38</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-04-11 08:12:38</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-04-11 08:12:38</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2025-04-11 12:02:47</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>16340</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>CASON ;R6</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>7</v>
+      </c>
+      <c r="M18" t="n">
+        <v>70</v>
+      </c>
+      <c r="N18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>251280</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CASON</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>346.6</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2025-04-11 07:59:04</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-04-11 08:39:34</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-04-11 08:39:34</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2025-04-11 14:26:10</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>19063</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>CASON ;R6</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>7</v>
+      </c>
+      <c r="M19" t="n">
+        <v>70</v>
+      </c>
+      <c r="N19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>251109</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>80</v>
+      </c>
+      <c r="D20" t="n">
+        <v>266.5915492957747</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2025-04-11 12:02:47</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-04-11 13:22:47</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-04-11 13:22:47</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2025-04-14 09:49:22</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>18928</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>16</v>
+      </c>
+      <c r="M20" t="n">
+        <v>70</v>
+      </c>
+      <c r="N20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>251427</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CASON</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>445.6363636363636</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2025-04-11 14:26:10</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-04-11 14:56:40</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-04-11 14:56:40</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2025-04-14 14:22:18</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>24510</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>CASON ;R6</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>7</v>
+      </c>
+      <c r="M21" t="n">
+        <v>70</v>
+      </c>
+      <c r="N21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>251442</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>80</v>
+      </c>
+      <c r="D22" t="n">
+        <v>230.1408450704225</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2025-04-14 09:49:22</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-04-14 11:09:22</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-04-14 11:09:22</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2025-04-14 14:59:31</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>16340</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>CASON ;R6</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
+        <v>7</v>
+      </c>
+      <c r="M22" t="n">
+        <v>70</v>
+      </c>
+      <c r="N22" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>251166</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CASON</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="D23" t="n">
+        <v>297.0909090909091</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2025-04-14 14:22:18</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-04-14 14:52:48</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-04-14 14:52:48</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2025-04-15 11:49:54</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>16340</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>CASON ;R6</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>7</v>
+      </c>
+      <c r="M23" t="n">
+        <v>70</v>
+      </c>
+      <c r="N23" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alcuni cambiamenti e prove fatti con Giulia
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>250866</v>
+        <v>250344</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1216,10 +1216,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D14" t="n">
-        <v>72.05633802816901</v>
+        <v>613.9859154929577</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1228,21 +1228,21 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-04-10 14:27:00</t>
+          <t>2025-04-10 14:22:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-04-10 14:27:00</t>
+          <t>2025-04-10 14:22:00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-04-11 07:39:03</t>
+          <t>2025-04-14 08:35:59</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>5116</v>
+        <v>43593</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1255,18 +1255,18 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M14" t="n">
         <v>70</v>
       </c>
       <c r="N14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251088</v>
+        <v>250866</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1274,10 +1274,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D15" t="n">
-        <v>101.3934426229508</v>
+        <v>83.8688524590164</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1286,21 +1286,21 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-04-11 07:05:00</t>
+          <t>2025-04-10 14:59:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-04-11 07:05:00</t>
+          <t>2025-04-10 14:59:00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-04-11 08:46:23</t>
+          <t>2025-04-11 08:22:52</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>6185</v>
+        <v>5116</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251204</v>
+        <v>251088</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1332,10 +1332,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" t="n">
-        <v>107.9295774647887</v>
+        <v>87.11267605633803</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1344,21 +1344,21 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-04-10 14:55:00</t>
+          <t>2025-04-10 14:53:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-04-10 14:55:00</t>
+          <t>2025-04-10 14:53:00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-04-11 08:42:55</t>
+          <t>2025-04-11 08:20:06</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>7663</v>
+        <v>6185</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251100</v>
+        <v>251204</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D17" t="n">
-        <v>76.40983606557377</v>
+        <v>125.6229508196721</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1402,21 +1402,21 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-04-11 08:33:00</t>
+          <t>2025-04-11 08:43:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-04-11 08:33:00</t>
+          <t>2025-04-11 08:43:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-04-11 09:49:24</t>
+          <t>2025-04-11 10:48:37</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>4661</v>
+        <v>7663</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1429,18 +1429,18 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M17" t="n">
         <v>70</v>
       </c>
       <c r="N17" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251097</v>
+        <v>251100</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1448,10 +1448,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D18" t="n">
-        <v>354.3061224489796</v>
+        <v>95.12244897959184</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1460,21 +1460,21 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-04-11 07:17:48</t>
+          <t>2025-04-11 07:22:48</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-04-11 07:17:48</t>
+          <t>2025-04-11 07:22:48</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-04-11 13:12:07</t>
+          <t>2025-04-11 08:57:56</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>17361</v>
+        <v>4661</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251327</v>
+        <v>251097</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1506,10 +1506,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D19" t="n">
-        <v>242.6666666666667</v>
+        <v>251.6086956521739</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1518,21 +1518,21 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-04-11 07:50:29</t>
+          <t>2025-04-11 07:55:29</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-04-11 07:50:29</t>
+          <t>2025-04-11 07:55:29</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-04-11 11:53:09</t>
+          <t>2025-04-11 12:07:06</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>16744</v>
+        <v>17361</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1545,18 +1545,18 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19" t="n">
         <v>70</v>
       </c>
       <c r="N19" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251281</v>
+        <v>251327</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1564,10 +1564,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>32.5</v>
+        <v>34.5</v>
       </c>
       <c r="D20" t="n">
-        <v>297.0909090909091</v>
+        <v>304.4363636363636</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1576,21 +1576,21 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-04-11 08:04:26</t>
+          <t>2025-04-11 08:06:26</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-04-11 08:04:26</t>
+          <t>2025-04-11 08:06:26</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-04-11 13:01:32</t>
+          <t>2025-04-11 13:10:52</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>16340</v>
+        <v>16744</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1599,56 +1599,56 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
         <v>70</v>
       </c>
       <c r="N20" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>250986</v>
+        <v>251402</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>185</v>
+        <v>19</v>
       </c>
       <c r="D21" t="n">
-        <v>282.7183098591549</v>
+        <v>139.5774647887324</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-04-11 07:39:03</t>
+          <t>2025-04-11 08:20:06</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-04-11 10:44:03</t>
+          <t>2025-04-11 08:39:06</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-04-11 10:44:03</t>
+          <t>2025-04-11 08:39:06</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-04-14 07:26:46</t>
+          <t>2025-04-11 10:58:41</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>20073</v>
+        <v>9910</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1657,11 +1657,11 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="M21" t="n">
         <v>70</v>
@@ -1672,41 +1672,41 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251402</v>
+        <v>251346</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D22" t="n">
-        <v>139.5774647887324</v>
+        <v>63.26229508196721</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-04-11 08:42:55</t>
+          <t>2025-04-11 08:22:52</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-04-11 09:03:55</t>
+          <t>2025-04-11 08:51:52</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-04-11 09:03:55</t>
+          <t>2025-04-11 08:51:52</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-04-11 11:23:30</t>
+          <t>2025-04-11 09:55:07</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>9910</v>
+        <v>3859</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M22" t="n">
         <v>70</v>
@@ -1730,41 +1730,41 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251346</v>
+        <v>251550</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D23" t="n">
-        <v>63.26229508196721</v>
+        <v>727.5714285714286</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-04-11 08:46:23</t>
+          <t>2025-04-11 08:57:56</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-04-11 09:21:23</t>
+          <t>2025-04-11 09:37:56</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-04-11 09:21:23</t>
+          <t>2025-04-11 09:37:56</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-04-11 10:24:39</t>
+          <t>2025-04-14 13:45:30</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>3859</v>
+        <v>35651</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1777,52 +1777,52 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M23" t="n">
         <v>70</v>
       </c>
       <c r="N23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251550</v>
+        <v>250780</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D24" t="n">
-        <v>584.4426229508197</v>
+        <v>428.3934426229508</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-04-11 09:49:24</t>
+          <t>2025-04-11 09:55:07</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-04-11 10:14:24</t>
+          <t>2025-04-11 10:24:07</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-04-11 10:14:24</t>
+          <t>2025-04-11 10:24:07</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-04-14 11:58:51</t>
+          <t>2025-04-14 09:32:31</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>35651</v>
+        <v>26132</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1831,56 +1831,56 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M24" t="n">
         <v>70</v>
       </c>
       <c r="N24" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>250780</v>
+        <v>251250</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D25" t="n">
-        <v>428.3934426229508</v>
+        <v>130</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-04-11 10:24:39</t>
+          <t>2025-04-11 10:48:37</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-04-11 10:53:39</t>
+          <t>2025-04-11 11:28:37</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-04-11 10:53:39</t>
+          <t>2025-04-11 11:28:37</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-04-14 10:02:02</t>
+          <t>2025-04-11 13:38:37</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>26132</v>
+        <v>7930</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1889,22 +1889,22 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M25" t="n">
         <v>70</v>
       </c>
       <c r="N25" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251250</v>
+        <v>251522</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1915,7 +1915,7 @@
         <v>34</v>
       </c>
       <c r="D26" t="n">
-        <v>123.90625</v>
+        <v>610.953125</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1934,11 +1934,11 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-04-11 13:29:35</t>
+          <t>2025-04-14 13:36:38</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>7930</v>
+        <v>39101</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1947,56 +1947,56 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M26" t="n">
         <v>70</v>
       </c>
       <c r="N26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251522</v>
+        <v>251281</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>21</v>
+        <v>36.5</v>
       </c>
       <c r="D27" t="n">
-        <v>550.7183098591549</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-04-11 11:23:30</t>
+          <t>2025-04-11 13:10:52</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-04-11 11:44:30</t>
+          <t>2025-04-11 13:47:22</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-04-11 11:44:30</t>
+          <t>2025-04-11 13:47:22</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-04-14 12:55:13</t>
+          <t>2025-04-14 10:44:28</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>39101</v>
+        <v>16340</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2005,56 +2005,56 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L27" t="n">
+        <v>7</v>
+      </c>
+      <c r="M27" t="n">
+        <v>70</v>
+      </c>
+      <c r="N27" t="n">
         <v>2</v>
-      </c>
-      <c r="M27" t="n">
-        <v>70</v>
-      </c>
-      <c r="N27" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251280</v>
+        <v>250986</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>30.5</v>
+        <v>190</v>
       </c>
       <c r="D28" t="n">
-        <v>346.6</v>
+        <v>282.7183098591549</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-04-11 13:01:32</t>
+          <t>2025-04-14 08:35:59</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-04-11 13:32:02</t>
+          <t>2025-04-14 11:45:59</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-04-11 13:32:02</t>
+          <t>2025-04-14 11:45:59</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-04-14 11:18:38</t>
+          <t>2025-04-15 08:28:42</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>19063</v>
+        <v>20073</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2063,56 +2063,56 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="M28" t="n">
         <v>70</v>
       </c>
       <c r="N28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251109</v>
+        <v>251280</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>135</v>
+        <v>30.5</v>
       </c>
       <c r="D29" t="n">
-        <v>266.5915492957747</v>
+        <v>346.6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-04-14 07:26:46</t>
+          <t>2025-04-14 10:44:28</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-04-14 09:41:46</t>
+          <t>2025-04-14 11:14:58</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-04-14 09:41:46</t>
+          <t>2025-04-14 11:14:58</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-04-14 14:08:21</t>
+          <t>2025-04-15 09:01:34</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>18928</v>
+        <v>19063</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2121,56 +2121,56 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="M29" t="n">
         <v>70</v>
       </c>
       <c r="N29" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251427</v>
+        <v>251109</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>30.5</v>
+        <v>135</v>
       </c>
       <c r="D30" t="n">
-        <v>445.6363636363636</v>
+        <v>266.5915492957747</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-04-14 11:18:38</t>
+          <t>2025-04-15 08:28:42</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-04-14 11:49:08</t>
+          <t>2025-04-15 10:43:42</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-04-14 11:49:08</t>
+          <t>2025-04-15 10:43:42</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-04-15 11:14:46</t>
+          <t>2025-04-16 07:10:17</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>24510</v>
+        <v>18928</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2179,56 +2179,56 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L30" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="M30" t="n">
         <v>70</v>
       </c>
       <c r="N30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>251442</v>
+        <v>251427</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>80</v>
+        <v>30.5</v>
       </c>
       <c r="D31" t="n">
-        <v>230.1408450704225</v>
+        <v>445.6363636363636</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-04-14 14:08:21</t>
+          <t>2025-04-15 09:01:34</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-04-15 07:28:21</t>
+          <t>2025-04-15 09:32:04</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-04-15 07:28:21</t>
+          <t>2025-04-15 09:32:04</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-04-15 11:18:30</t>
+          <t>2025-04-16 08:57:42</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>16340</v>
+        <v>24510</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2252,37 +2252,37 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>251166</v>
+        <v>251442</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>30.5</v>
+        <v>80</v>
       </c>
       <c r="D32" t="n">
-        <v>297.0909090909091</v>
+        <v>230.1408450704225</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-04-15 11:14:46</t>
+          <t>2025-04-16 07:10:17</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-04-15 11:45:16</t>
+          <t>2025-04-16 08:30:17</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-04-15 11:45:16</t>
+          <t>2025-04-16 08:30:17</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-04-16 08:42:21</t>
+          <t>2025-04-16 12:20:26</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2305,6 +2305,64 @@
         <v>70</v>
       </c>
       <c r="N32" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>251166</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CASON</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="D33" t="n">
+        <v>297.0909090909091</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2025-04-16 08:57:42</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-04-16 09:28:12</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-04-16 09:28:12</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2025-04-16 14:25:18</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>16340</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>CASON ;R6</t>
+        </is>
+      </c>
+      <c r="L33" t="n">
+        <v>7</v>
+      </c>
+      <c r="M33" t="n">
+        <v>70</v>
+      </c>
+      <c r="N33" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiornato funzionamento della priorità (ordine invertito), aggiornato check 3 (in base al nuovo comportamneto della priorità), aggiornato README, aggiornata archiviazione cartelle
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -512,7 +512,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251168</v>
+        <v>251308</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="n">
-        <v>142.3114754098361</v>
+        <v>81.9672131147541</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -542,11 +542,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-04-24 09:42:18</t>
+          <t>2025-04-24 08:41:58</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>8681</v>
+        <v>5000</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251167</v>
+        <v>251168</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -633,30 +633,30 @@
         <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>173.655737704918</v>
+        <v>142.3114754098361</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-04-24 09:42:18</t>
+          <t>2025-04-24 08:41:58</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-04-24 10:02:18</t>
+          <t>2025-04-24 09:01:58</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-04-24 10:02:18</t>
+          <t>2025-04-24 09:01:58</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-04-24 12:55:58</t>
+          <t>2025-04-24 11:24:16</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>10593</v>
+        <v>8681</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251308</v>
+        <v>251167</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -688,21 +688,21 @@
         <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>81.9672131147541</v>
+        <v>173.655737704918</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-24 12:55:58</t>
+          <t>2025-04-24 11:24:16</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-04-24 13:15:58</t>
+          <t>2025-04-24 11:44:16</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-04-24 13:15:58</t>
+          <t>2025-04-24 11:44:16</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>5000</v>
+        <v>10593</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Cambiamenti finali del giorno
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>243569</v>
+        <v>243335</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1950,10 +1950,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" t="n">
-        <v>42.63934426229508</v>
+        <v>541.0491803278688</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1962,21 +1962,21 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-04-28 12:21:36</t>
+          <t>2025-04-28 12:19:36</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-04-28 12:21:36</t>
+          <t>2025-04-28 12:19:36</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-04-28 13:04:14</t>
+          <t>2025-04-29 13:20:39</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>2601</v>
+        <v>33004</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1989,13 +1989,13 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M28" t="n">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="N28" t="n">
-        <v>3</v>
+        <v>39705</v>
       </c>
     </row>
     <row r="29">
@@ -2053,7 +2053,7 @@
         <v>70</v>
       </c>
       <c r="N29" t="n">
-        <v>3</v>
+        <v>39710</v>
       </c>
     </row>
     <row r="30">
@@ -2111,46 +2111,46 @@
         <v>70</v>
       </c>
       <c r="N30" t="n">
-        <v>3</v>
+        <v>39710</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>251053</v>
+        <v>251072</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D31" t="n">
-        <v>187.7377049180328</v>
+        <v>82.28169014084507</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-04-28 13:04:14</t>
+          <t>2025-04-28 13:49:27</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-04-28 13:46:14</t>
+          <t>2025-04-28 14:06:27</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-04-28 13:46:14</t>
+          <t>2025-04-28 14:06:27</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-04-29 08:53:59</t>
+          <t>2025-04-29 07:28:44</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>11452</v>
+        <v>5842</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2163,52 +2163,52 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M31" t="n">
         <v>70</v>
       </c>
       <c r="N31" t="n">
-        <v>3</v>
+        <v>39705</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>250819</v>
+        <v>251126</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C32" t="n">
         <v>19</v>
       </c>
       <c r="D32" t="n">
-        <v>120.0985915492958</v>
+        <v>156.40625</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-04-28 13:49:27</t>
+          <t>2025-04-28 13:50:02</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-04-28 14:08:27</t>
+          <t>2025-04-28 14:09:02</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-04-28 14:08:27</t>
+          <t>2025-04-28 14:09:02</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-04-29 08:08:33</t>
+          <t>2025-04-29 08:45:27</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>8527</v>
+        <v>10010</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2221,245 +2221,13 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M32" t="n">
         <v>70</v>
       </c>
       <c r="N32" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>251346</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>BIMEC 2</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>19</v>
-      </c>
-      <c r="D33" t="n">
-        <v>60.296875</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>2025-04-28 13:50:02</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>2025-04-28 14:09:02</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>2025-04-28 14:09:02</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>2025-04-29 07:09:20</t>
-        </is>
-      </c>
-      <c r="I33" t="n">
-        <v>3859</v>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L33" t="n">
-        <v>8</v>
-      </c>
-      <c r="M33" t="n">
-        <v>70</v>
-      </c>
-      <c r="N33" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>251550</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>R3</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>40</v>
-      </c>
-      <c r="D34" t="n">
-        <v>727.5714285714286</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>2025-04-28 13:59:23</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>2025-04-28 14:39:23</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>2025-04-28 14:39:23</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>2025-04-30 10:46:57</t>
-        </is>
-      </c>
-      <c r="I34" t="n">
-        <v>35651</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L34" t="n">
-        <v>3</v>
-      </c>
-      <c r="M34" t="n">
-        <v>70</v>
-      </c>
-      <c r="N34" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>251109</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>R6</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>85</v>
-      </c>
-      <c r="D35" t="n">
-        <v>266.5915492957747</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>2025-04-28 14:17:23</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>2025-04-29 07:42:23</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>2025-04-29 07:42:23</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>2025-04-29 12:08:59</t>
-        </is>
-      </c>
-      <c r="I35" t="n">
-        <v>18928</v>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>R6</t>
-        </is>
-      </c>
-      <c r="L35" t="n">
-        <v>16</v>
-      </c>
-      <c r="M35" t="n">
-        <v>70</v>
-      </c>
-      <c r="N35" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>251846</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>CASON</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>38.5</v>
-      </c>
-      <c r="D36" t="n">
-        <v>207.1272727272727</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>2025-04-28 14:19:50</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>2025-04-28 14:58:20</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>2025-04-28 14:58:20</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>2025-04-29 10:25:27</t>
-        </is>
-      </c>
-      <c r="I36" t="n">
-        <v>11392</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L36" t="n">
-        <v>2</v>
-      </c>
-      <c r="M36" t="n">
-        <v>70</v>
-      </c>
-      <c r="N36" t="n">
-        <v>3</v>
+        <v>39705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funziona euristico, male ricerche locali
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Veicolo esterno</t>
+          <t>Veicolo esterno aperto</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Veicolo esterno</t>
+          <t>Veicolo esterno aperto</t>
         </is>
       </c>
     </row>
@@ -748,7 +748,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>243335</v>
+        <v>251391</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D6" t="n">
-        <v>515.6875</v>
+        <v>167.21875</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -768,21 +768,21 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-07 07:34:00</t>
+          <t>2025-05-07 07:21:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-07 07:34:00</t>
+          <t>2025-05-07 07:21:00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-08 08:09:41</t>
+          <t>2025-05-07 10:08:13</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>33004</v>
+        <v>10702</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -791,56 +791,56 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M6" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N6" t="n">
-        <v>39755</v>
+        <v>39754</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251247</v>
+        <v>251742</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D7" t="n">
-        <v>379.3521126760563</v>
+        <v>128.53125</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 10:08:13</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-08 07:38:00</t>
+          <t>2025-05-07 10:25:13</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-08 07:38:00</t>
+          <t>2025-05-07 10:25:13</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-08 13:57:21</t>
+          <t>2025-05-07 12:33:45</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>26934</v>
+        <v>8226</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -849,11 +849,11 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
@@ -864,41 +864,41 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251391</v>
+        <v>245275</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D8" t="n">
-        <v>175.4426229508197</v>
+        <v>352.078125</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 12:33:45</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-07 13:08:45</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-07 13:08:45</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-08 10:25:26</t>
+          <t>2025-05-08 11:00:49</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>10702</v>
+        <v>22533</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -907,11 +907,11 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;CASON ;R6</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
@@ -926,14 +926,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="D9" t="n">
-        <v>234.5102040816327</v>
+        <v>161.8450704225352</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -942,17 +942,17 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:52:00</t>
+          <t>2025-05-08 07:21:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:52:00</t>
+          <t>2025-05-08 07:21:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 11:46:30</t>
+          <t>2025-05-08 10:02:50</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -980,41 +980,41 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>245275</v>
+        <v>251416</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D10" t="n">
-        <v>352.078125</v>
+        <v>183.9672131147541</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-08 08:09:41</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 08:59:41</t>
+          <t>2025-05-08 07:25:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 08:59:41</t>
+          <t>2025-05-08 07:25:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 14:51:45</t>
+          <t>2025-05-08 10:28:58</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>22533</v>
+        <v>11222</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1023,56 +1023,56 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
       </c>
       <c r="N10" t="n">
-        <v>39754</v>
+        <v>39755</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251840</v>
+        <v>251340</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D11" t="n">
-        <v>93.67213114754098</v>
+        <v>669.3877551020408</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 10:25:26</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 10:45:26</t>
+          <t>2025-05-08 07:37:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 10:45:26</t>
+          <t>2025-05-08 07:37:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:06</t>
+          <t>2025-05-09 10:46:23</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>5714</v>
+        <v>32800</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1081,17 +1081,19 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M11" t="n">
-        <v>70</v>
-      </c>
-      <c r="N11" t="n">
-        <v>39755</v>
+        <v>76</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -1100,33 +1102,33 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>955.7142857142857</v>
+        <v>659.5774647887324</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 11:46:30</t>
+          <t>2025-05-08 10:02:50</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:30</t>
+          <t>2025-05-08 10:17:50</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:30</t>
+          <t>2025-05-08 10:17:50</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-12 12:17:13</t>
+          <t>2025-05-09 13:17:25</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1154,41 +1156,41 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>245623</v>
+        <v>251840</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D13" t="n">
-        <v>372.0985915492957</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 10:28:58</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:30:00</t>
+          <t>2025-05-08 11:03:58</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:30:00</t>
+          <t>2025-05-08 11:03:58</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-09 10:42:05</t>
+          <t>2025-05-08 12:37:38</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>26419</v>
+        <v>5714</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1197,58 +1199,56 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M13" t="n">
-        <v>152</v>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N13" t="n">
+        <v>39755</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251795</v>
+        <v>245623</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="D14" t="n">
-        <v>307.1967213114754</v>
+        <v>412.796875</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:06</t>
+          <t>2025-05-08 11:00:49</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:44:06</t>
+          <t>2025-05-08 11:54:49</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:44:06</t>
+          <t>2025-05-08 11:54:49</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-09 09:51:18</t>
+          <t>2025-05-09 10:47:37</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>18739</v>
+        <v>26419</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1257,58 +1257,58 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M14" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>245090</v>
+        <v>251750</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>32</v>
       </c>
       <c r="D15" t="n">
-        <v>7277.718309859155</v>
+        <v>54.80281690140845</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-08 13:57:21</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-08 14:29:21</t>
+          <t>2025-05-08 12:32:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-08 14:29:21</t>
+          <t>2025-05-08 12:32:00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-30 07:47:04</t>
+          <t>2025-05-08 13:26:48</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>516718</v>
+        <v>3891</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1321,54 +1321,54 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M15" t="n">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>245089</v>
+        <v>251247</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D16" t="n">
-        <v>1916.640625</v>
+        <v>441.5409836065574</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-08 14:51:45</t>
+          <t>2025-05-08 12:37:38</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-09 07:41:45</t>
+          <t>2025-05-08 13:02:38</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-09 07:41:45</t>
+          <t>2025-05-08 13:02:38</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-15 07:38:24</t>
+          <t>2025-05-09 12:24:10</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>122665</v>
+        <v>26934</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1377,58 +1377,56 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M16" t="n">
-        <v>76</v>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N16" t="n">
+        <v>39754</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251750</v>
+        <v>245090</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D17" t="n">
-        <v>63.78688524590164</v>
+        <v>7277.718309859155</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 13:26:48</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:00</t>
+          <t>2025-05-08 14:00:48</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:00</t>
+          <t>2025-05-08 14:00:48</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-09 08:43:47</t>
+          <t>2025-05-30 07:18:31</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>3891</v>
+        <v>516718</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1441,31 +1439,31 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M17" t="n">
-        <v>152</v>
+        <v>76</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251396</v>
+        <v>251795</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>38.5</v>
+        <v>46</v>
       </c>
       <c r="D18" t="n">
-        <v>41.12727272727273</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1474,21 +1472,21 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-09 07:38:30</t>
+          <t>2025-05-09 07:46:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-09 07:38:30</t>
+          <t>2025-05-09 07:46:00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-09 08:19:37</t>
+          <t>2025-05-09 12:53:11</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>2262</v>
+        <v>18739</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1497,7 +1495,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L18" t="n">
@@ -1508,47 +1506,47 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251340</v>
+        <v>245089</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D19" t="n">
-        <v>461.9718309859155</v>
+        <v>1916.640625</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 10:47:37</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-09 07:37:00</t>
+          <t>2025-05-09 11:21:37</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-09 07:37:00</t>
+          <t>2025-05-09 11:21:37</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-12 07:18:58</t>
+          <t>2025-05-15 11:18:15</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>32800</v>
+        <v>122665</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1557,18 +1555,18 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M19" t="n">
         <v>76</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
     </row>
@@ -1589,22 +1587,22 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-09 08:19:37</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-09 08:54:07</t>
+          <t>2025-05-09 07:34:30</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-09 08:54:07</t>
+          <t>2025-05-09 07:34:30</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-09 10:30:26</t>
+          <t>2025-05-09 09:10:48</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1628,47 +1626,47 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251548</v>
+        <v>251395</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D21" t="n">
-        <v>217.0819672131148</v>
+        <v>31.85915492957746</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-09 08:43:47</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-09 09:25:47</t>
+          <t>2025-05-09 07:57:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-09 09:25:47</t>
+          <t>2025-05-09 07:57:00</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-09 13:02:52</t>
+          <t>2025-05-09 08:28:51</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>13242</v>
+        <v>2262</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1681,54 +1679,54 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M21" t="n">
         <v>70</v>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251547</v>
+        <v>251396</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D22" t="n">
-        <v>215.2295081967213</v>
+        <v>31.85915492957746</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-09 09:51:18</t>
+          <t>2025-05-09 08:28:51</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-09 10:21:18</t>
+          <t>2025-05-09 09:03:51</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-09 10:21:18</t>
+          <t>2025-05-09 09:03:51</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-09 13:56:32</t>
+          <t>2025-05-09 09:35:43</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>13129</v>
+        <v>2262</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1741,20 +1739,20 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M22" t="n">
         <v>70</v>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251742</v>
+        <v>251548</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1765,30 +1763,30 @@
         <v>30.5</v>
       </c>
       <c r="D23" t="n">
-        <v>149.5636363636364</v>
+        <v>240.7636363636364</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-09 10:30:26</t>
+          <t>2025-05-09 09:10:48</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-09 11:00:56</t>
+          <t>2025-05-09 09:41:18</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-09 11:00:56</t>
+          <t>2025-05-09 09:41:18</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-09 13:30:30</t>
+          <t>2025-05-09 13:42:04</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>8226</v>
+        <v>13242</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1808,47 +1806,47 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251986</v>
+        <v>251547</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D24" t="n">
-        <v>5930.323943661971</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-09 10:42:05</t>
+          <t>2025-05-09 09:35:43</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-09 11:20:05</t>
+          <t>2025-05-09 10:20:43</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-09 11:20:05</t>
+          <t>2025-05-09 10:20:43</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-27 14:10:25</t>
+          <t>2025-05-09 13:25:38</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>421053</v>
+        <v>13129</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1857,58 +1855,58 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M24" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251395</v>
+        <v>251550</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D25" t="n">
-        <v>37.08196721311475</v>
+        <v>727.5714285714286</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-09 13:02:52</t>
+          <t>2025-05-09 10:46:23</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-09 13:31:52</t>
+          <t>2025-05-09 11:28:23</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-09 13:31:52</t>
+          <t>2025-05-09 11:28:23</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-09 14:08:57</t>
+          <t>2025-05-13 07:35:57</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>2262</v>
+        <v>35651</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1921,54 +1919,54 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M25" t="n">
         <v>70</v>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251164</v>
+        <v>251846</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>34.5</v>
+        <v>40</v>
       </c>
       <c r="D26" t="n">
-        <v>157.8363636363636</v>
+        <v>186.7540983606557</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:30:30</t>
+          <t>2025-05-09 12:24:10</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-09 14:05:00</t>
+          <t>2025-05-09 13:04:10</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-09 14:05:00</t>
+          <t>2025-05-09 13:04:10</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-12 08:42:50</t>
+          <t>2025-05-12 08:10:56</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>8681</v>
+        <v>11392</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1981,54 +1979,54 @@
         </is>
       </c>
       <c r="L26" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M26" t="n">
         <v>70</v>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251416</v>
+        <v>245350</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D27" t="n">
-        <v>183.9672131147541</v>
+        <v>458.5245901639344</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-09 13:56:32</t>
+          <t>2025-05-09 12:53:11</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-09 14:26:32</t>
+          <t>2025-05-09 13:26:11</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-09 14:26:32</t>
+          <t>2025-05-09 13:26:11</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-12 09:30:30</t>
+          <t>2025-05-12 13:04:43</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>11222</v>
+        <v>27970</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2037,58 +2035,58 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M27" t="n">
         <v>70</v>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>244023</v>
+        <v>235572</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D28" t="n">
-        <v>16.34426229508197</v>
+        <v>140.2535211267606</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-09 14:08:57</t>
+          <t>2025-05-09 13:17:25</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-09 14:33:57</t>
+          <t>2025-05-09 13:47:25</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-09 14:33:57</t>
+          <t>2025-05-09 13:47:25</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-09 14:50:17</t>
+          <t>2025-05-12 08:07:40</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>997</v>
+        <v>9958</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2097,58 +2095,58 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M28" t="n">
         <v>70</v>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251846</v>
+        <v>251164</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D29" t="n">
-        <v>186.7540983606557</v>
+        <v>122.2676056338028</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-09 14:50:17</t>
+          <t>2025-05-09 13:25:38</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-12 07:23:17</t>
+          <t>2025-05-09 14:10:38</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-12 07:23:17</t>
+          <t>2025-05-09 14:10:38</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-12 10:30:02</t>
+          <t>2025-05-12 08:12:54</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>11392</v>
+        <v>8681</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2161,54 +2159,54 @@
         </is>
       </c>
       <c r="L29" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M29" t="n">
         <v>70</v>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251283</v>
+        <v>250819</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>45</v>
+        <v>34.5</v>
       </c>
       <c r="D30" t="n">
-        <v>10.92753623188406</v>
+        <v>155.0363636363636</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 13:42:04</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-12 07:45:00</t>
+          <t>2025-05-09 14:16:34</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-12 07:45:00</t>
+          <t>2025-05-09 14:16:34</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-12 07:55:55</t>
+          <t>2025-05-12 08:51:36</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>754</v>
+        <v>8527</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2217,7 +2215,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L30" t="n">
@@ -2228,47 +2226,47 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>251284</v>
+        <v>251346</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D31" t="n">
-        <v>230.1408450704225</v>
+        <v>55.92753623188405</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-05-12 07:18:58</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-05-12 08:20:58</t>
+          <t>2025-05-12 07:55:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-05-12 08:20:58</t>
+          <t>2025-05-12 07:55:00</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-05-12 12:11:06</t>
+          <t>2025-05-12 08:50:55</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>16340</v>
+        <v>3859</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2277,58 +2275,58 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L31" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M31" t="n">
         <v>70</v>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>251245</v>
+        <v>250641</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D32" t="n">
-        <v>10.92753623188406</v>
+        <v>72.05633802816901</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-05-12 07:55:55</t>
+          <t>2025-05-12 08:07:40</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-05-12 08:20:55</t>
+          <t>2025-05-12 08:24:40</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-05-12 08:20:55</t>
+          <t>2025-05-12 08:24:40</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-05-12 08:31:51</t>
+          <t>2025-05-12 09:36:43</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>754</v>
+        <v>5116</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2337,7 +2335,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L32" t="n">
@@ -2348,47 +2346,47 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>251061</v>
+        <v>244023</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D33" t="n">
-        <v>327.8840579710145</v>
+        <v>16.34426229508197</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-05-12 08:31:51</t>
+          <t>2025-05-12 08:10:56</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-12 08:56:51</t>
+          <t>2025-05-12 08:50:56</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-05-12 08:56:51</t>
+          <t>2025-05-12 08:50:56</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-12 14:24:44</t>
+          <t>2025-05-12 09:07:16</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>22624</v>
+        <v>997</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -2397,7 +2395,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L33" t="n">
@@ -2408,47 +2406,47 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>251520</v>
+        <v>251109</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>32.5</v>
+        <v>85</v>
       </c>
       <c r="D34" t="n">
-        <v>297.0909090909091</v>
+        <v>266.5915492957747</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-05-12 08:42:50</t>
+          <t>2025-05-12 08:12:54</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-05-12 09:15:20</t>
+          <t>2025-05-12 09:37:54</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-05-12 09:15:20</t>
+          <t>2025-05-12 09:37:54</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-05-12 14:12:25</t>
+          <t>2025-05-12 14:04:29</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>16340</v>
+        <v>18928</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2457,58 +2455,58 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L34" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="M34" t="n">
         <v>70</v>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>251062</v>
+        <v>243335</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D35" t="n">
-        <v>370.8852459016393</v>
+        <v>478.3188405797101</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-05-12 09:30:30</t>
+          <t>2025-05-12 08:50:55</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-12 10:10:30</t>
+          <t>2025-05-12 09:40:55</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-05-12 10:10:30</t>
+          <t>2025-05-12 09:40:55</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-05-13 08:21:23</t>
+          <t>2025-05-13 09:39:14</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>22624</v>
+        <v>33004</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -2517,58 +2515,58 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M35" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>251246</v>
+        <v>251283</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>33</v>
+        <v>30.5</v>
       </c>
       <c r="D36" t="n">
-        <v>196.7540983606557</v>
+        <v>13.70909090909091</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-05-12 10:30:02</t>
+          <t>2025-05-12 08:51:36</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-12 11:03:02</t>
+          <t>2025-05-12 09:22:06</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-05-12 11:03:02</t>
+          <t>2025-05-12 09:22:06</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-12 14:19:48</t>
+          <t>2025-05-12 09:35:49</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>12002</v>
+        <v>754</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -2588,47 +2586,47 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>245350</v>
+        <v>251245</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D37" t="n">
-        <v>393.943661971831</v>
+        <v>12.36065573770492</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-05-12 12:11:06</t>
+          <t>2025-05-12 09:07:16</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-12 13:01:06</t>
+          <t>2025-05-12 09:27:16</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-05-12 13:01:06</t>
+          <t>2025-05-12 09:27:16</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-05-13 11:35:03</t>
+          <t>2025-05-12 09:39:38</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>27970</v>
+        <v>754</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -2637,58 +2635,58 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M37" t="n">
         <v>70</v>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>251987</v>
+        <v>251061</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>40</v>
+        <v>30.5</v>
       </c>
       <c r="D38" t="n">
-        <v>4296.448979591837</v>
+        <v>411.3454545454546</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-05-12 12:17:13</t>
+          <t>2025-05-12 09:35:49</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-05-12 12:57:13</t>
+          <t>2025-05-12 10:06:19</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-05-12 12:57:13</t>
+          <t>2025-05-12 10:06:19</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-05-23 12:33:40</t>
+          <t>2025-05-13 08:57:39</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>210526</v>
+        <v>22624</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -2697,18 +2695,858 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L38" t="n">
         <v>6</v>
       </c>
       <c r="M38" t="n">
+        <v>70</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>251246</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>BIMEC 5</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>15</v>
+      </c>
+      <c r="D39" t="n">
+        <v>169.0422535211268</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2025-05-12 09:36:43</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-05-12 09:51:43</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-05-12 09:51:43</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2025-05-12 12:40:46</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>12002</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+        </is>
+      </c>
+      <c r="L39" t="n">
+        <v>6</v>
+      </c>
+      <c r="M39" t="n">
+        <v>70</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>251458</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>R10</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>35</v>
+      </c>
+      <c r="D40" t="n">
+        <v>166.6393442622951</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2025-05-12 09:39:38</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-05-12 10:14:38</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-05-12 10:14:38</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2025-05-12 13:01:16</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>10165</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L40" t="n">
+        <v>3</v>
+      </c>
+      <c r="M40" t="n">
+        <v>70</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>251463</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BIMEC 5</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>19</v>
+      </c>
+      <c r="D41" t="n">
+        <v>98.12676056338029</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2025-05-12 12:40:46</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-05-12 12:59:46</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2025-05-12 12:59:46</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2025-05-12 14:37:54</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>6967</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L41" t="n">
+        <v>4</v>
+      </c>
+      <c r="M41" t="n">
+        <v>70</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>251464</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>R10</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>25</v>
+      </c>
+      <c r="D42" t="n">
+        <v>117.2622950819672</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2025-05-12 13:01:16</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-05-12 13:26:16</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2025-05-12 13:26:16</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:23:32</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>7153</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L42" t="n">
+        <v>4</v>
+      </c>
+      <c r="M42" t="n">
+        <v>70</v>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>251465</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>BIMEC 4</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>41</v>
+      </c>
+      <c r="D43" t="n">
+        <v>102.0655737704918</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2025-05-12 13:04:43</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-05-12 13:45:43</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2025-05-12 13:45:43</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:27:47</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>6226</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L43" t="n">
+        <v>2</v>
+      </c>
+      <c r="M43" t="n">
+        <v>70</v>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>251462</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>105</v>
+      </c>
+      <c r="D44" t="n">
+        <v>87.69014084507042</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2025-05-12 14:04:29</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:49:29</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:49:29</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2025-05-13 09:17:10</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>6226</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L44" t="n">
+        <v>2</v>
+      </c>
+      <c r="M44" t="n">
+        <v>70</v>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>251467</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BIMEC 5</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>19</v>
+      </c>
+      <c r="D45" t="n">
+        <v>87.69014084507042</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2025-05-12 14:37:54</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-05-12 14:56:54</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2025-05-12 14:56:54</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2025-05-13 08:24:35</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>6226</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L45" t="n">
+        <v>2</v>
+      </c>
+      <c r="M45" t="n">
+        <v>70</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>251568</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>R10</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>30</v>
+      </c>
+      <c r="D46" t="n">
+        <v>212</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:23:32</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:53:32</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:53:32</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2025-05-13 11:25:32</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>12932</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L46" t="n">
+        <v>2</v>
+      </c>
+      <c r="M46" t="n">
+        <v>70</v>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>251580</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>BIMEC 4</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>29</v>
+      </c>
+      <c r="D47" t="n">
+        <v>117.2622950819672</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:27:47</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:56:47</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:56:47</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2025-05-13 09:54:02</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>7153</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L47" t="n">
+        <v>4</v>
+      </c>
+      <c r="M47" t="n">
+        <v>70</v>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>251062</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>50</v>
+      </c>
+      <c r="D48" t="n">
+        <v>461.7142857142857</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:35:57</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2025-05-13 08:25:57</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2025-05-13 08:25:57</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2025-05-14 08:07:40</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>22624</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+        </is>
+      </c>
+      <c r="L48" t="n">
+        <v>6</v>
+      </c>
+      <c r="M48" t="n">
+        <v>70</v>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>251986</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>BIMEC 5</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>38</v>
+      </c>
+      <c r="D49" t="n">
+        <v>5930.323943661971</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2025-05-13 08:24:35</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2025-05-13 09:02:35</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2025-05-13 09:02:35</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2025-05-29 11:52:54</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>421053</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+        </is>
+      </c>
+      <c r="L49" t="n">
+        <v>6</v>
+      </c>
+      <c r="M49" t="n">
         <v>76</v>
       </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (solo macchina)</t>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>251284</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>CASON</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="D50" t="n">
+        <v>297.0909090909091</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2025-05-13 08:57:39</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2025-05-13 09:30:09</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2025-05-13 09:30:09</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2025-05-13 14:27:15</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>16340</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>CASON ;R6</t>
+        </is>
+      </c>
+      <c r="L50" t="n">
+        <v>7</v>
+      </c>
+      <c r="M50" t="n">
+        <v>70</v>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>251520</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>R6</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>60</v>
+      </c>
+      <c r="D51" t="n">
+        <v>230.1408450704225</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2025-05-13 09:17:10</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2025-05-13 10:17:10</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2025-05-13 10:17:10</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2025-05-13 14:07:19</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>16340</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>CASON ;R6</t>
+        </is>
+      </c>
+      <c r="L51" t="n">
+        <v>7</v>
+      </c>
+      <c r="M51" t="n">
+        <v>70</v>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>251987</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>R9</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>40</v>
+      </c>
+      <c r="D52" t="n">
+        <v>3051.101449275362</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2025-05-13 09:39:14</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2025-05-13 10:19:14</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2025-05-13 10:19:14</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2025-05-21 13:10:20</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>210526</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+        </is>
+      </c>
+      <c r="L52" t="n">
+        <v>6</v>
+      </c>
+      <c r="M52" t="n">
+        <v>76</v>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ricerche locali in loop infinito
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2228,41 +2228,41 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251561</v>
+        <v>251340</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D28" t="n">
-        <v>84.921875</v>
+        <v>461.9718309859155</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-07 07:21:00</t>
+          <t>2025-05-08 12:15:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-07 07:21:00</t>
+          <t>2025-05-08 12:15:00</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-07 08:45:55</t>
+          <t>2025-05-09 11:56:58</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>5435</v>
+        <v>32800</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2271,14 +2271,14 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M28" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N28" t="inlineStr">
         <is>
@@ -2294,41 +2294,41 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251564</v>
+        <v>251561</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29" t="n">
-        <v>42.453125</v>
+        <v>76.54929577464789</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-07 08:45:55</t>
+          <t>2025-05-09 07:27:22</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-07 09:04:55</t>
+          <t>2025-05-09 07:44:22</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-07 09:04:55</t>
+          <t>2025-05-09 07:44:22</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-07 09:47:22</t>
+          <t>2025-05-09 09:00:55</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>2717</v>
+        <v>5435</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2341,7 +2341,7 @@
         </is>
       </c>
       <c r="L29" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M29" t="n">
         <v>70</v>
@@ -2360,41 +2360,41 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251566</v>
+        <v>251564</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D30" t="n">
-        <v>107.640625</v>
+        <v>38.26760563380282</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-07 09:47:22</t>
+          <t>2025-05-09 09:00:55</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-07 10:04:22</t>
+          <t>2025-05-09 09:19:55</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-07 10:04:22</t>
+          <t>2025-05-09 09:19:55</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-07 11:52:00</t>
+          <t>2025-05-09 09:58:11</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>6889</v>
+        <v>2717</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="L30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M30" t="n">
         <v>70</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>251519</v>
+        <v>251566</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2434,33 +2434,33 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D31" t="n">
-        <v>205.859375</v>
+        <v>107.640625</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-05-07 11:52:00</t>
+          <t>2025-05-09 09:06:46</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-05-07 12:11:00</t>
+          <t>2025-05-09 09:23:46</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-05-07 12:11:00</t>
+          <t>2025-05-09 09:23:46</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-05-08 07:36:52</t>
+          <t>2025-05-09 11:11:25</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>13175</v>
+        <v>6889</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M31" t="n">
         <v>70</v>
@@ -2492,41 +2492,41 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>251340</v>
+        <v>251519</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="D32" t="n">
-        <v>461.9718309859155</v>
+        <v>268.8775510204082</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 09:14:40</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-05-08 07:15:00</t>
+          <t>2025-05-09 09:59:40</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-05-08 07:15:00</t>
+          <t>2025-05-09 09:59:40</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-05-08 14:56:58</t>
+          <t>2025-05-09 14:28:33</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>32800</v>
+        <v>13175</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2535,14 +2535,14 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L32" t="n">
         <v>2</v>
       </c>
       <c r="M32" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N32" t="inlineStr">
         <is>
@@ -2562,33 +2562,33 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D33" t="n">
-        <v>280.2295081967213</v>
+        <v>240.7605633802817</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 09:58:11</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-09 10:17:11</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-09 10:17:11</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-08 12:15:13</t>
+          <t>2025-05-09 14:17:57</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2628,33 +2628,33 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D34" t="n">
-        <v>197.1836734693877</v>
+        <v>158.3934426229508</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 10:06:22</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-05-08 07:45:00</t>
+          <t>2025-05-09 10:36:22</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-05-08 07:45:00</t>
+          <t>2025-05-09 10:36:22</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:11</t>
+          <t>2025-05-09 13:14:46</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2705,22 +2705,22 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-05-08 07:36:52</t>
+          <t>2025-05-09 11:11:25</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-08 07:53:52</t>
+          <t>2025-05-09 11:28:25</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-05-08 07:53:52</t>
+          <t>2025-05-09 11:28:25</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-05-08 09:18:47</t>
+          <t>2025-05-09 12:53:20</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -2756,41 +2756,41 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>251475</v>
+        <v>250894</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D36" t="n">
-        <v>135.640625</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-05-08 09:18:47</t>
+          <t>2025-05-09 11:56:58</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-08 09:35:47</t>
+          <t>2025-05-09 12:17:58</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-05-08 09:35:47</t>
+          <t>2025-05-09 12:17:58</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-08 11:51:26</t>
+          <t>2025-05-12 14:41:22</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>8681</v>
+        <v>44262</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -2799,19 +2799,17 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M36" t="n">
-        <v>70</v>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N36" t="n">
+        <v>39755</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
@@ -2822,41 +2820,41 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>250894</v>
+        <v>251475</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>42</v>
+        <v>36.5</v>
       </c>
       <c r="D37" t="n">
-        <v>903.3061224489796</v>
+        <v>157.8363636363636</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:11</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-08 11:44:11</t>
+          <t>2025-05-09 13:14:05</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-05-08 11:44:11</t>
+          <t>2025-05-09 13:14:05</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-05-12 10:47:29</t>
+          <t>2025-05-12 07:51:55</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>44262</v>
+        <v>8681</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -2865,17 +2863,19 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M37" t="n">
-        <v>76</v>
-      </c>
-      <c r="N37" t="n">
-        <v>39755</v>
+        <v>70</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
       <c r="O37" t="n">
         <v>0</v>
@@ -2890,33 +2890,33 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D38" t="n">
-        <v>101.03125</v>
+        <v>106</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-05-08 11:51:26</t>
+          <t>2025-05-09 12:53:11</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-05-08 12:06:26</t>
+          <t>2025-05-09 13:22:11</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-05-08 12:06:26</t>
+          <t>2025-05-09 13:22:11</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-05-08 13:47:28</t>
+          <t>2025-05-12 07:08:11</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -2952,41 +2952,41 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>251651</v>
+        <v>244354</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D39" t="n">
-        <v>659.5774647887324</v>
+        <v>67.34375</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-09 12:53:20</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:00</t>
+          <t>2025-05-09 13:10:20</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:00</t>
+          <t>2025-05-09 13:10:20</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-05-12 07:20:34</t>
+          <t>2025-05-09 14:17:41</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>46830</v>
+        <v>4310</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -2995,17 +2995,19 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M39" t="n">
-        <v>76</v>
-      </c>
-      <c r="N39" t="n">
-        <v>39755</v>
+        <v>70</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
       <c r="O39" t="n">
         <v>0</v>
@@ -3016,7 +3018,7 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>244354</v>
+        <v>244355</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -3024,29 +3026,29 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D40" t="n">
         <v>70.65573770491804</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-05-08 12:15:13</t>
+          <t>2025-05-09 13:14:46</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-05-08 12:40:13</t>
+          <t>2025-05-09 13:34:46</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-05-08 12:40:13</t>
+          <t>2025-05-09 13:34:46</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-05-08 13:50:53</t>
+          <t>2025-05-09 14:45:25</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3082,7 +3084,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>244355</v>
+        <v>244204</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -3093,30 +3095,30 @@
         <v>15</v>
       </c>
       <c r="D41" t="n">
-        <v>67.34375</v>
+        <v>54.25</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-05-08 13:47:28</t>
+          <t>2025-05-09 14:17:41</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-05-08 14:02:28</t>
+          <t>2025-05-09 14:32:41</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-05-08 14:02:28</t>
+          <t>2025-05-09 14:32:41</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-05-09 07:09:48</t>
+          <t>2025-05-12 07:26:56</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>4310</v>
+        <v>3472</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3148,41 +3150,41 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>244204</v>
+        <v>251651</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D42" t="n">
-        <v>56.91803278688525</v>
+        <v>659.5774647887324</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-05-08 13:50:53</t>
+          <t>2025-05-09 14:17:57</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-05-08 14:10:53</t>
+          <t>2025-05-09 14:47:57</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-05-08 14:10:53</t>
+          <t>2025-05-09 14:47:57</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-05-09 07:07:48</t>
+          <t>2025-05-13 09:47:32</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>3472</v>
+        <v>46830</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3191,19 +3193,17 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M42" t="n">
-        <v>70</v>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N42" t="n">
+        <v>39755</v>
       </c>
       <c r="O42" t="n">
         <v>0</v>
@@ -3218,33 +3218,33 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D43" t="n">
-        <v>151.7746478873239</v>
+        <v>219.9183673469388</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-05-08 14:56:58</t>
+          <t>2025-05-09 14:28:33</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:58</t>
+          <t>2025-05-12 07:13:33</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:58</t>
+          <t>2025-05-12 07:13:33</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-05-09 10:02:44</t>
+          <t>2025-05-12 10:53:28</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3284,33 +3284,33 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D44" t="n">
         <v>142.3114754098361</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 14:45:25</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 07:05:25</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 07:05:25</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-05-09 10:04:18</t>
+          <t>2025-05-12 09:27:44</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3346,41 +3346,41 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>251416</v>
+        <v>245623</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>30.5</v>
+        <v>30</v>
       </c>
       <c r="D45" t="n">
-        <v>204.0363636363636</v>
+        <v>382.8840579710145</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:30</t>
+          <t>2025-05-12 07:30:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:30</t>
+          <t>2025-05-12 07:30:00</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-05-09 10:54:32</t>
+          <t>2025-05-12 13:52:53</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>11222</v>
+        <v>26419</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3389,17 +3389,19 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L45" t="n">
         <v>2</v>
       </c>
       <c r="M45" t="n">
-        <v>70</v>
-      </c>
-      <c r="N45" t="n">
-        <v>39755</v>
+        <v>152</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
       <c r="O45" t="n">
         <v>0</v>
@@ -3410,41 +3412,41 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>251260</v>
+        <v>251416</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D46" t="n">
-        <v>153.5901639344262</v>
+        <v>183.9672131147541</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-05-09 07:07:48</t>
+          <t>2025-05-12 07:08:11</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-05-09 07:37:48</t>
+          <t>2025-05-12 07:37:11</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-05-09 07:37:48</t>
+          <t>2025-05-12 07:37:11</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-05-09 10:11:23</t>
+          <t>2025-05-12 10:41:09</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>9369</v>
+        <v>11222</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3453,19 +3455,17 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L46" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M46" t="n">
         <v>70</v>
       </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+      <c r="N46" t="n">
+        <v>39755</v>
       </c>
       <c r="O46" t="n">
         <v>0</v>
@@ -3476,7 +3476,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>245623</v>
+        <v>251260</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -3484,33 +3484,33 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D47" t="n">
-        <v>412.796875</v>
+        <v>146.390625</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-05-09 07:09:48</t>
+          <t>2025-05-12 07:26:56</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-05-09 07:43:48</t>
+          <t>2025-05-12 07:45:56</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-05-09 07:43:48</t>
+          <t>2025-05-12 07:45:56</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-05-09 14:36:36</t>
+          <t>2025-05-12 10:12:19</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>26419</v>
+        <v>9369</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3519,14 +3519,14 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L47" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M47" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N47" t="inlineStr">
         <is>
@@ -3542,41 +3542,41 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>251750</v>
+        <v>251795</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>32</v>
+        <v>34.5</v>
       </c>
       <c r="D48" t="n">
-        <v>54.80281690140845</v>
+        <v>340.7090909090909</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-05-09 10:02:44</t>
+          <t>2025-05-12 07:51:55</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-05-09 10:34:44</t>
+          <t>2025-05-12 08:26:25</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-05-09 10:34:44</t>
+          <t>2025-05-12 08:26:25</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-05-09 11:29:32</t>
+          <t>2025-05-12 14:07:08</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>3891</v>
+        <v>18739</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -3585,14 +3585,14 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L48" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M48" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N48" t="inlineStr">
         <is>
@@ -3608,41 +3608,41 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>251795</v>
+        <v>251750</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D49" t="n">
-        <v>307.1967213114754</v>
+        <v>60.796875</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-05-09 10:04:18</t>
+          <t>2025-05-12 10:12:19</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-05-09 10:33:18</t>
+          <t>2025-05-12 10:48:19</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-05-09 10:33:18</t>
+          <t>2025-05-12 10:48:19</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:30</t>
+          <t>2025-05-12 11:49:07</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>18739</v>
+        <v>3891</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -3651,14 +3651,14 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L49" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M49" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N49" t="inlineStr">
         <is>
@@ -3678,33 +3678,33 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D50" t="n">
-        <v>7277.718309859155</v>
+        <v>8470.786885245901</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-05-09 11:29:32</t>
+          <t>2025-05-12 10:41:09</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-05-09 12:03:32</t>
+          <t>2025-05-12 11:27:09</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-05-09 12:03:32</t>
+          <t>2025-05-12 11:27:09</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-05-30 13:21:16</t>
+          <t>2025-06-05 08:37:57</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -3748,29 +3748,29 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D51" t="n">
         <v>1916.640625</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-05-09 14:36:36</t>
+          <t>2025-05-12 11:49:07</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-05-12 07:10:36</t>
+          <t>2025-05-12 12:21:07</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-05-12 07:10:36</t>
+          <t>2025-05-12 12:21:07</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-05-16 07:07:15</t>
+          <t>2025-05-16 12:17:45</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -3810,33 +3810,33 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D52" t="n">
-        <v>176.056338028169</v>
+        <v>204.9180327868852</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 09:27:44</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 09:52:44</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 09:52:44</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-05-09 10:38:03</t>
+          <t>2025-05-12 13:17:39</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -3876,33 +3876,33 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D53" t="n">
-        <v>106</v>
+        <v>131.9591836734694</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-05-09 10:11:23</t>
+          <t>2025-05-12 10:53:28</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-09 10:36:23</t>
+          <t>2025-05-12 11:33:28</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-09 10:36:23</t>
+          <t>2025-05-12 11:33:28</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-05-09 12:22:23</t>
+          <t>2025-05-12 13:45:25</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -3942,33 +3942,33 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D54" t="n">
-        <v>200.7746478873239</v>
+        <v>233.6885245901639</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-05-09 10:38:03</t>
+          <t>2025-05-12 13:17:39</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-09 11:23:03</t>
+          <t>2025-05-12 13:47:39</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-05-09 11:23:03</t>
+          <t>2025-05-12 13:47:39</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-05-09 14:43:49</t>
+          <t>2025-05-13 09:41:20</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4008,33 +4008,33 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>30.5</v>
+        <v>50</v>
       </c>
       <c r="D55" t="n">
-        <v>207.1272727272727</v>
+        <v>232.4897959183673</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-05-09 10:54:32</t>
+          <t>2025-05-12 13:45:25</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-09 11:25:02</t>
+          <t>2025-05-12 14:35:25</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-05-09 11:25:02</t>
+          <t>2025-05-12 14:35:25</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-05-09 14:52:09</t>
+          <t>2025-05-13 10:27:55</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4070,41 +4070,41 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>250819</v>
+        <v>245350</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D56" t="n">
-        <v>139.7868852459016</v>
+        <v>405.3623188405797</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-05-09 12:22:23</t>
+          <t>2025-05-12 13:52:53</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-05-09 12:47:23</t>
+          <t>2025-05-13 07:02:53</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-05-09 12:47:23</t>
+          <t>2025-05-13 07:02:53</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-05-12 07:07:10</t>
+          <t>2025-05-13 13:48:14</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>8527</v>
+        <v>27970</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -4113,11 +4113,11 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L56" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M56" t="n">
         <v>70</v>
@@ -4140,33 +4140,33 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>80</v>
+        <v>46.5</v>
       </c>
       <c r="D57" t="n">
-        <v>342.1690140845071</v>
+        <v>441.7090909090909</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-05-09 14:43:49</t>
+          <t>2025-05-12 14:07:08</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-12 08:03:49</t>
+          <t>2025-05-12 14:53:38</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-05-12 08:03:49</t>
+          <t>2025-05-12 14:53:38</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-05-12 13:46:00</t>
+          <t>2025-05-13 14:15:20</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4202,41 +4202,41 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>245350</v>
+        <v>243569</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>46.5</v>
+        <v>19</v>
       </c>
       <c r="D58" t="n">
-        <v>508.5454545454546</v>
+        <v>36.63380281690141</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-05-09 14:52:09</t>
+          <t>2025-05-12 14:41:22</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-05-12 07:38:39</t>
+          <t>2025-05-13 07:00:22</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-05-12 07:38:39</t>
+          <t>2025-05-13 07:00:22</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:12</t>
+          <t>2025-05-13 07:37:00</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>27970</v>
+        <v>2601</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -4245,14 +4245,14 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L58" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M58" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N58" t="inlineStr">
         <is>
@@ -4268,41 +4268,41 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>235572</v>
+        <v>250670</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D59" t="n">
-        <v>144.3188405797102</v>
+        <v>22.01408450704225</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-13 07:37:00</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:00</t>
+          <t>2025-05-13 07:54:00</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:00</t>
+          <t>2025-05-13 07:54:00</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2025-05-12 10:04:19</t>
+          <t>2025-05-13 08:16:01</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>9958</v>
+        <v>1563</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -4311,14 +4311,14 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M59" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N59" t="inlineStr">
         <is>
@@ -4334,41 +4334,41 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>251485</v>
+        <v>243335</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D60" t="n">
-        <v>78.81967213114754</v>
+        <v>464.8450704225352</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-05-12 07:07:10</t>
+          <t>2025-05-13 08:16:01</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-12 07:32:10</t>
+          <t>2025-05-13 08:46:01</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-05-12 07:32:10</t>
+          <t>2025-05-13 08:46:01</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-05-12 08:51:00</t>
+          <t>2025-05-14 08:30:52</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>4808</v>
+        <v>33004</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4377,14 +4377,14 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M60" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N60" t="inlineStr">
         <is>
@@ -4400,41 +4400,41 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>243569</v>
+        <v>250819</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D61" t="n">
-        <v>36.63380281690141</v>
+        <v>139.7868852459016</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-05-12 07:20:34</t>
+          <t>2025-05-13 09:41:20</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-12 07:39:34</t>
+          <t>2025-05-13 10:06:20</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-05-12 07:39:34</t>
+          <t>2025-05-13 10:06:20</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-05-12 08:16:12</t>
+          <t>2025-05-13 12:26:07</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>2601</v>
+        <v>8527</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -4443,14 +4443,14 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M61" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N61" t="inlineStr">
         <is>
@@ -4466,41 +4466,41 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>251346</v>
+        <v>235572</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D62" t="n">
-        <v>63.26229508196721</v>
+        <v>140.2535211267606</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:30</t>
+          <t>2025-05-13 09:47:32</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-12 08:09:30</t>
+          <t>2025-05-13 10:17:32</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-05-12 08:09:30</t>
+          <t>2025-05-13 10:17:32</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-05-12 09:12:46</t>
+          <t>2025-05-13 12:37:47</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>3859</v>
+        <v>9958</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -4509,11 +4509,11 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M62" t="n">
         <v>70</v>
@@ -4532,41 +4532,41 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>250670</v>
+        <v>251485</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="D63" t="n">
-        <v>22.01408450704225</v>
+        <v>98.12244897959184</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-05-12 08:16:12</t>
+          <t>2025-05-13 10:27:55</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-12 08:33:12</t>
+          <t>2025-05-13 11:17:55</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-05-12 08:33:12</t>
+          <t>2025-05-13 11:17:55</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-05-12 08:55:13</t>
+          <t>2025-05-13 12:56:02</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>1563</v>
+        <v>4808</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -4575,14 +4575,14 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L63" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M63" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N63" t="inlineStr">
         <is>
@@ -4598,7 +4598,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>250641</v>
+        <v>251346</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -4606,33 +4606,33 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D64" t="n">
-        <v>83.8688524590164</v>
+        <v>63.26229508196721</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-05-12 08:51:00</t>
+          <t>2025-05-13 12:26:07</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-05-12 09:16:00</t>
+          <t>2025-05-13 12:56:07</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-05-12 09:16:00</t>
+          <t>2025-05-13 12:56:07</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>2025-05-12 10:39:52</t>
+          <t>2025-05-13 13:59:23</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>5116</v>
+        <v>3859</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -4645,7 +4645,7 @@
         </is>
       </c>
       <c r="L64" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M64" t="n">
         <v>70</v>
@@ -4664,41 +4664,41 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>243335</v>
+        <v>250641</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D65" t="n">
-        <v>464.8450704225352</v>
+        <v>72.05633802816901</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-05-12 08:55:13</t>
+          <t>2025-05-13 12:37:47</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-05-12 09:25:13</t>
+          <t>2025-05-13 12:54:47</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-05-12 09:25:13</t>
+          <t>2025-05-13 12:54:47</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>2025-05-13 09:10:04</t>
+          <t>2025-05-13 14:06:50</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>33004</v>
+        <v>5116</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -4707,14 +4707,14 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L65" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M65" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N65" t="inlineStr">
         <is>
@@ -4734,33 +4734,33 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="D66" t="n">
-        <v>81.9672131147541</v>
+        <v>102.0408163265306</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-05-12 09:12:46</t>
+          <t>2025-05-13 12:56:02</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-05-12 09:39:46</t>
+          <t>2025-05-13 13:51:02</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-05-12 09:39:46</t>
+          <t>2025-05-13 13:51:02</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>2025-05-12 11:01:44</t>
+          <t>2025-05-14 07:33:04</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -4804,29 +4804,29 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D67" t="n">
         <v>192.4492753623188</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-05-12 10:04:19</t>
+          <t>2025-05-13 13:48:14</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-05-12 10:34:19</t>
+          <t>2025-05-13 14:43:14</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-05-12 10:34:19</t>
+          <t>2025-05-13 14:43:14</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>2025-05-12 13:46:46</t>
+          <t>2025-05-14 09:55:41</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -4870,29 +4870,29 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D68" t="n">
         <v>16.34426229508197</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-05-12 10:39:52</t>
+          <t>2025-05-13 13:59:23</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-05-12 10:59:52</t>
+          <t>2025-05-13 14:29:23</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-05-12 10:59:52</t>
+          <t>2025-05-13 14:29:23</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>2025-05-12 11:16:12</t>
+          <t>2025-05-13 14:45:44</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -4932,33 +4932,33 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D69" t="n">
-        <v>15.38775510204082</v>
+        <v>10.61971830985915</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-05-12 10:47:29</t>
+          <t>2025-05-13 14:06:50</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-05-12 11:29:29</t>
+          <t>2025-05-13 14:21:50</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-05-12 11:29:29</t>
+          <t>2025-05-13 14:21:50</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2025-05-12 11:44:52</t>
+          <t>2025-05-13 14:32:27</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -4998,33 +4998,33 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>31</v>
+        <v>46.5</v>
       </c>
       <c r="D70" t="n">
-        <v>12.36065573770492</v>
+        <v>13.70909090909091</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-05-12 11:01:44</t>
+          <t>2025-05-13 14:15:20</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-05-12 11:32:44</t>
+          <t>2025-05-14 07:01:50</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-05-12 11:32:44</t>
+          <t>2025-05-14 07:01:50</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-05-12 11:45:05</t>
+          <t>2025-05-14 07:15:33</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5064,33 +5064,33 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D71" t="n">
-        <v>393.3934426229508</v>
+        <v>337.9859154929578</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-05-12 11:16:12</t>
+          <t>2025-05-13 14:32:27</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-05-12 11:36:12</t>
+          <t>2025-05-13 14:47:27</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-05-12 11:36:12</t>
+          <t>2025-05-13 14:47:27</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>2025-05-13 10:09:36</t>
+          <t>2025-05-14 12:25:27</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5130,33 +5130,33 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D72" t="n">
-        <v>549.6734693877551</v>
+        <v>441.5409836065574</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-05-12 11:44:52</t>
+          <t>2025-05-13 14:45:44</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-05-12 12:19:52</t>
+          <t>2025-05-14 07:05:44</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-05-12 12:19:52</t>
+          <t>2025-05-14 07:05:44</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>2025-05-13 13:29:33</t>
+          <t>2025-05-14 14:27:16</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5196,33 +5196,33 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>25</v>
+        <v>30.5</v>
       </c>
       <c r="D73" t="n">
-        <v>196.7540983606557</v>
+        <v>218.2181818181818</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-05-12 11:45:05</t>
+          <t>2025-05-14 07:15:33</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-05-12 12:10:05</t>
+          <t>2025-05-14 07:46:03</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-05-12 12:10:05</t>
+          <t>2025-05-14 07:46:03</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>2025-05-13 07:26:51</t>
+          <t>2025-05-14 11:24:16</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5258,41 +5258,41 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>251109</v>
+        <v>251466</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D74" t="n">
-        <v>266.5915492957747</v>
+        <v>113.6122448979592</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-05-12 13:46:00</t>
+          <t>2025-05-14 07:33:04</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-05-12 14:31:00</t>
+          <t>2025-05-14 08:38:04</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-05-12 14:31:00</t>
+          <t>2025-05-14 08:38:04</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-05-13 10:57:35</t>
+          <t>2025-05-14 10:31:41</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>18928</v>
+        <v>5567</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -5301,11 +5301,11 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="M74" t="n">
         <v>70</v>
@@ -5324,41 +5324,41 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>251466</v>
+        <v>251987</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D75" t="n">
-        <v>80.68115942028986</v>
+        <v>2965.154929577465</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-05-12 13:46:46</t>
+          <t>2025-05-14 08:30:52</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-05-12 14:16:46</t>
+          <t>2025-05-14 09:04:52</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-05-12 14:16:46</t>
+          <t>2025-05-14 09:04:52</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-05-13 07:37:26</t>
+          <t>2025-05-22 10:30:01</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>5567</v>
+        <v>210526</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -5367,14 +5367,14 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L75" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M75" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N75" t="inlineStr">
         <is>
@@ -5394,33 +5394,33 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D76" t="n">
-        <v>114.2131147540984</v>
+        <v>100.9710144927536</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2025-05-13 07:26:51</t>
+          <t>2025-05-14 09:55:41</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-05-13 07:55:51</t>
+          <t>2025-05-14 10:20:41</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2025-05-13 07:55:51</t>
+          <t>2025-05-14 10:20:41</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>2025-05-13 09:50:03</t>
+          <t>2025-05-14 12:01:40</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -5460,33 +5460,33 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D77" t="n">
-        <v>103.6666666666667</v>
+        <v>145.9795918367347</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2025-05-13 07:37:26</t>
+          <t>2025-05-14 10:31:41</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:26</t>
+          <t>2025-05-14 11:11:41</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:26</t>
+          <t>2025-05-14 11:11:41</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>2025-05-13 09:51:06</t>
+          <t>2025-05-14 13:37:40</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -5530,29 +5530,29 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>46.5</v>
+        <v>38.5</v>
       </c>
       <c r="D78" t="n">
         <v>113.2</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:12</t>
+          <t>2025-05-14 11:24:16</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-05-13 08:53:42</t>
+          <t>2025-05-14 12:02:46</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>2025-05-13 08:53:42</t>
+          <t>2025-05-14 12:02:46</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>2025-05-13 10:46:54</t>
+          <t>2025-05-14 13:55:58</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -5588,41 +5588,41 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>251987</v>
+        <v>251462</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D79" t="n">
-        <v>2965.154929577465</v>
+        <v>90.23188405797102</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2025-05-13 09:10:04</t>
+          <t>2025-05-14 12:01:40</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-05-13 09:44:04</t>
+          <t>2025-05-14 12:36:40</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>2025-05-13 09:44:04</t>
+          <t>2025-05-14 12:36:40</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>2025-05-21 11:09:13</t>
+          <t>2025-05-14 14:06:53</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>210526</v>
+        <v>6226</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -5631,14 +5631,14 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L79" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M79" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N79" t="inlineStr">
         <is>
@@ -5654,37 +5654,37 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>251462</v>
+        <v>251467</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D80" t="n">
-        <v>102.0655737704918</v>
+        <v>87.69014084507042</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2025-05-13 09:50:03</t>
+          <t>2025-05-14 12:25:27</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-05-13 10:19:03</t>
+          <t>2025-05-14 12:48:27</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>2025-05-13 10:19:03</t>
+          <t>2025-05-14 12:48:27</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>2025-05-13 12:01:07</t>
+          <t>2025-05-14 14:16:08</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -5720,41 +5720,41 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>251467</v>
+        <v>251374</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D81" t="n">
-        <v>90.23188405797102</v>
+        <v>558.0204081632653</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2025-05-13 09:51:06</t>
+          <t>2025-05-14 13:37:40</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-05-13 10:26:06</t>
+          <t>2025-05-14 14:27:40</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2025-05-13 10:26:06</t>
+          <t>2025-05-14 14:27:40</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>2025-05-13 11:56:20</t>
+          <t>2025-05-16 07:45:41</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>6226</v>
+        <v>27343</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -5763,11 +5763,11 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M81" t="n">
         <v>70</v>
@@ -5786,41 +5786,41 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>251374</v>
+        <v>251520</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>25</v>
+        <v>40.5</v>
       </c>
       <c r="D82" t="n">
-        <v>448.2459016393443</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025-05-13 10:09:36</t>
+          <t>2025-05-14 13:55:58</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-05-13 10:34:36</t>
+          <t>2025-05-14 14:36:28</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>2025-05-13 10:34:36</t>
+          <t>2025-05-14 14:36:28</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>2025-05-14 10:02:51</t>
+          <t>2025-05-15 11:33:33</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>27343</v>
+        <v>16340</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L82" t="n">
@@ -5852,41 +5852,41 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>251520</v>
+        <v>251580</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>40.5</v>
+        <v>35</v>
       </c>
       <c r="D83" t="n">
-        <v>297.0909090909091</v>
+        <v>103.6666666666667</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-05-13 10:46:54</t>
+          <t>2025-05-14 14:06:53</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:24</t>
+          <t>2025-05-14 14:41:53</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:24</t>
+          <t>2025-05-14 14:41:53</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>2025-05-14 08:24:30</t>
+          <t>2025-05-15 08:25:33</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>16340</v>
+        <v>7153</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -5895,11 +5895,11 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M83" t="n">
         <v>70</v>
@@ -5918,41 +5918,41 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>251580</v>
+        <v>251557</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="D84" t="n">
-        <v>100.7464788732394</v>
+        <v>94.43661971830986</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-05-13 10:57:35</t>
+          <t>2025-05-14 14:16:08</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-05-13 12:32:35</t>
+          <t>2025-05-14 14:31:08</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2025-05-13 12:32:35</t>
+          <t>2025-05-14 14:31:08</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>2025-05-13 14:13:20</t>
+          <t>2025-05-15 08:05:34</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>7153</v>
+        <v>6705</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -5965,7 +5965,7 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M84" t="n">
         <v>70</v>
@@ -5984,41 +5984,41 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>251557</v>
+        <v>251562</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D85" t="n">
-        <v>97.17391304347827</v>
+        <v>133.4754098360656</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-05-13 11:56:20</t>
+          <t>2025-05-14 14:27:16</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-05-13 12:21:20</t>
+          <t>2025-05-15 07:07:16</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2025-05-13 12:21:20</t>
+          <t>2025-05-15 07:07:16</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>2025-05-13 13:58:31</t>
+          <t>2025-05-15 09:20:45</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>6705</v>
+        <v>8142</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -6050,41 +6050,41 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>251562</v>
+        <v>251062</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D86" t="n">
-        <v>133.4754098360656</v>
+        <v>318.6478873239437</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-05-13 12:01:07</t>
+          <t>2025-05-15 08:05:34</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-05-13 12:26:07</t>
+          <t>2025-05-15 08:28:34</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>2025-05-13 12:26:07</t>
+          <t>2025-05-15 08:28:34</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>2025-05-13 14:39:36</t>
+          <t>2025-05-15 13:47:13</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>8142</v>
+        <v>22624</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -6093,11 +6093,11 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L86" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M86" t="n">
         <v>70</v>
@@ -6116,41 +6116,41 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>251062</v>
+        <v>251252</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C87" t="n">
         <v>35</v>
       </c>
       <c r="D87" t="n">
-        <v>461.7142857142857</v>
+        <v>218.5942028985507</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2025-05-13 13:29:33</t>
+          <t>2025-05-15 08:25:33</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-05-13 14:04:33</t>
+          <t>2025-05-15 09:00:33</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>2025-05-13 14:04:33</t>
+          <t>2025-05-15 09:00:33</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>2025-05-14 13:46:15</t>
+          <t>2025-05-15 12:39:09</t>
         </is>
       </c>
       <c r="I87" t="n">
-        <v>22624</v>
+        <v>15083</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -6182,41 +6182,41 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>251252</v>
+        <v>251251</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D88" t="n">
-        <v>218.5942028985507</v>
+        <v>260</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2025-05-13 13:58:31</t>
+          <t>2025-05-15 09:20:45</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-05-13 14:43:31</t>
+          <t>2025-05-15 10:00:45</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>2025-05-13 14:43:31</t>
+          <t>2025-05-15 10:00:45</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>2025-05-14 10:22:06</t>
+          <t>2025-05-15 14:20:45</t>
         </is>
       </c>
       <c r="I88" t="n">
-        <v>15083</v>
+        <v>15860</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -6248,41 +6248,41 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>251251</v>
+        <v>251249</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>33</v>
+        <v>32.5</v>
       </c>
       <c r="D89" t="n">
-        <v>260</v>
+        <v>86.50909090909092</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2025-05-13 14:39:36</t>
+          <t>2025-05-15 11:33:33</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2025-05-14 07:12:36</t>
+          <t>2025-05-15 12:06:03</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>2025-05-14 07:12:36</t>
+          <t>2025-05-15 12:06:03</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>2025-05-14 11:32:36</t>
+          <t>2025-05-15 13:32:34</t>
         </is>
       </c>
       <c r="I89" t="n">
-        <v>15860</v>
+        <v>4758</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -6309,72 +6309,6 @@
         <v>0</v>
       </c>
       <c r="P89" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>251249</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>CASON</t>
-        </is>
-      </c>
-      <c r="C90" t="n">
-        <v>32.5</v>
-      </c>
-      <c r="D90" t="n">
-        <v>86.50909090909092</v>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>2025-05-14 08:24:30</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>2025-05-14 08:57:00</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>2025-05-14 08:57:00</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>2025-05-14 10:23:30</t>
-        </is>
-      </c>
-      <c r="I90" t="n">
-        <v>4758</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
-        </is>
-      </c>
-      <c r="L90" t="n">
-        <v>6</v>
-      </c>
-      <c r="M90" t="n">
-        <v>70</v>
-      </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P90" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Da risolvere LS2, LS3 e capire gli esclusi da LS1
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2228,41 +2228,41 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251561</v>
+        <v>251340</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D28" t="n">
-        <v>84.921875</v>
+        <v>461.9718309859155</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-07 07:21:00</t>
+          <t>2025-05-08 12:15:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-07 07:21:00</t>
+          <t>2025-05-08 12:15:00</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-07 08:45:55</t>
+          <t>2025-05-09 11:56:58</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>5435</v>
+        <v>32800</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2271,14 +2271,14 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M28" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N28" t="inlineStr">
         <is>
@@ -2294,41 +2294,41 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251564</v>
+        <v>251561</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29" t="n">
-        <v>42.453125</v>
+        <v>76.54929577464789</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-07 08:45:55</t>
+          <t>2025-05-09 07:27:22</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-07 09:04:55</t>
+          <t>2025-05-09 07:44:22</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-07 09:04:55</t>
+          <t>2025-05-09 07:44:22</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-07 09:47:22</t>
+          <t>2025-05-09 09:00:55</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>2717</v>
+        <v>5435</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2341,7 +2341,7 @@
         </is>
       </c>
       <c r="L29" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M29" t="n">
         <v>70</v>
@@ -2360,41 +2360,41 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251566</v>
+        <v>251564</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D30" t="n">
-        <v>107.640625</v>
+        <v>38.26760563380282</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-07 09:47:22</t>
+          <t>2025-05-09 09:00:55</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-07 10:04:22</t>
+          <t>2025-05-09 09:19:55</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-07 10:04:22</t>
+          <t>2025-05-09 09:19:55</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-07 11:52:00</t>
+          <t>2025-05-09 09:58:11</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>6889</v>
+        <v>2717</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="L30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M30" t="n">
         <v>70</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>251519</v>
+        <v>251566</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2434,33 +2434,33 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D31" t="n">
-        <v>205.859375</v>
+        <v>107.640625</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-05-07 11:52:00</t>
+          <t>2025-05-09 09:06:46</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-05-07 12:11:00</t>
+          <t>2025-05-09 09:23:46</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-05-07 12:11:00</t>
+          <t>2025-05-09 09:23:46</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-05-08 07:36:52</t>
+          <t>2025-05-09 11:11:25</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>13175</v>
+        <v>6889</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M31" t="n">
         <v>70</v>
@@ -2492,41 +2492,41 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>251340</v>
+        <v>251519</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="D32" t="n">
-        <v>461.9718309859155</v>
+        <v>268.8775510204082</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 09:14:40</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-05-08 07:15:00</t>
+          <t>2025-05-09 09:59:40</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-05-08 07:15:00</t>
+          <t>2025-05-09 09:59:40</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-05-08 14:56:58</t>
+          <t>2025-05-09 14:28:33</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>32800</v>
+        <v>13175</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2535,14 +2535,14 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L32" t="n">
         <v>2</v>
       </c>
       <c r="M32" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N32" t="inlineStr">
         <is>
@@ -2562,33 +2562,33 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D33" t="n">
-        <v>280.2295081967213</v>
+        <v>240.7605633802817</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 09:58:11</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-09 10:17:11</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-09 10:17:11</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-08 12:15:13</t>
+          <t>2025-05-09 14:17:57</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2628,33 +2628,33 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D34" t="n">
-        <v>197.1836734693877</v>
+        <v>158.3934426229508</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 10:06:22</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-05-08 07:45:00</t>
+          <t>2025-05-09 10:36:22</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-05-08 07:45:00</t>
+          <t>2025-05-09 10:36:22</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:11</t>
+          <t>2025-05-09 13:14:46</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2705,22 +2705,22 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-05-08 07:36:52</t>
+          <t>2025-05-09 11:11:25</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-08 07:53:52</t>
+          <t>2025-05-09 11:28:25</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-05-08 07:53:52</t>
+          <t>2025-05-09 11:28:25</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-05-08 09:18:47</t>
+          <t>2025-05-09 12:53:20</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -2756,41 +2756,41 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>251475</v>
+        <v>250894</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D36" t="n">
-        <v>135.640625</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-05-08 09:18:47</t>
+          <t>2025-05-09 11:56:58</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-08 09:35:47</t>
+          <t>2025-05-09 12:17:58</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-05-08 09:35:47</t>
+          <t>2025-05-09 12:17:58</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-08 11:51:26</t>
+          <t>2025-05-12 14:41:22</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>8681</v>
+        <v>44262</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -2799,19 +2799,17 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M36" t="n">
-        <v>70</v>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N36" t="n">
+        <v>39755</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
@@ -2822,41 +2820,41 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>250894</v>
+        <v>251475</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>42</v>
+        <v>36.5</v>
       </c>
       <c r="D37" t="n">
-        <v>903.3061224489796</v>
+        <v>157.8363636363636</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:11</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-08 11:44:11</t>
+          <t>2025-05-09 13:14:05</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-05-08 11:44:11</t>
+          <t>2025-05-09 13:14:05</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-05-12 10:47:29</t>
+          <t>2025-05-12 07:51:55</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>44262</v>
+        <v>8681</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -2865,17 +2863,19 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M37" t="n">
-        <v>76</v>
-      </c>
-      <c r="N37" t="n">
-        <v>39755</v>
+        <v>70</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
       <c r="O37" t="n">
         <v>0</v>
@@ -2890,33 +2890,33 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D38" t="n">
-        <v>101.03125</v>
+        <v>106</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-05-08 11:51:26</t>
+          <t>2025-05-09 12:53:11</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-05-08 12:06:26</t>
+          <t>2025-05-09 13:22:11</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-05-08 12:06:26</t>
+          <t>2025-05-09 13:22:11</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-05-08 13:47:28</t>
+          <t>2025-05-12 07:08:11</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -2952,41 +2952,41 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>251651</v>
+        <v>244354</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D39" t="n">
-        <v>659.5774647887324</v>
+        <v>67.34375</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-09 12:53:20</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:00</t>
+          <t>2025-05-09 13:10:20</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:00</t>
+          <t>2025-05-09 13:10:20</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-05-12 07:20:34</t>
+          <t>2025-05-09 14:17:41</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>46830</v>
+        <v>4310</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -2995,17 +2995,19 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M39" t="n">
-        <v>76</v>
-      </c>
-      <c r="N39" t="n">
-        <v>39755</v>
+        <v>70</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
       <c r="O39" t="n">
         <v>0</v>
@@ -3016,7 +3018,7 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>244354</v>
+        <v>244355</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -3024,29 +3026,29 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D40" t="n">
         <v>70.65573770491804</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-05-08 12:15:13</t>
+          <t>2025-05-09 13:14:46</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-05-08 12:40:13</t>
+          <t>2025-05-09 13:34:46</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-05-08 12:40:13</t>
+          <t>2025-05-09 13:34:46</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-05-08 13:50:53</t>
+          <t>2025-05-09 14:45:25</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3082,7 +3084,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>244355</v>
+        <v>244204</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -3093,30 +3095,30 @@
         <v>15</v>
       </c>
       <c r="D41" t="n">
-        <v>67.34375</v>
+        <v>54.25</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-05-08 13:47:28</t>
+          <t>2025-05-09 14:17:41</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-05-08 14:02:28</t>
+          <t>2025-05-09 14:32:41</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-05-08 14:02:28</t>
+          <t>2025-05-09 14:32:41</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-05-09 07:09:48</t>
+          <t>2025-05-12 07:26:56</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>4310</v>
+        <v>3472</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3148,41 +3150,41 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>244204</v>
+        <v>251651</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D42" t="n">
-        <v>56.91803278688525</v>
+        <v>659.5774647887324</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-05-08 13:50:53</t>
+          <t>2025-05-09 14:17:57</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-05-08 14:10:53</t>
+          <t>2025-05-09 14:47:57</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-05-08 14:10:53</t>
+          <t>2025-05-09 14:47:57</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-05-09 07:07:48</t>
+          <t>2025-05-13 09:47:32</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>3472</v>
+        <v>46830</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3191,19 +3193,17 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M42" t="n">
-        <v>70</v>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N42" t="n">
+        <v>39755</v>
       </c>
       <c r="O42" t="n">
         <v>0</v>
@@ -3218,33 +3218,33 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D43" t="n">
-        <v>151.7746478873239</v>
+        <v>219.9183673469388</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-05-08 14:56:58</t>
+          <t>2025-05-09 14:28:33</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:58</t>
+          <t>2025-05-12 07:13:33</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:58</t>
+          <t>2025-05-12 07:13:33</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-05-09 10:02:44</t>
+          <t>2025-05-12 10:53:28</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3284,33 +3284,33 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D44" t="n">
         <v>142.3114754098361</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 14:45:25</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 07:05:25</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 07:05:25</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-05-09 10:04:18</t>
+          <t>2025-05-12 09:27:44</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3346,41 +3346,41 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>251416</v>
+        <v>245623</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>30.5</v>
+        <v>30</v>
       </c>
       <c r="D45" t="n">
-        <v>204.0363636363636</v>
+        <v>382.8840579710145</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:30</t>
+          <t>2025-05-12 07:30:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-05-09 07:30:30</t>
+          <t>2025-05-12 07:30:00</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-05-09 10:54:32</t>
+          <t>2025-05-12 13:52:53</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>11222</v>
+        <v>26419</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3389,17 +3389,19 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L45" t="n">
         <v>2</v>
       </c>
       <c r="M45" t="n">
-        <v>70</v>
-      </c>
-      <c r="N45" t="n">
-        <v>39755</v>
+        <v>152</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
       <c r="O45" t="n">
         <v>0</v>
@@ -3410,41 +3412,41 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>251260</v>
+        <v>251416</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D46" t="n">
-        <v>153.5901639344262</v>
+        <v>183.9672131147541</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-05-09 07:07:48</t>
+          <t>2025-05-12 07:08:11</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-05-09 07:37:48</t>
+          <t>2025-05-12 07:37:11</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-05-09 07:37:48</t>
+          <t>2025-05-12 07:37:11</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-05-09 10:11:23</t>
+          <t>2025-05-12 10:41:09</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>9369</v>
+        <v>11222</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3453,19 +3455,17 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L46" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M46" t="n">
         <v>70</v>
       </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+      <c r="N46" t="n">
+        <v>39755</v>
       </c>
       <c r="O46" t="n">
         <v>0</v>
@@ -3476,7 +3476,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>245623</v>
+        <v>251260</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -3484,33 +3484,33 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D47" t="n">
-        <v>412.796875</v>
+        <v>146.390625</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-05-09 07:09:48</t>
+          <t>2025-05-12 07:26:56</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-05-09 07:43:48</t>
+          <t>2025-05-12 07:45:56</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-05-09 07:43:48</t>
+          <t>2025-05-12 07:45:56</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-05-09 14:36:36</t>
+          <t>2025-05-12 10:12:19</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>26419</v>
+        <v>9369</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3519,14 +3519,14 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L47" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M47" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N47" t="inlineStr">
         <is>
@@ -3542,41 +3542,41 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>251750</v>
+        <v>251795</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>32</v>
+        <v>34.5</v>
       </c>
       <c r="D48" t="n">
-        <v>54.80281690140845</v>
+        <v>340.7090909090909</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-05-09 10:02:44</t>
+          <t>2025-05-12 07:51:55</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-05-09 10:34:44</t>
+          <t>2025-05-12 08:26:25</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-05-09 10:34:44</t>
+          <t>2025-05-12 08:26:25</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-05-09 11:29:32</t>
+          <t>2025-05-12 14:07:08</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>3891</v>
+        <v>18739</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -3585,14 +3585,14 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L48" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M48" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N48" t="inlineStr">
         <is>
@@ -3608,41 +3608,41 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>251795</v>
+        <v>251750</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D49" t="n">
-        <v>307.1967213114754</v>
+        <v>60.796875</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-05-09 10:04:18</t>
+          <t>2025-05-12 10:12:19</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-05-09 10:33:18</t>
+          <t>2025-05-12 10:48:19</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-05-09 10:33:18</t>
+          <t>2025-05-12 10:48:19</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:30</t>
+          <t>2025-05-12 11:49:07</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>18739</v>
+        <v>3891</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -3651,14 +3651,14 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L49" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M49" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N49" t="inlineStr">
         <is>
@@ -3678,33 +3678,33 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D50" t="n">
-        <v>7277.718309859155</v>
+        <v>8470.786885245901</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-05-09 11:29:32</t>
+          <t>2025-05-12 10:41:09</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-05-09 12:03:32</t>
+          <t>2025-05-12 11:27:09</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-05-09 12:03:32</t>
+          <t>2025-05-12 11:27:09</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-05-30 13:21:16</t>
+          <t>2025-06-05 08:37:57</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -3748,29 +3748,29 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D51" t="n">
         <v>1916.640625</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-05-09 14:36:36</t>
+          <t>2025-05-12 11:49:07</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-05-12 07:10:36</t>
+          <t>2025-05-12 12:21:07</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-05-12 07:10:36</t>
+          <t>2025-05-12 12:21:07</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-05-16 07:07:15</t>
+          <t>2025-05-16 12:17:45</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -3810,33 +3810,33 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D52" t="n">
-        <v>176.056338028169</v>
+        <v>204.9180327868852</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 09:27:44</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 09:52:44</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-12 09:52:44</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-05-09 10:38:03</t>
+          <t>2025-05-12 13:17:39</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -3876,33 +3876,33 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D53" t="n">
-        <v>106</v>
+        <v>131.9591836734694</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-05-09 10:11:23</t>
+          <t>2025-05-12 10:53:28</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-09 10:36:23</t>
+          <t>2025-05-12 11:33:28</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-09 10:36:23</t>
+          <t>2025-05-12 11:33:28</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-05-09 12:22:23</t>
+          <t>2025-05-12 13:45:25</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -3942,33 +3942,33 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D54" t="n">
-        <v>200.7746478873239</v>
+        <v>233.6885245901639</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-05-09 10:38:03</t>
+          <t>2025-05-12 13:17:39</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-09 11:23:03</t>
+          <t>2025-05-12 13:47:39</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-05-09 11:23:03</t>
+          <t>2025-05-12 13:47:39</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-05-09 14:43:49</t>
+          <t>2025-05-13 09:41:20</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4008,33 +4008,33 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>30.5</v>
+        <v>50</v>
       </c>
       <c r="D55" t="n">
-        <v>207.1272727272727</v>
+        <v>232.4897959183673</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-05-09 10:54:32</t>
+          <t>2025-05-12 13:45:25</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-09 11:25:02</t>
+          <t>2025-05-12 14:35:25</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-05-09 11:25:02</t>
+          <t>2025-05-12 14:35:25</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-05-09 14:52:09</t>
+          <t>2025-05-13 10:27:55</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4070,41 +4070,41 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>250819</v>
+        <v>245350</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D56" t="n">
-        <v>139.7868852459016</v>
+        <v>405.3623188405797</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-05-09 12:22:23</t>
+          <t>2025-05-12 13:52:53</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-05-09 12:47:23</t>
+          <t>2025-05-13 07:02:53</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-05-09 12:47:23</t>
+          <t>2025-05-13 07:02:53</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-05-12 07:07:10</t>
+          <t>2025-05-13 13:48:14</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>8527</v>
+        <v>27970</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -4113,11 +4113,11 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L56" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M56" t="n">
         <v>70</v>
@@ -4140,33 +4140,33 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>80</v>
+        <v>46.5</v>
       </c>
       <c r="D57" t="n">
-        <v>342.1690140845071</v>
+        <v>441.7090909090909</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-05-09 14:43:49</t>
+          <t>2025-05-12 14:07:08</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-12 08:03:49</t>
+          <t>2025-05-12 14:53:38</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-05-12 08:03:49</t>
+          <t>2025-05-12 14:53:38</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-05-12 13:46:00</t>
+          <t>2025-05-13 14:15:20</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4202,41 +4202,41 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>245350</v>
+        <v>243569</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>46.5</v>
+        <v>19</v>
       </c>
       <c r="D58" t="n">
-        <v>508.5454545454546</v>
+        <v>36.63380281690141</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-05-09 14:52:09</t>
+          <t>2025-05-12 14:41:22</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-05-12 07:38:39</t>
+          <t>2025-05-13 07:00:22</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-05-12 07:38:39</t>
+          <t>2025-05-13 07:00:22</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:12</t>
+          <t>2025-05-13 07:37:00</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>27970</v>
+        <v>2601</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -4245,14 +4245,14 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L58" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M58" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N58" t="inlineStr">
         <is>
@@ -4268,41 +4268,41 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>235572</v>
+        <v>250670</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D59" t="n">
-        <v>144.3188405797102</v>
+        <v>22.01408450704225</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-13 07:37:00</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:00</t>
+          <t>2025-05-13 07:54:00</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:00</t>
+          <t>2025-05-13 07:54:00</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2025-05-12 10:04:19</t>
+          <t>2025-05-13 08:16:01</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>9958</v>
+        <v>1563</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -4311,14 +4311,14 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M59" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N59" t="inlineStr">
         <is>
@@ -4334,41 +4334,41 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>251485</v>
+        <v>243335</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D60" t="n">
-        <v>78.81967213114754</v>
+        <v>464.8450704225352</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-05-12 07:07:10</t>
+          <t>2025-05-13 08:16:01</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-12 07:32:10</t>
+          <t>2025-05-13 08:46:01</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-05-12 07:32:10</t>
+          <t>2025-05-13 08:46:01</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-05-12 08:51:00</t>
+          <t>2025-05-14 08:30:52</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>4808</v>
+        <v>33004</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4377,14 +4377,14 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M60" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N60" t="inlineStr">
         <is>
@@ -4400,41 +4400,41 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>243569</v>
+        <v>250819</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D61" t="n">
-        <v>36.63380281690141</v>
+        <v>139.7868852459016</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-05-12 07:20:34</t>
+          <t>2025-05-13 09:41:20</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-12 07:39:34</t>
+          <t>2025-05-13 10:06:20</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-05-12 07:39:34</t>
+          <t>2025-05-13 10:06:20</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-05-12 08:16:12</t>
+          <t>2025-05-13 12:26:07</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>2601</v>
+        <v>8527</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -4443,14 +4443,14 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M61" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N61" t="inlineStr">
         <is>
@@ -4466,41 +4466,41 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>251346</v>
+        <v>235572</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D62" t="n">
-        <v>63.26229508196721</v>
+        <v>140.2535211267606</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-05-12 07:40:30</t>
+          <t>2025-05-13 09:47:32</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-12 08:09:30</t>
+          <t>2025-05-13 10:17:32</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-05-12 08:09:30</t>
+          <t>2025-05-13 10:17:32</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-05-12 09:12:46</t>
+          <t>2025-05-13 12:37:47</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>3859</v>
+        <v>9958</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -4509,11 +4509,11 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M62" t="n">
         <v>70</v>
@@ -4532,41 +4532,41 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>250670</v>
+        <v>251485</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="D63" t="n">
-        <v>22.01408450704225</v>
+        <v>98.12244897959184</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-05-12 08:16:12</t>
+          <t>2025-05-13 10:27:55</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-12 08:33:12</t>
+          <t>2025-05-13 11:17:55</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-05-12 08:33:12</t>
+          <t>2025-05-13 11:17:55</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-05-12 08:55:13</t>
+          <t>2025-05-13 12:56:02</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>1563</v>
+        <v>4808</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -4575,14 +4575,14 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L63" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M63" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N63" t="inlineStr">
         <is>
@@ -4598,7 +4598,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>250641</v>
+        <v>251346</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -4606,33 +4606,33 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D64" t="n">
-        <v>83.8688524590164</v>
+        <v>63.26229508196721</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-05-12 08:51:00</t>
+          <t>2025-05-13 12:26:07</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-05-12 09:16:00</t>
+          <t>2025-05-13 12:56:07</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-05-12 09:16:00</t>
+          <t>2025-05-13 12:56:07</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>2025-05-12 10:39:52</t>
+          <t>2025-05-13 13:59:23</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>5116</v>
+        <v>3859</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -4645,7 +4645,7 @@
         </is>
       </c>
       <c r="L64" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M64" t="n">
         <v>70</v>
@@ -4664,41 +4664,41 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>243335</v>
+        <v>250641</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D65" t="n">
-        <v>464.8450704225352</v>
+        <v>72.05633802816901</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-05-12 08:55:13</t>
+          <t>2025-05-13 12:37:47</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-05-12 09:25:13</t>
+          <t>2025-05-13 12:54:47</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-05-12 09:25:13</t>
+          <t>2025-05-13 12:54:47</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>2025-05-13 09:10:04</t>
+          <t>2025-05-13 14:06:50</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>33004</v>
+        <v>5116</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -4707,14 +4707,14 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L65" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M65" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N65" t="inlineStr">
         <is>
@@ -4734,33 +4734,33 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="D66" t="n">
-        <v>81.9672131147541</v>
+        <v>102.0408163265306</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-05-12 09:12:46</t>
+          <t>2025-05-13 12:56:02</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-05-12 09:39:46</t>
+          <t>2025-05-13 13:51:02</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-05-12 09:39:46</t>
+          <t>2025-05-13 13:51:02</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>2025-05-12 11:01:44</t>
+          <t>2025-05-14 07:33:04</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -4804,29 +4804,29 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D67" t="n">
         <v>192.4492753623188</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-05-12 10:04:19</t>
+          <t>2025-05-13 13:48:14</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-05-12 10:34:19</t>
+          <t>2025-05-13 14:43:14</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-05-12 10:34:19</t>
+          <t>2025-05-13 14:43:14</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>2025-05-12 13:46:46</t>
+          <t>2025-05-14 09:55:41</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -4870,29 +4870,29 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D68" t="n">
         <v>16.34426229508197</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-05-12 10:39:52</t>
+          <t>2025-05-13 13:59:23</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-05-12 10:59:52</t>
+          <t>2025-05-13 14:29:23</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-05-12 10:59:52</t>
+          <t>2025-05-13 14:29:23</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>2025-05-12 11:16:12</t>
+          <t>2025-05-13 14:45:44</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -4932,33 +4932,33 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D69" t="n">
-        <v>15.38775510204082</v>
+        <v>10.61971830985915</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-05-12 10:47:29</t>
+          <t>2025-05-13 14:06:50</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-05-12 11:29:29</t>
+          <t>2025-05-13 14:21:50</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-05-12 11:29:29</t>
+          <t>2025-05-13 14:21:50</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2025-05-12 11:44:52</t>
+          <t>2025-05-13 14:32:27</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -4998,33 +4998,33 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>31</v>
+        <v>46.5</v>
       </c>
       <c r="D70" t="n">
-        <v>12.36065573770492</v>
+        <v>13.70909090909091</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-05-12 11:01:44</t>
+          <t>2025-05-13 14:15:20</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-05-12 11:32:44</t>
+          <t>2025-05-14 07:01:50</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-05-12 11:32:44</t>
+          <t>2025-05-14 07:01:50</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-05-12 11:45:05</t>
+          <t>2025-05-14 07:15:33</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5064,33 +5064,33 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D71" t="n">
-        <v>393.3934426229508</v>
+        <v>337.9859154929578</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-05-12 11:16:12</t>
+          <t>2025-05-13 14:32:27</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-05-12 11:36:12</t>
+          <t>2025-05-13 14:47:27</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-05-12 11:36:12</t>
+          <t>2025-05-13 14:47:27</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>2025-05-13 10:09:36</t>
+          <t>2025-05-14 12:25:27</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5130,33 +5130,33 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D72" t="n">
-        <v>549.6734693877551</v>
+        <v>441.5409836065574</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-05-12 11:44:52</t>
+          <t>2025-05-13 14:45:44</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-05-12 12:19:52</t>
+          <t>2025-05-14 07:05:44</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-05-12 12:19:52</t>
+          <t>2025-05-14 07:05:44</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>2025-05-13 13:29:33</t>
+          <t>2025-05-14 14:27:16</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5196,33 +5196,33 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>25</v>
+        <v>30.5</v>
       </c>
       <c r="D73" t="n">
-        <v>196.7540983606557</v>
+        <v>218.2181818181818</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-05-12 11:45:05</t>
+          <t>2025-05-14 07:15:33</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-05-12 12:10:05</t>
+          <t>2025-05-14 07:46:03</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-05-12 12:10:05</t>
+          <t>2025-05-14 07:46:03</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>2025-05-13 07:26:51</t>
+          <t>2025-05-14 11:24:16</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5258,41 +5258,41 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>251109</v>
+        <v>251466</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D74" t="n">
-        <v>266.5915492957747</v>
+        <v>113.6122448979592</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-05-12 13:46:00</t>
+          <t>2025-05-14 07:33:04</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-05-12 14:31:00</t>
+          <t>2025-05-14 08:38:04</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-05-12 14:31:00</t>
+          <t>2025-05-14 08:38:04</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-05-13 10:57:35</t>
+          <t>2025-05-14 10:31:41</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>18928</v>
+        <v>5567</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -5301,11 +5301,11 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="M74" t="n">
         <v>70</v>
@@ -5324,41 +5324,41 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>251466</v>
+        <v>251987</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D75" t="n">
-        <v>80.68115942028986</v>
+        <v>2965.154929577465</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-05-12 13:46:46</t>
+          <t>2025-05-14 08:30:52</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-05-12 14:16:46</t>
+          <t>2025-05-14 09:04:52</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-05-12 14:16:46</t>
+          <t>2025-05-14 09:04:52</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-05-13 07:37:26</t>
+          <t>2025-05-22 10:30:01</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>5567</v>
+        <v>210526</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -5367,14 +5367,14 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L75" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M75" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N75" t="inlineStr">
         <is>
@@ -5394,33 +5394,33 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D76" t="n">
-        <v>114.2131147540984</v>
+        <v>100.9710144927536</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2025-05-13 07:26:51</t>
+          <t>2025-05-14 09:55:41</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-05-13 07:55:51</t>
+          <t>2025-05-14 10:20:41</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2025-05-13 07:55:51</t>
+          <t>2025-05-14 10:20:41</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>2025-05-13 09:50:03</t>
+          <t>2025-05-14 12:01:40</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -5460,33 +5460,33 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D77" t="n">
-        <v>103.6666666666667</v>
+        <v>145.9795918367347</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2025-05-13 07:37:26</t>
+          <t>2025-05-14 10:31:41</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:26</t>
+          <t>2025-05-14 11:11:41</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:26</t>
+          <t>2025-05-14 11:11:41</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>2025-05-13 09:51:06</t>
+          <t>2025-05-14 13:37:40</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -5530,29 +5530,29 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>46.5</v>
+        <v>38.5</v>
       </c>
       <c r="D78" t="n">
         <v>113.2</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:12</t>
+          <t>2025-05-14 11:24:16</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-05-13 08:53:42</t>
+          <t>2025-05-14 12:02:46</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>2025-05-13 08:53:42</t>
+          <t>2025-05-14 12:02:46</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>2025-05-13 10:46:54</t>
+          <t>2025-05-14 13:55:58</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -5588,41 +5588,41 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>251987</v>
+        <v>251462</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D79" t="n">
-        <v>2965.154929577465</v>
+        <v>90.23188405797102</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2025-05-13 09:10:04</t>
+          <t>2025-05-14 12:01:40</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-05-13 09:44:04</t>
+          <t>2025-05-14 12:36:40</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>2025-05-13 09:44:04</t>
+          <t>2025-05-14 12:36:40</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>2025-05-21 11:09:13</t>
+          <t>2025-05-14 14:06:53</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>210526</v>
+        <v>6226</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -5631,14 +5631,14 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L79" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M79" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N79" t="inlineStr">
         <is>
@@ -5654,37 +5654,37 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>251462</v>
+        <v>251467</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D80" t="n">
-        <v>102.0655737704918</v>
+        <v>87.69014084507042</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2025-05-13 09:50:03</t>
+          <t>2025-05-14 12:25:27</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-05-13 10:19:03</t>
+          <t>2025-05-14 12:48:27</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>2025-05-13 10:19:03</t>
+          <t>2025-05-14 12:48:27</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>2025-05-13 12:01:07</t>
+          <t>2025-05-14 14:16:08</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -5720,41 +5720,41 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>251467</v>
+        <v>251374</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D81" t="n">
-        <v>90.23188405797102</v>
+        <v>558.0204081632653</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2025-05-13 09:51:06</t>
+          <t>2025-05-14 13:37:40</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-05-13 10:26:06</t>
+          <t>2025-05-14 14:27:40</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2025-05-13 10:26:06</t>
+          <t>2025-05-14 14:27:40</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>2025-05-13 11:56:20</t>
+          <t>2025-05-16 07:45:41</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>6226</v>
+        <v>27343</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -5763,11 +5763,11 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M81" t="n">
         <v>70</v>
@@ -5786,41 +5786,41 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>251374</v>
+        <v>251520</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>25</v>
+        <v>40.5</v>
       </c>
       <c r="D82" t="n">
-        <v>448.2459016393443</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025-05-13 10:09:36</t>
+          <t>2025-05-14 13:55:58</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-05-13 10:34:36</t>
+          <t>2025-05-14 14:36:28</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>2025-05-13 10:34:36</t>
+          <t>2025-05-14 14:36:28</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>2025-05-14 10:02:51</t>
+          <t>2025-05-15 11:33:33</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>27343</v>
+        <v>16340</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L82" t="n">
@@ -5852,41 +5852,41 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>251520</v>
+        <v>251580</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>40.5</v>
+        <v>35</v>
       </c>
       <c r="D83" t="n">
-        <v>297.0909090909091</v>
+        <v>103.6666666666667</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-05-13 10:46:54</t>
+          <t>2025-05-14 14:06:53</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:24</t>
+          <t>2025-05-14 14:41:53</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:24</t>
+          <t>2025-05-14 14:41:53</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>2025-05-14 08:24:30</t>
+          <t>2025-05-15 08:25:33</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>16340</v>
+        <v>7153</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -5895,11 +5895,11 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M83" t="n">
         <v>70</v>
@@ -5918,41 +5918,41 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>251580</v>
+        <v>251557</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="D84" t="n">
-        <v>100.7464788732394</v>
+        <v>94.43661971830986</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-05-13 10:57:35</t>
+          <t>2025-05-14 14:16:08</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-05-13 12:32:35</t>
+          <t>2025-05-14 14:31:08</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2025-05-13 12:32:35</t>
+          <t>2025-05-14 14:31:08</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>2025-05-13 14:13:20</t>
+          <t>2025-05-15 08:05:34</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>7153</v>
+        <v>6705</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -5965,7 +5965,7 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M84" t="n">
         <v>70</v>
@@ -5984,41 +5984,41 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>251557</v>
+        <v>251562</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D85" t="n">
-        <v>97.17391304347827</v>
+        <v>133.4754098360656</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-05-13 11:56:20</t>
+          <t>2025-05-14 14:27:16</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-05-13 12:21:20</t>
+          <t>2025-05-15 07:07:16</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2025-05-13 12:21:20</t>
+          <t>2025-05-15 07:07:16</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>2025-05-13 13:58:31</t>
+          <t>2025-05-15 09:20:45</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>6705</v>
+        <v>8142</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -6050,41 +6050,41 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>251562</v>
+        <v>251062</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D86" t="n">
-        <v>133.4754098360656</v>
+        <v>318.6478873239437</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-05-13 12:01:07</t>
+          <t>2025-05-15 08:05:34</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-05-13 12:26:07</t>
+          <t>2025-05-15 08:28:34</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>2025-05-13 12:26:07</t>
+          <t>2025-05-15 08:28:34</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>2025-05-13 14:39:36</t>
+          <t>2025-05-15 13:47:13</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>8142</v>
+        <v>22624</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -6093,11 +6093,11 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L86" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M86" t="n">
         <v>70</v>
@@ -6116,41 +6116,41 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>251062</v>
+        <v>251252</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C87" t="n">
         <v>35</v>
       </c>
       <c r="D87" t="n">
-        <v>461.7142857142857</v>
+        <v>218.5942028985507</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2025-05-13 13:29:33</t>
+          <t>2025-05-15 08:25:33</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-05-13 14:04:33</t>
+          <t>2025-05-15 09:00:33</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>2025-05-13 14:04:33</t>
+          <t>2025-05-15 09:00:33</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>2025-05-14 13:46:15</t>
+          <t>2025-05-15 12:39:09</t>
         </is>
       </c>
       <c r="I87" t="n">
-        <v>22624</v>
+        <v>15083</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -6182,41 +6182,41 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>251252</v>
+        <v>251251</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D88" t="n">
-        <v>218.5942028985507</v>
+        <v>260</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2025-05-13 13:58:31</t>
+          <t>2025-05-15 09:20:45</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-05-13 14:43:31</t>
+          <t>2025-05-15 10:00:45</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>2025-05-13 14:43:31</t>
+          <t>2025-05-15 10:00:45</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>2025-05-14 10:22:06</t>
+          <t>2025-05-15 14:20:45</t>
         </is>
       </c>
       <c r="I88" t="n">
-        <v>15083</v>
+        <v>15860</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -6248,41 +6248,41 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>251251</v>
+        <v>251249</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>33</v>
+        <v>32.5</v>
       </c>
       <c r="D89" t="n">
-        <v>260</v>
+        <v>86.50909090909092</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2025-05-13 14:39:36</t>
+          <t>2025-05-15 11:33:33</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2025-05-14 07:12:36</t>
+          <t>2025-05-15 12:06:03</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>2025-05-14 07:12:36</t>
+          <t>2025-05-15 12:06:03</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>2025-05-14 11:32:36</t>
+          <t>2025-05-15 13:32:34</t>
         </is>
       </c>
       <c r="I89" t="n">
-        <v>15860</v>
+        <v>4758</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -6309,72 +6309,6 @@
         <v>0</v>
       </c>
       <c r="P89" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>251249</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>CASON</t>
-        </is>
-      </c>
-      <c r="C90" t="n">
-        <v>32.5</v>
-      </c>
-      <c r="D90" t="n">
-        <v>86.50909090909092</v>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>2025-05-14 08:24:30</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>2025-05-14 08:57:00</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>2025-05-14 08:57:00</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>2025-05-14 10:23:30</t>
-        </is>
-      </c>
-      <c r="I90" t="n">
-        <v>4758</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
-        </is>
-      </c>
-      <c r="L90" t="n">
-        <v>6</v>
-      </c>
-      <c r="M90" t="n">
-        <v>70</v>
-      </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (interno)</t>
-        </is>
-      </c>
-      <c r="O90" t="n">
-        <v>0</v>
-      </c>
-      <c r="P90" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Risolto: basta creare appropriatamente la lista come fatto ora (prima alcuen ne erano escluse in quanto lista_macchine_2 non era una lista appropriatamente contenente tutte le macchine)
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3810,33 +3810,33 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>25</v>
+        <v>210</v>
       </c>
       <c r="D52" t="n">
-        <v>204.9180327868852</v>
+        <v>176.056338028169</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-05-12 09:27:44</t>
+          <t>2025-05-12 07:29:25</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-05-12 09:52:44</t>
+          <t>2025-05-12 10:59:25</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-05-12 09:52:44</t>
+          <t>2025-05-12 10:59:25</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-05-12 13:17:39</t>
+          <t>2025-05-12 13:55:28</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -3876,33 +3876,33 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D53" t="n">
-        <v>131.9591836734694</v>
+        <v>106</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-05-12 10:53:28</t>
+          <t>2025-05-12 09:27:44</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-12 11:33:28</t>
+          <t>2025-05-12 09:52:44</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-12 11:33:28</t>
+          <t>2025-05-12 09:52:44</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-05-12 13:45:25</t>
+          <t>2025-05-12 11:38:44</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -3942,33 +3942,33 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D54" t="n">
-        <v>233.6885245901639</v>
+        <v>290.9183673469388</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-05-12 13:17:39</t>
+          <t>2025-05-12 10:53:28</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-12 13:47:39</t>
+          <t>2025-05-12 11:33:28</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-05-12 13:47:39</t>
+          <t>2025-05-12 11:33:28</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-05-13 09:41:20</t>
+          <t>2025-05-13 08:24:23</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4008,33 +4008,33 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D55" t="n">
-        <v>232.4897959183673</v>
+        <v>186.7540983606557</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-05-12 13:45:25</t>
+          <t>2025-05-12 11:38:44</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-12 14:35:25</t>
+          <t>2025-05-12 12:13:44</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-05-12 14:35:25</t>
+          <t>2025-05-12 12:13:44</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-05-13 10:27:55</t>
+          <t>2025-05-13 07:20:29</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4140,33 +4140,33 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>46.5</v>
+        <v>90</v>
       </c>
       <c r="D57" t="n">
-        <v>441.7090909090909</v>
+        <v>342.1690140845071</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-05-12 14:07:08</t>
+          <t>2025-05-12 13:55:28</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-12 14:53:38</t>
+          <t>2025-05-13 07:25:28</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-05-12 14:53:38</t>
+          <t>2025-05-13 07:25:28</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-05-13 14:15:20</t>
+          <t>2025-05-13 13:07:38</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4202,41 +4202,41 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>243569</v>
+        <v>235572</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>19</v>
+        <v>32.5</v>
       </c>
       <c r="D58" t="n">
-        <v>36.63380281690141</v>
+        <v>181.0545454545455</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-05-12 14:41:22</t>
+          <t>2025-05-12 14:07:08</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-05-13 07:00:22</t>
+          <t>2025-05-12 14:39:38</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-05-13 07:00:22</t>
+          <t>2025-05-12 14:39:38</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2025-05-13 07:37:00</t>
+          <t>2025-05-13 09:40:41</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>2601</v>
+        <v>9958</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -4245,14 +4245,14 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L58" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M58" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N58" t="inlineStr">
         <is>
@@ -4268,7 +4268,7 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>250670</v>
+        <v>243569</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -4276,33 +4276,33 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D59" t="n">
-        <v>22.01408450704225</v>
+        <v>36.63380281690141</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
+          <t>2025-05-12 14:41:22</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:00:22</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2025-05-13 07:00:22</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
           <t>2025-05-13 07:37:00</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>2025-05-13 07:54:00</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>2025-05-13 07:54:00</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>2025-05-13 08:16:01</t>
-        </is>
-      </c>
       <c r="I59" t="n">
-        <v>1563</v>
+        <v>2601</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -4311,11 +4311,11 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M59" t="n">
         <v>76</v>
@@ -4334,41 +4334,41 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>243335</v>
+        <v>250819</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D60" t="n">
-        <v>464.8450704225352</v>
+        <v>139.7868852459016</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-05-13 08:16:01</t>
+          <t>2025-05-13 07:20:29</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-13 08:46:01</t>
+          <t>2025-05-13 08:00:29</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-05-13 08:46:01</t>
+          <t>2025-05-13 08:00:29</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-05-14 08:30:52</t>
+          <t>2025-05-13 10:20:16</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>33004</v>
+        <v>8527</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4377,14 +4377,14 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M60" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N60" t="inlineStr">
         <is>
@@ -4400,41 +4400,41 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>250819</v>
+        <v>250670</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D61" t="n">
-        <v>139.7868852459016</v>
+        <v>22.01408450704225</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-05-13 09:41:20</t>
+          <t>2025-05-13 07:37:00</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-13 10:06:20</t>
+          <t>2025-05-13 07:54:00</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-05-13 10:06:20</t>
+          <t>2025-05-13 07:54:00</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-05-13 12:26:07</t>
+          <t>2025-05-13 08:16:01</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>8527</v>
+        <v>1563</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -4443,14 +4443,14 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M61" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N61" t="inlineStr">
         <is>
@@ -4466,41 +4466,41 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>235572</v>
+        <v>243335</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C62" t="n">
         <v>30</v>
       </c>
       <c r="D62" t="n">
-        <v>140.2535211267606</v>
+        <v>464.8450704225352</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-05-13 09:47:32</t>
+          <t>2025-05-13 08:16:01</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-13 10:17:32</t>
+          <t>2025-05-13 08:46:01</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-05-13 10:17:32</t>
+          <t>2025-05-13 08:46:01</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-05-13 12:37:47</t>
+          <t>2025-05-14 08:30:52</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>9958</v>
+        <v>33004</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -4509,14 +4509,14 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M62" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N62" t="inlineStr">
         <is>
@@ -4540,29 +4540,29 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D63" t="n">
         <v>98.12244897959184</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-05-13 10:27:55</t>
+          <t>2025-05-13 08:24:23</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-13 11:17:55</t>
+          <t>2025-05-13 08:59:23</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-05-13 11:17:55</t>
+          <t>2025-05-13 08:59:23</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-05-13 12:56:02</t>
+          <t>2025-05-13 10:37:30</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -4602,33 +4602,33 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>30</v>
+        <v>36.5</v>
       </c>
       <c r="D64" t="n">
-        <v>63.26229508196721</v>
+        <v>70.16363636363636</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-05-13 12:26:07</t>
+          <t>2025-05-13 09:40:41</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-05-13 12:56:07</t>
+          <t>2025-05-13 10:17:11</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-05-13 12:56:07</t>
+          <t>2025-05-13 10:17:11</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>2025-05-13 13:59:23</t>
+          <t>2025-05-13 11:27:21</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -4672,29 +4672,29 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D65" t="n">
         <v>72.05633802816901</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-05-13 12:37:47</t>
+          <t>2025-05-13 09:47:32</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-05-13 12:54:47</t>
+          <t>2025-05-13 10:19:32</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-05-13 12:54:47</t>
+          <t>2025-05-13 10:19:32</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>2025-05-13 14:06:50</t>
+          <t>2025-05-13 11:31:35</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -4734,33 +4734,33 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D66" t="n">
-        <v>102.0408163265306</v>
+        <v>81.9672131147541</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-05-13 12:56:02</t>
+          <t>2025-05-13 10:20:16</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-05-13 13:51:02</t>
+          <t>2025-05-13 10:55:16</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-05-13 13:51:02</t>
+          <t>2025-05-13 10:55:16</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>2025-05-14 07:33:04</t>
+          <t>2025-05-13 12:17:14</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -4800,33 +4800,33 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D67" t="n">
-        <v>192.4492753623188</v>
+        <v>271</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-05-13 13:48:14</t>
+          <t>2025-05-13 10:37:30</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-05-13 14:43:14</t>
+          <t>2025-05-13 11:17:30</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-05-13 14:43:14</t>
+          <t>2025-05-13 11:17:30</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>2025-05-14 09:55:41</t>
+          <t>2025-05-14 07:48:30</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -4866,33 +4866,33 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>30</v>
+        <v>34.5</v>
       </c>
       <c r="D68" t="n">
-        <v>16.34426229508197</v>
+        <v>18.12727272727273</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-05-13 13:59:23</t>
+          <t>2025-05-13 11:27:21</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-05-13 14:29:23</t>
+          <t>2025-05-13 12:01:51</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-05-13 14:29:23</t>
+          <t>2025-05-13 12:01:51</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>2025-05-13 14:45:44</t>
+          <t>2025-05-13 12:19:58</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -4943,22 +4943,22 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-05-13 14:06:50</t>
+          <t>2025-05-13 11:31:35</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-05-13 14:21:50</t>
+          <t>2025-05-13 11:46:35</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-05-13 14:21:50</t>
+          <t>2025-05-13 11:46:35</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2025-05-13 14:32:27</t>
+          <t>2025-05-13 11:57:12</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -4998,33 +4998,33 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>46.5</v>
+        <v>15</v>
       </c>
       <c r="D70" t="n">
-        <v>13.70909090909091</v>
+        <v>10.61971830985915</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-05-13 14:15:20</t>
+          <t>2025-05-13 11:57:12</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-05-14 07:01:50</t>
+          <t>2025-05-13 12:12:12</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-05-14 07:01:50</t>
+          <t>2025-05-13 12:12:12</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-05-14 07:15:33</t>
+          <t>2025-05-13 12:22:49</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5064,33 +5064,33 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D71" t="n">
-        <v>337.9859154929578</v>
+        <v>393.3934426229508</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-05-13 14:32:27</t>
+          <t>2025-05-13 12:17:14</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-05-13 14:47:27</t>
+          <t>2025-05-13 12:52:14</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-05-13 14:47:27</t>
+          <t>2025-05-13 12:52:14</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>2025-05-14 12:25:27</t>
+          <t>2025-05-14 11:25:38</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5130,33 +5130,33 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>20</v>
+        <v>30.5</v>
       </c>
       <c r="D72" t="n">
-        <v>441.5409836065574</v>
+        <v>489.7090909090909</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-05-13 14:45:44</t>
+          <t>2025-05-13 12:19:58</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-05-14 07:05:44</t>
+          <t>2025-05-13 12:50:28</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-05-14 07:05:44</t>
+          <t>2025-05-13 12:50:28</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>2025-05-14 14:27:16</t>
+          <t>2025-05-14 13:00:11</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5196,33 +5196,33 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>30.5</v>
+        <v>15</v>
       </c>
       <c r="D73" t="n">
-        <v>218.2181818181818</v>
+        <v>169.0422535211268</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-05-14 07:15:33</t>
+          <t>2025-05-13 12:22:49</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-05-14 07:46:03</t>
+          <t>2025-05-13 12:37:49</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-05-14 07:46:03</t>
+          <t>2025-05-13 12:37:49</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>2025-05-14 11:24:16</t>
+          <t>2025-05-14 07:26:52</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5258,41 +5258,41 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>251466</v>
+        <v>251109</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D74" t="n">
-        <v>113.6122448979592</v>
+        <v>266.5915492957747</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-05-14 07:33:04</t>
+          <t>2025-05-13 13:07:38</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-05-14 08:38:04</t>
+          <t>2025-05-13 13:52:38</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-05-14 08:38:04</t>
+          <t>2025-05-13 13:52:38</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-05-14 10:31:41</t>
+          <t>2025-05-14 10:19:14</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>5567</v>
+        <v>18928</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -5301,11 +5301,11 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="M74" t="n">
         <v>70</v>
@@ -5324,41 +5324,41 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>251987</v>
+        <v>251466</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D75" t="n">
-        <v>2965.154929577465</v>
+        <v>80.68115942028986</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-05-14 08:30:52</t>
+          <t>2025-05-13 13:48:14</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-05-14 09:04:52</t>
+          <t>2025-05-13 14:48:14</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-05-14 09:04:52</t>
+          <t>2025-05-13 14:48:14</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-05-22 10:30:01</t>
+          <t>2025-05-14 08:08:55</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>210526</v>
+        <v>5567</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -5367,14 +5367,14 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L75" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M75" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N75" t="inlineStr">
         <is>
@@ -5394,33 +5394,33 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D76" t="n">
-        <v>100.9710144927536</v>
+        <v>98.12676056338029</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2025-05-14 09:55:41</t>
+          <t>2025-05-14 07:26:52</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-05-14 10:20:41</t>
+          <t>2025-05-14 07:45:52</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2025-05-14 10:20:41</t>
+          <t>2025-05-14 07:45:52</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>2025-05-14 12:01:40</t>
+          <t>2025-05-14 09:24:00</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -5464,29 +5464,29 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D77" t="n">
         <v>145.9795918367347</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2025-05-14 10:31:41</t>
+          <t>2025-05-14 07:48:30</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-05-14 11:11:41</t>
+          <t>2025-05-14 08:23:30</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>2025-05-14 11:11:41</t>
+          <t>2025-05-14 08:23:30</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>2025-05-14 13:37:40</t>
+          <t>2025-05-14 10:49:29</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -5526,33 +5526,33 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>38.5</v>
+        <v>30</v>
       </c>
       <c r="D78" t="n">
-        <v>113.2</v>
+        <v>90.23188405797102</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-05-14 11:24:16</t>
+          <t>2025-05-14 08:08:55</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-05-14 12:02:46</t>
+          <t>2025-05-14 08:38:55</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>2025-05-14 12:02:46</t>
+          <t>2025-05-14 08:38:55</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>2025-05-14 13:55:58</t>
+          <t>2025-05-14 10:09:09</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -5588,41 +5588,41 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>251462</v>
+        <v>251987</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D79" t="n">
-        <v>90.23188405797102</v>
+        <v>2965.154929577465</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2025-05-14 12:01:40</t>
+          <t>2025-05-14 08:30:52</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-05-14 12:36:40</t>
+          <t>2025-05-14 09:04:52</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>2025-05-14 12:36:40</t>
+          <t>2025-05-14 09:04:52</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>2025-05-14 14:06:53</t>
+          <t>2025-05-22 10:30:01</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>6226</v>
+        <v>210526</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -5631,14 +5631,14 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L79" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M79" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N79" t="inlineStr">
         <is>
@@ -5654,7 +5654,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>251467</v>
+        <v>251462</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -5662,29 +5662,29 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D80" t="n">
         <v>87.69014084507042</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2025-05-14 12:25:27</t>
+          <t>2025-05-14 09:24:00</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-05-14 12:48:27</t>
+          <t>2025-05-14 09:43:00</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>2025-05-14 12:48:27</t>
+          <t>2025-05-14 09:43:00</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>2025-05-14 14:16:08</t>
+          <t>2025-05-14 11:10:41</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -5720,41 +5720,41 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>251374</v>
+        <v>251467</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D81" t="n">
-        <v>558.0204081632653</v>
+        <v>90.23188405797102</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2025-05-14 13:37:40</t>
+          <t>2025-05-14 10:09:09</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-05-14 14:27:40</t>
+          <t>2025-05-14 10:34:09</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2025-05-14 14:27:40</t>
+          <t>2025-05-14 10:34:09</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>2025-05-16 07:45:41</t>
+          <t>2025-05-14 12:04:23</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>27343</v>
+        <v>6226</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -5763,11 +5763,11 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M81" t="n">
         <v>70</v>
@@ -5790,33 +5790,33 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>40.5</v>
+        <v>80</v>
       </c>
       <c r="D82" t="n">
-        <v>297.0909090909091</v>
+        <v>230.1408450704225</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025-05-14 13:55:58</t>
+          <t>2025-05-14 10:19:14</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-05-14 14:36:28</t>
+          <t>2025-05-14 11:39:14</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>2025-05-14 14:36:28</t>
+          <t>2025-05-14 11:39:14</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>2025-05-15 11:33:33</t>
+          <t>2025-05-15 07:29:22</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -5852,41 +5852,41 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>251580</v>
+        <v>251374</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D83" t="n">
-        <v>103.6666666666667</v>
+        <v>558.0204081632653</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-05-14 14:06:53</t>
+          <t>2025-05-14 10:49:29</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-05-14 14:41:53</t>
+          <t>2025-05-14 11:39:29</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>2025-05-14 14:41:53</t>
+          <t>2025-05-14 11:39:29</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>2025-05-15 08:25:33</t>
+          <t>2025-05-15 12:57:30</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>7153</v>
+        <v>27343</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -5895,11 +5895,11 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M83" t="n">
         <v>70</v>
@@ -5918,7 +5918,7 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>251557</v>
+        <v>251580</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -5926,33 +5926,33 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D84" t="n">
-        <v>94.43661971830986</v>
+        <v>100.7464788732394</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-05-14 14:16:08</t>
+          <t>2025-05-14 11:10:41</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-05-14 14:31:08</t>
+          <t>2025-05-14 11:29:41</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2025-05-14 14:31:08</t>
+          <t>2025-05-14 11:29:41</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>2025-05-15 08:05:34</t>
+          <t>2025-05-14 13:10:26</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>6705</v>
+        <v>7153</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -5965,7 +5965,7 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M84" t="n">
         <v>70</v>
@@ -5984,7 +5984,7 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>251562</v>
+        <v>251557</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -5995,30 +5995,30 @@
         <v>40</v>
       </c>
       <c r="D85" t="n">
-        <v>133.4754098360656</v>
+        <v>109.9180327868852</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-05-14 14:27:16</t>
+          <t>2025-05-14 11:25:38</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-05-15 07:07:16</t>
+          <t>2025-05-14 12:05:38</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2025-05-15 07:07:16</t>
+          <t>2025-05-14 12:05:38</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>2025-05-15 09:20:45</t>
+          <t>2025-05-14 13:55:33</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>8142</v>
+        <v>6705</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -6050,41 +6050,41 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>251062</v>
+        <v>251562</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D86" t="n">
-        <v>318.6478873239437</v>
+        <v>118</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-05-15 08:05:34</t>
+          <t>2025-05-14 12:04:23</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-05-15 08:28:34</t>
+          <t>2025-05-14 12:29:23</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>2025-05-15 08:28:34</t>
+          <t>2025-05-14 12:29:23</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>2025-05-15 13:47:13</t>
+          <t>2025-05-14 14:27:23</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>22624</v>
+        <v>8142</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -6093,11 +6093,11 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L86" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M86" t="n">
         <v>70</v>
@@ -6116,41 +6116,41 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>251252</v>
+        <v>251062</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>35</v>
+        <v>30.5</v>
       </c>
       <c r="D87" t="n">
-        <v>218.5942028985507</v>
+        <v>411.3454545454546</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2025-05-15 08:25:33</t>
+          <t>2025-05-14 13:00:11</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-05-15 09:00:33</t>
+          <t>2025-05-14 13:30:41</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>2025-05-15 09:00:33</t>
+          <t>2025-05-14 13:30:41</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>2025-05-15 12:39:09</t>
+          <t>2025-05-15 12:22:02</t>
         </is>
       </c>
       <c r="I87" t="n">
-        <v>15083</v>
+        <v>22624</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -6182,41 +6182,41 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>251251</v>
+        <v>251252</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D88" t="n">
-        <v>260</v>
+        <v>212.4366197183099</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2025-05-15 09:20:45</t>
+          <t>2025-05-14 13:10:26</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-05-15 10:00:45</t>
+          <t>2025-05-14 13:29:26</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>2025-05-15 10:00:45</t>
+          <t>2025-05-14 13:29:26</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>2025-05-15 14:20:45</t>
+          <t>2025-05-15 09:01:52</t>
         </is>
       </c>
       <c r="I88" t="n">
-        <v>15860</v>
+        <v>15083</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -6248,41 +6248,41 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>251249</v>
+        <v>251251</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>32.5</v>
+        <v>40</v>
       </c>
       <c r="D89" t="n">
-        <v>86.50909090909092</v>
+        <v>260</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2025-05-15 11:33:33</t>
+          <t>2025-05-14 13:55:33</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2025-05-15 12:06:03</t>
+          <t>2025-05-14 14:35:33</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>2025-05-15 12:06:03</t>
+          <t>2025-05-14 14:35:33</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>2025-05-15 13:32:34</t>
+          <t>2025-05-15 10:55:33</t>
         </is>
       </c>
       <c r="I89" t="n">
-        <v>4758</v>
+        <v>15860</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -6309,6 +6309,72 @@
         <v>0</v>
       </c>
       <c r="P89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>251249</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>R9</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>45</v>
+      </c>
+      <c r="D90" t="n">
+        <v>68.95652173913044</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2025-05-14 14:27:23</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>2025-05-15 07:12:23</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>2025-05-15 07:12:23</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2025-05-15 08:21:20</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>4758</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+        </is>
+      </c>
+      <c r="L90" t="n">
+        <v>6</v>
+      </c>
+      <c r="M90" t="n">
+        <v>70</v>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
+      </c>
+      <c r="O90" t="n">
+        <v>0</v>
+      </c>
+      <c r="P90" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambiamenti minori al codice + fatto sì che le commesse esterne senza veicolo tassativamente associato fossero trattate alla stregua di commesse interne a zona chiusa (come da riunione)
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -2228,7 +2228,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251340</v>
+        <v>250894</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2236,10 +2236,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D28" t="n">
-        <v>461.9718309859155</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -2248,21 +2248,21 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-08 12:15:00</t>
+          <t>2025-05-08 12:21:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-08 12:15:00</t>
+          <t>2025-05-08 12:21:00</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-09 11:56:58</t>
+          <t>2025-05-09 14:44:24</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>32800</v>
+        <v>44262</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2275,15 +2275,13 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M28" t="n">
         <v>76</v>
       </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+      <c r="N28" t="n">
+        <v>39755</v>
       </c>
       <c r="O28" t="n">
         <v>0</v>
@@ -2294,7 +2292,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251561</v>
+        <v>251651</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2302,10 +2300,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D29" t="n">
-        <v>76.54929577464789</v>
+        <v>659.5774647887324</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -2314,21 +2312,21 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:44:22</t>
+          <t>2025-05-09 07:59:22</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:44:22</t>
+          <t>2025-05-09 07:59:22</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-09 09:00:55</t>
+          <t>2025-05-12 10:58:57</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>5435</v>
+        <v>46830</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2337,19 +2335,17 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L29" t="n">
         <v>5</v>
       </c>
       <c r="M29" t="n">
-        <v>70</v>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N29" t="n">
+        <v>39755</v>
       </c>
       <c r="O29" t="n">
         <v>0</v>
@@ -2360,41 +2356,41 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251564</v>
+        <v>251416</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D30" t="n">
-        <v>38.26760563380282</v>
+        <v>175.34375</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-09 09:00:55</t>
+          <t>2025-05-09 09:06:46</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-09 09:19:55</t>
+          <t>2025-05-09 09:23:46</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-09 09:19:55</t>
+          <t>2025-05-09 09:23:46</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-09 09:58:11</t>
+          <t>2025-05-09 12:19:07</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>2717</v>
+        <v>11222</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2407,15 +2403,13 @@
         </is>
       </c>
       <c r="L30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M30" t="n">
         <v>70</v>
       </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>NESSUN VEICOLO (esterno)</t>
-        </is>
+      <c r="N30" t="n">
+        <v>39755</v>
       </c>
       <c r="O30" t="n">
         <v>0</v>
@@ -2426,41 +2420,41 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>251566</v>
+        <v>251561</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D31" t="n">
-        <v>107.640625</v>
+        <v>110.9183673469388</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-05-09 09:06:46</t>
+          <t>2025-05-09 09:14:40</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-05-09 09:23:46</t>
+          <t>2025-05-09 09:54:40</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-05-09 09:23:46</t>
+          <t>2025-05-09 09:54:40</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-05-09 11:11:25</t>
+          <t>2025-05-09 11:45:35</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>6889</v>
+        <v>5435</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2473,14 +2467,14 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M31" t="n">
         <v>70</v>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O31" t="n">
@@ -2492,41 +2486,41 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>251519</v>
+        <v>251564</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D32" t="n">
-        <v>268.8775510204082</v>
+        <v>44.54098360655738</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-05-09 09:14:40</t>
+          <t>2025-05-09 10:06:22</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-05-09 09:59:40</t>
+          <t>2025-05-09 10:41:22</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-05-09 09:59:40</t>
+          <t>2025-05-09 10:41:22</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-05-09 14:28:33</t>
+          <t>2025-05-09 11:25:55</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>13175</v>
+        <v>2717</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2539,14 +2533,14 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M32" t="n">
         <v>70</v>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O32" t="n">
@@ -2558,41 +2552,41 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>251373</v>
+        <v>251566</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D33" t="n">
-        <v>240.7605633802817</v>
+        <v>112.9344262295082</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-05-09 09:58:11</t>
+          <t>2025-05-09 11:25:55</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-09 10:17:11</t>
+          <t>2025-05-09 11:50:55</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-05-09 10:17:11</t>
+          <t>2025-05-09 11:50:55</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-09 14:17:57</t>
+          <t>2025-05-09 13:43:51</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>17094</v>
+        <v>6889</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -2605,14 +2599,14 @@
         </is>
       </c>
       <c r="L33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M33" t="n">
         <v>70</v>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O33" t="n">
@@ -2624,41 +2618,41 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>251424</v>
+        <v>251626</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D34" t="n">
-        <v>158.3934426229508</v>
+        <v>255.1020408163265</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-05-09 10:06:22</t>
+          <t>2025-05-09 11:45:35</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-05-09 10:36:22</t>
+          <t>2025-05-09 12:30:35</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-05-09 10:36:22</t>
+          <t>2025-05-09 12:30:35</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-05-09 13:14:46</t>
+          <t>2025-05-12 08:45:41</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>9662</v>
+        <v>12500</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2671,7 +2665,7 @@
         </is>
       </c>
       <c r="L34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M34" t="n">
         <v>70</v>
@@ -2690,7 +2684,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>251397</v>
+        <v>251546</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -2698,33 +2692,33 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D35" t="n">
-        <v>84.921875</v>
+        <v>101.03125</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-05-09 11:11:25</t>
+          <t>2025-05-09 12:19:07</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-09 11:28:25</t>
+          <t>2025-05-09 12:40:07</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-05-09 11:28:25</t>
+          <t>2025-05-09 12:40:07</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-05-09 12:53:20</t>
+          <t>2025-05-09 14:21:09</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>5435</v>
+        <v>6466</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -2737,7 +2731,7 @@
         </is>
       </c>
       <c r="L35" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M35" t="n">
         <v>70</v>
@@ -2756,41 +2750,41 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>250894</v>
+        <v>251505</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>21</v>
+        <v>34.5</v>
       </c>
       <c r="D36" t="n">
-        <v>623.4084507042254</v>
+        <v>259.1818181818182</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-05-09 11:56:58</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-09 12:17:58</t>
+          <t>2025-05-09 13:12:05</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-05-09 12:17:58</t>
+          <t>2025-05-09 13:12:05</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-12 14:41:22</t>
+          <t>2025-05-12 09:31:16</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>44262</v>
+        <v>14255</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -2799,17 +2793,19 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L36" t="n">
         <v>5</v>
       </c>
       <c r="M36" t="n">
-        <v>76</v>
-      </c>
-      <c r="N36" t="n">
-        <v>39755</v>
+        <v>70</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
       <c r="O36" t="n">
         <v>0</v>
@@ -2820,41 +2816,41 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>251475</v>
+        <v>251846</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>36.5</v>
+        <v>33</v>
       </c>
       <c r="D37" t="n">
-        <v>157.8363636363636</v>
+        <v>186.7540983606557</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-09 12:53:11</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-09 13:14:05</t>
+          <t>2025-05-09 13:26:11</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-05-09 13:14:05</t>
+          <t>2025-05-09 13:26:11</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-05-12 07:51:55</t>
+          <t>2025-05-12 08:32:57</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>8681</v>
+        <v>11392</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -2867,7 +2863,7 @@
         </is>
       </c>
       <c r="L37" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M37" t="n">
         <v>70</v>
@@ -2886,41 +2882,41 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>251594</v>
+        <v>251519</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D38" t="n">
-        <v>106</v>
+        <v>215.983606557377</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-05-09 12:53:11</t>
+          <t>2025-05-09 13:43:51</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-05-09 13:22:11</t>
+          <t>2025-05-09 14:13:51</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-05-09 13:22:11</t>
+          <t>2025-05-09 14:13:51</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-05-12 07:08:11</t>
+          <t>2025-05-12 09:49:50</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>6466</v>
+        <v>13175</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -2933,14 +2929,14 @@
         </is>
       </c>
       <c r="L38" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M38" t="n">
         <v>70</v>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O38" t="n">
@@ -2952,7 +2948,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>244354</v>
+        <v>245275</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -2960,33 +2956,33 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D39" t="n">
-        <v>67.34375</v>
+        <v>379.59375</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-05-09 12:53:20</t>
+          <t>2025-05-09 14:21:09</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-05-09 13:10:20</t>
+          <t>2025-05-09 14:54:09</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-05-09 13:10:20</t>
+          <t>2025-05-09 14:54:09</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-05-09 14:17:41</t>
+          <t>2025-05-12 13:13:45</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>4310</v>
+        <v>24294</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -2995,11 +2991,11 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;CASON ;R6</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="M39" t="n">
         <v>70</v>
@@ -3018,41 +3014,41 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>244355</v>
+        <v>251340</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D40" t="n">
-        <v>70.65573770491804</v>
+        <v>461.9718309859155</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-05-09 13:14:46</t>
+          <t>2025-05-09 14:44:24</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-05-09 13:34:46</t>
+          <t>2025-05-12 07:05:24</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-05-09 13:34:46</t>
+          <t>2025-05-12 07:05:24</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-05-09 14:45:25</t>
+          <t>2025-05-12 14:47:22</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>4310</v>
+        <v>32800</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3061,18 +3057,18 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L40" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M40" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O40" t="n">
@@ -3084,41 +3080,41 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>244204</v>
+        <v>245350</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D41" t="n">
-        <v>54.25</v>
+        <v>405.3623188405797</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-05-09 14:17:41</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-05-09 14:32:41</t>
+          <t>2025-05-12 08:05:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-05-09 14:32:41</t>
+          <t>2025-05-12 08:05:00</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-05-12 07:26:56</t>
+          <t>2025-05-12 14:50:21</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>3472</v>
+        <v>27970</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3127,11 +3123,11 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M41" t="n">
         <v>70</v>
@@ -3150,41 +3146,41 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>251651</v>
+        <v>235572</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="D42" t="n">
-        <v>659.5774647887324</v>
+        <v>140.2535211267606</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-05-09 14:17:57</t>
+          <t>2025-05-12 07:29:25</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-05-09 14:47:57</t>
+          <t>2025-05-12 10:49:25</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-05-09 14:47:57</t>
+          <t>2025-05-12 10:49:25</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-05-13 09:47:32</t>
+          <t>2025-05-12 13:09:40</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>46830</v>
+        <v>9958</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3193,17 +3189,19 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L42" t="n">
         <v>5</v>
       </c>
       <c r="M42" t="n">
-        <v>76</v>
-      </c>
-      <c r="N42" t="n">
-        <v>39755</v>
+        <v>70</v>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (esterno)</t>
+        </is>
       </c>
       <c r="O42" t="n">
         <v>0</v>
@@ -3214,41 +3212,41 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>251743</v>
+        <v>251373</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D43" t="n">
-        <v>219.9183673469388</v>
+        <v>280.2295081967213</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-05-09 14:28:33</t>
+          <t>2025-05-12 08:32:57</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-05-12 07:13:33</t>
+          <t>2025-05-12 09:03:57</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-05-12 07:13:33</t>
+          <t>2025-05-12 09:03:57</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-05-12 10:53:28</t>
+          <t>2025-05-12 13:44:10</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>10776</v>
+        <v>17094</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3261,14 +3259,14 @@
         </is>
       </c>
       <c r="L43" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M43" t="n">
         <v>70</v>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O43" t="n">
@@ -3280,41 +3278,41 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>251809</v>
+        <v>251424</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D44" t="n">
-        <v>142.3114754098361</v>
+        <v>197.1836734693877</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-05-09 14:45:25</t>
+          <t>2025-05-12 08:45:41</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-05-12 07:05:25</t>
+          <t>2025-05-12 09:25:41</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-05-12 07:05:25</t>
+          <t>2025-05-12 09:25:41</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-05-12 09:27:44</t>
+          <t>2025-05-12 12:42:52</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>8681</v>
+        <v>9662</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3334,7 +3332,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O44" t="n">
@@ -3346,41 +3344,41 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>245623</v>
+        <v>251397</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>30</v>
+        <v>34.5</v>
       </c>
       <c r="D45" t="n">
-        <v>382.8840579710145</v>
+        <v>98.81818181818181</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-12 09:31:16</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-05-12 07:30:00</t>
+          <t>2025-05-12 10:05:46</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-05-12 07:30:00</t>
+          <t>2025-05-12 10:05:46</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-05-12 13:52:53</t>
+          <t>2025-05-12 11:44:35</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>26419</v>
+        <v>5435</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3389,18 +3387,18 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M45" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O45" t="n">
@@ -3412,41 +3410,41 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>251416</v>
+        <v>251475</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D46" t="n">
-        <v>183.9672131147541</v>
+        <v>142.3114754098361</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-05-12 07:08:11</t>
+          <t>2025-05-12 09:49:50</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-05-12 07:37:11</t>
+          <t>2025-05-12 10:19:50</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-05-12 07:37:11</t>
+          <t>2025-05-12 10:19:50</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-05-12 10:41:09</t>
+          <t>2025-05-12 12:42:08</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>11222</v>
+        <v>8681</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3459,13 +3457,15 @@
         </is>
       </c>
       <c r="L46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M46" t="n">
         <v>70</v>
       </c>
-      <c r="N46" t="n">
-        <v>39755</v>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>NESSUN VEICOLO (interno)</t>
+        </is>
       </c>
       <c r="O46" t="n">
         <v>0</v>
@@ -3476,41 +3476,41 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>251260</v>
+        <v>251594</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D47" t="n">
-        <v>146.390625</v>
+        <v>91.07042253521126</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-05-12 07:26:56</t>
+          <t>2025-05-12 10:58:57</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-05-12 07:45:56</t>
+          <t>2025-05-12 11:30:57</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-05-12 07:45:56</t>
+          <t>2025-05-12 11:30:57</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-05-12 10:12:19</t>
+          <t>2025-05-12 13:02:01</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>9369</v>
+        <v>6466</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3519,18 +3519,18 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L47" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M47" t="n">
         <v>70</v>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O47" t="n">
@@ -3542,7 +3542,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>251795</v>
+        <v>244354</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -3550,33 +3550,33 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
       <c r="D48" t="n">
-        <v>340.7090909090909</v>
+        <v>78.36363636363636</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-05-12 07:51:55</t>
+          <t>2025-05-12 11:44:35</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-05-12 08:26:25</t>
+          <t>2025-05-12 12:17:05</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-05-12 08:26:25</t>
+          <t>2025-05-12 12:17:05</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-05-12 14:07:08</t>
+          <t>2025-05-12 13:35:27</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>18739</v>
+        <v>4310</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -3585,18 +3585,18 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L48" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M48" t="n">
         <v>70</v>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O48" t="n">
@@ -3608,41 +3608,41 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>251750</v>
+        <v>244355</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D49" t="n">
-        <v>60.796875</v>
+        <v>70.65573770491804</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-05-12 10:12:19</t>
+          <t>2025-05-12 12:42:08</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-05-12 10:48:19</t>
+          <t>2025-05-12 13:02:08</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-05-12 10:48:19</t>
+          <t>2025-05-12 13:02:08</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-05-12 11:49:07</t>
+          <t>2025-05-12 14:12:48</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>3891</v>
+        <v>4310</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -3651,18 +3651,18 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L49" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M49" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O49" t="n">
@@ -3674,41 +3674,41 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>245090</v>
+        <v>244204</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D50" t="n">
-        <v>8470.786885245901</v>
+        <v>70.85714285714286</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-05-12 10:41:09</t>
+          <t>2025-05-12 12:42:52</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-05-12 11:27:09</t>
+          <t>2025-05-12 13:17:52</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-05-12 11:27:09</t>
+          <t>2025-05-12 13:17:52</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-06-05 08:37:57</t>
+          <t>2025-05-12 14:28:44</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>516718</v>
+        <v>3472</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -3717,18 +3717,18 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M50" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O50" t="n">
@@ -3740,41 +3740,41 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>245089</v>
+        <v>251743</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D51" t="n">
-        <v>1916.640625</v>
+        <v>151.7746478873239</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-05-12 11:49:07</t>
+          <t>2025-05-12 13:02:01</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-05-12 12:21:07</t>
+          <t>2025-05-12 13:17:01</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-05-12 12:21:07</t>
+          <t>2025-05-12 13:17:01</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-05-16 12:17:45</t>
+          <t>2025-05-13 07:48:48</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>122665</v>
+        <v>10776</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -3783,18 +3783,18 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L51" t="n">
         <v>4</v>
       </c>
       <c r="M51" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (esterno)</t>
+          <t>NESSUN VEICOLO (interno)</t>
         </is>
       </c>
       <c r="O51" t="n">
@@ -3806,7 +3806,7 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>251626</v>
+        <v>251809</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -3814,33 +3814,33 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>210</v>
+        <v>40</v>
       </c>
       <c r="D52" t="n">
-        <v>176.056338028169</v>
+        <v>122.2676056338028</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-05-12 07:29:25</t>
+          <t>2025-05-12 13:09:40</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-05-12 10:59:25</t>
+          <t>2025-05-12 13:49:40</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-05-12 10:59:25</t>
+          <t>2025-05-12 13:49:40</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-05-12 13:55:28</t>
+          <t>2025-05-13 07:51:56</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>12500</v>
+        <v>8681</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
         </is>
       </c>
       <c r="L52" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M52" t="n">
         <v>70</v>
@@ -3872,41 +3872,41 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>251546</v>
+        <v>243569</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D53" t="n">
-        <v>106</v>
+        <v>40.640625</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-05-12 09:27:44</t>
+          <t>2025-05-12 13:13:45</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-12 09:52:44</t>
+          <t>2025-05-12 14:05:45</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-12 09:52:44</t>
+          <t>2025-05-12 14:05:45</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-05-12 11:38:44</t>
+          <t>2025-05-12 14:46:23</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>6466</v>
+        <v>2601</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -3915,18 +3915,18 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L53" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M53" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O53" t="n">
@@ -3938,41 +3938,41 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>251505</v>
+        <v>250819</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>40</v>
+        <v>34.5</v>
       </c>
       <c r="D54" t="n">
-        <v>290.9183673469388</v>
+        <v>155.0363636363636</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-05-12 10:53:28</t>
+          <t>2025-05-12 13:35:27</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-12 11:33:28</t>
+          <t>2025-05-12 14:09:57</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-05-12 11:33:28</t>
+          <t>2025-05-12 14:09:57</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-05-13 08:24:23</t>
+          <t>2025-05-13 08:44:59</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>14255</v>
+        <v>8527</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -3985,14 +3985,14 @@
         </is>
       </c>
       <c r="L54" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M54" t="n">
         <v>70</v>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O54" t="n">
@@ -4004,41 +4004,41 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>251846</v>
+        <v>245623</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D55" t="n">
-        <v>186.7540983606557</v>
+        <v>433.0983606557377</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-05-12 11:38:44</t>
+          <t>2025-05-12 13:44:10</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-12 12:13:44</t>
+          <t>2025-05-12 14:30:10</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-05-12 12:13:44</t>
+          <t>2025-05-12 14:30:10</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-05-13 07:20:29</t>
+          <t>2025-05-13 13:43:16</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>11392</v>
+        <v>26419</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -4047,14 +4047,14 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L55" t="n">
         <v>2</v>
       </c>
       <c r="M55" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N55" t="inlineStr">
         <is>
@@ -4070,41 +4070,41 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>245350</v>
+        <v>251485</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="D56" t="n">
-        <v>405.3623188405797</v>
+        <v>78.81967213114754</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-05-12 13:52:53</t>
+          <t>2025-05-12 14:12:48</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-05-13 07:02:53</t>
+          <t>2025-05-12 14:37:48</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-05-13 07:02:53</t>
+          <t>2025-05-12 14:37:48</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-05-13 13:48:14</t>
+          <t>2025-05-13 07:56:37</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>27970</v>
+        <v>4808</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -4113,18 +4113,18 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L56" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M56" t="n">
         <v>70</v>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O56" t="n">
@@ -4136,41 +4136,41 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>245275</v>
+        <v>251346</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="D57" t="n">
-        <v>342.1690140845071</v>
+        <v>78.75510204081633</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-05-12 13:55:28</t>
+          <t>2025-05-12 14:28:44</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-13 07:25:28</t>
+          <t>2025-05-13 07:23:44</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-05-13 07:25:28</t>
+          <t>2025-05-13 07:23:44</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-05-13 13:07:38</t>
+          <t>2025-05-13 08:42:29</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>24294</v>
+        <v>3859</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -4179,18 +4179,18 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L57" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="M57" t="n">
         <v>70</v>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O57" t="n">
@@ -4202,41 +4202,41 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>235572</v>
+        <v>250641</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>32.5</v>
+        <v>36</v>
       </c>
       <c r="D58" t="n">
-        <v>181.0545454545455</v>
+        <v>79.9375</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-05-12 14:07:08</t>
+          <t>2025-05-12 14:46:23</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-05-12 14:39:38</t>
+          <t>2025-05-13 07:22:23</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-05-12 14:39:38</t>
+          <t>2025-05-13 07:22:23</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2025-05-13 09:40:41</t>
+          <t>2025-05-13 08:42:19</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>9958</v>
+        <v>5116</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -4245,18 +4245,18 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L58" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M58" t="n">
         <v>70</v>
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O58" t="n">
@@ -4268,7 +4268,7 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>243569</v>
+        <v>250670</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -4279,30 +4279,30 @@
         <v>19</v>
       </c>
       <c r="D59" t="n">
-        <v>36.63380281690141</v>
+        <v>22.01408450704225</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-05-12 14:41:22</t>
+          <t>2025-05-12 14:47:22</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-05-13 07:00:22</t>
+          <t>2025-05-13 07:06:22</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-05-13 07:00:22</t>
+          <t>2025-05-13 07:06:22</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2025-05-13 07:37:00</t>
+          <t>2025-05-13 07:28:23</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>2601</v>
+        <v>1563</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -4311,18 +4311,18 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L59" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M59" t="n">
         <v>76</v>
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O59" t="n">
@@ -4334,41 +4334,41 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>250819</v>
+        <v>251259</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D60" t="n">
-        <v>139.7868852459016</v>
+        <v>72.46376811594203</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-05-13 07:20:29</t>
+          <t>2025-05-12 14:50:21</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-13 08:00:29</t>
+          <t>2025-05-13 07:20:21</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-05-13 08:00:29</t>
+          <t>2025-05-13 07:20:21</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-05-13 10:20:16</t>
+          <t>2025-05-13 08:32:49</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>8527</v>
+        <v>5000</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4381,14 +4381,14 @@
         </is>
       </c>
       <c r="L60" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M60" t="n">
         <v>70</v>
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O60" t="n">
@@ -4400,7 +4400,7 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>250670</v>
+        <v>243335</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -4408,33 +4408,33 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D61" t="n">
-        <v>22.01408450704225</v>
+        <v>464.8450704225352</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-05-13 07:37:00</t>
+          <t>2025-05-13 07:28:23</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-13 07:54:00</t>
+          <t>2025-05-13 07:58:23</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-05-13 07:54:00</t>
+          <t>2025-05-13 07:58:23</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-05-13 08:16:01</t>
+          <t>2025-05-14 07:43:14</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>1563</v>
+        <v>33004</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -4443,18 +4443,18 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L61" t="n">
         <v>4</v>
       </c>
       <c r="M61" t="n">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O61" t="n">
@@ -4466,41 +4466,41 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>243335</v>
+        <v>251761</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D62" t="n">
-        <v>464.8450704225352</v>
+        <v>187.0281690140845</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:16:01</t>
+          <t>2025-05-13 07:48:48</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:46:01</t>
+          <t>2025-05-13 08:03:48</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:46:01</t>
+          <t>2025-05-13 08:03:48</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-05-14 08:30:52</t>
+          <t>2025-05-13 11:10:49</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>33004</v>
+        <v>13279</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -4509,18 +4509,18 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L62" t="n">
         <v>4</v>
       </c>
       <c r="M62" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O62" t="n">
@@ -4532,41 +4532,41 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>251485</v>
+        <v>251109</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="D63" t="n">
-        <v>98.12244897959184</v>
+        <v>266.5915492957747</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-05-13 08:24:23</t>
+          <t>2025-05-13 07:51:56</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-13 08:59:23</t>
+          <t>2025-05-13 09:26:56</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-05-13 08:59:23</t>
+          <t>2025-05-13 09:26:56</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-05-13 10:37:30</t>
+          <t>2025-05-13 13:53:32</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>4808</v>
+        <v>18928</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -4575,18 +4575,18 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L63" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="M63" t="n">
         <v>70</v>
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O63" t="n">
@@ -4598,41 +4598,41 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>251346</v>
+        <v>244023</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>36.5</v>
+        <v>25</v>
       </c>
       <c r="D64" t="n">
-        <v>70.16363636363636</v>
+        <v>16.34426229508197</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-05-13 09:40:41</t>
+          <t>2025-05-13 07:56:37</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-05-13 10:17:11</t>
+          <t>2025-05-13 08:21:37</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-05-13 10:17:11</t>
+          <t>2025-05-13 08:21:37</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:21</t>
+          <t>2025-05-13 08:37:58</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>3859</v>
+        <v>997</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -4645,14 +4645,14 @@
         </is>
       </c>
       <c r="L64" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M64" t="n">
         <v>70</v>
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O64" t="n">
@@ -4664,41 +4664,41 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>250641</v>
+        <v>251283</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D65" t="n">
-        <v>72.05633802816901</v>
+        <v>10.92753623188406</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-05-13 09:47:32</t>
+          <t>2025-05-13 08:32:49</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-05-13 10:19:32</t>
+          <t>2025-05-13 09:12:49</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-05-13 10:19:32</t>
+          <t>2025-05-13 09:12:49</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>2025-05-13 11:31:35</t>
+          <t>2025-05-13 09:23:45</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>5116</v>
+        <v>754</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -4707,7 +4707,7 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L65" t="n">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O65" t="n">
@@ -4730,7 +4730,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>251259</v>
+        <v>251245</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -4738,33 +4738,33 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D66" t="n">
-        <v>81.9672131147541</v>
+        <v>12.36065573770492</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-05-13 10:20:16</t>
+          <t>2025-05-13 08:37:58</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-05-13 10:55:16</t>
+          <t>2025-05-13 08:57:58</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-05-13 10:55:16</t>
+          <t>2025-05-13 08:57:58</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>2025-05-13 12:17:14</t>
+          <t>2025-05-13 09:10:19</t>
         </is>
       </c>
       <c r="I66" t="n">
-        <v>5000</v>
+        <v>754</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -4773,18 +4773,18 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L66" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M66" t="n">
         <v>70</v>
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O66" t="n">
@@ -4796,41 +4796,41 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>251761</v>
+        <v>251061</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D67" t="n">
-        <v>271</v>
+        <v>374.953125</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-05-13 10:37:30</t>
+          <t>2025-05-13 08:42:19</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-05-13 11:17:30</t>
+          <t>2025-05-13 08:57:19</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-05-13 11:17:30</t>
+          <t>2025-05-13 08:57:19</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>2025-05-14 07:48:30</t>
+          <t>2025-05-14 07:12:16</t>
         </is>
       </c>
       <c r="I67" t="n">
-        <v>13279</v>
+        <v>23997</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -4839,18 +4839,18 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L67" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M67" t="n">
         <v>70</v>
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O67" t="n">
@@ -4862,41 +4862,41 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>244023</v>
+        <v>251247</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>34.5</v>
+        <v>45</v>
       </c>
       <c r="D68" t="n">
-        <v>18.12727272727273</v>
+        <v>549.6734693877551</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:21</t>
+          <t>2025-05-13 08:42:29</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-05-13 12:01:51</t>
+          <t>2025-05-13 09:27:29</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-05-13 12:01:51</t>
+          <t>2025-05-13 09:27:29</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>2025-05-13 12:19:58</t>
+          <t>2025-05-14 10:37:09</t>
         </is>
       </c>
       <c r="I68" t="n">
-        <v>997</v>
+        <v>26934</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L68" t="n">
@@ -4916,7 +4916,7 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O68" t="n">
@@ -4928,41 +4928,41 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>251283</v>
+        <v>251246</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>15</v>
+        <v>30.5</v>
       </c>
       <c r="D69" t="n">
-        <v>10.61971830985915</v>
+        <v>218.2181818181818</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-05-13 11:31:35</t>
+          <t>2025-05-13 08:44:59</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-05-13 11:46:35</t>
+          <t>2025-05-13 09:15:29</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-05-13 11:46:35</t>
+          <t>2025-05-13 09:15:29</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2025-05-13 11:57:12</t>
+          <t>2025-05-13 12:53:42</t>
         </is>
       </c>
       <c r="I69" t="n">
-        <v>754</v>
+        <v>12002</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O69" t="n">
@@ -4994,41 +4994,41 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>251245</v>
+        <v>251466</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D70" t="n">
-        <v>10.61971830985915</v>
+        <v>91.26229508196721</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-05-13 11:57:12</t>
+          <t>2025-05-13 09:10:19</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-05-13 12:12:12</t>
+          <t>2025-05-13 09:45:19</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-05-13 12:12:12</t>
+          <t>2025-05-13 09:45:19</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-05-13 12:22:49</t>
+          <t>2025-05-13 11:16:35</t>
         </is>
       </c>
       <c r="I70" t="n">
-        <v>754</v>
+        <v>5567</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -5037,18 +5037,18 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L70" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M70" t="n">
         <v>70</v>
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O70" t="n">
@@ -5060,41 +5060,41 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>251061</v>
+        <v>251463</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C71" t="n">
         <v>35</v>
       </c>
       <c r="D71" t="n">
-        <v>393.3934426229508</v>
+        <v>100.9710144927536</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-05-13 12:17:14</t>
+          <t>2025-05-13 09:23:45</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-05-13 12:52:14</t>
+          <t>2025-05-13 09:58:45</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-05-13 12:52:14</t>
+          <t>2025-05-13 09:58:45</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>2025-05-14 11:25:38</t>
+          <t>2025-05-13 11:39:43</t>
         </is>
       </c>
       <c r="I71" t="n">
-        <v>23997</v>
+        <v>6967</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -5103,18 +5103,18 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L71" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M71" t="n">
         <v>70</v>
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O71" t="n">
@@ -5126,41 +5126,41 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>251247</v>
+        <v>251464</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>30.5</v>
+        <v>15</v>
       </c>
       <c r="D72" t="n">
-        <v>489.7090909090909</v>
+        <v>100.7464788732394</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-05-13 12:19:58</t>
+          <t>2025-05-13 11:10:49</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-05-13 12:50:28</t>
+          <t>2025-05-13 11:25:49</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-05-13 12:50:28</t>
+          <t>2025-05-13 11:25:49</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>2025-05-14 13:00:11</t>
+          <t>2025-05-13 13:06:34</t>
         </is>
       </c>
       <c r="I72" t="n">
-        <v>26934</v>
+        <v>7153</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -5169,18 +5169,18 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L72" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M72" t="n">
         <v>70</v>
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O72" t="n">
@@ -5192,41 +5192,41 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>251246</v>
+        <v>251465</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D73" t="n">
-        <v>169.0422535211268</v>
+        <v>102.0655737704918</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-05-13 12:22:49</t>
+          <t>2025-05-13 11:16:35</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-05-13 12:37:49</t>
+          <t>2025-05-13 11:41:35</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-05-13 12:37:49</t>
+          <t>2025-05-13 11:41:35</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>2025-05-14 07:26:52</t>
+          <t>2025-05-13 13:23:39</t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>12002</v>
+        <v>6226</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -5235,18 +5235,18 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L73" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M73" t="n">
         <v>70</v>
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O73" t="n">
@@ -5258,41 +5258,41 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>251109</v>
+        <v>251462</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D74" t="n">
-        <v>266.5915492957747</v>
+        <v>90.23188405797102</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-05-13 13:07:38</t>
+          <t>2025-05-13 11:39:43</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-05-13 13:52:38</t>
+          <t>2025-05-13 12:14:43</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-05-13 13:52:38</t>
+          <t>2025-05-13 12:14:43</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-05-14 10:19:14</t>
+          <t>2025-05-13 13:44:57</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>18928</v>
+        <v>6226</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -5301,18 +5301,18 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M74" t="n">
         <v>70</v>
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O74" t="n">
@@ -5324,41 +5324,41 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>251466</v>
+        <v>251467</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>60</v>
+        <v>38.5</v>
       </c>
       <c r="D75" t="n">
-        <v>80.68115942028986</v>
+        <v>113.2</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-05-13 13:48:14</t>
+          <t>2025-05-13 12:53:42</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-05-13 14:48:14</t>
+          <t>2025-05-13 13:32:12</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-05-13 14:48:14</t>
+          <t>2025-05-13 13:32:12</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-05-14 08:08:55</t>
+          <t>2025-05-14 07:25:24</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>5567</v>
+        <v>6226</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -5371,14 +5371,14 @@
         </is>
       </c>
       <c r="L75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M75" t="n">
         <v>70</v>
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O75" t="n">
@@ -5390,7 +5390,7 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>251463</v>
+        <v>251374</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -5398,33 +5398,33 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D76" t="n">
-        <v>98.12676056338029</v>
+        <v>385.112676056338</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2025-05-14 07:26:52</t>
+          <t>2025-05-13 13:06:34</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-05-14 07:45:52</t>
+          <t>2025-05-13 13:27:34</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2025-05-14 07:45:52</t>
+          <t>2025-05-13 13:27:34</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>2025-05-14 09:24:00</t>
+          <t>2025-05-14 11:52:41</t>
         </is>
       </c>
       <c r="I76" t="n">
-        <v>6967</v>
+        <v>27343</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -5433,18 +5433,18 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L76" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M76" t="n">
         <v>70</v>
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O76" t="n">
@@ -5456,37 +5456,37 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>251464</v>
+        <v>251580</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D77" t="n">
-        <v>145.9795918367347</v>
+        <v>117.2622950819672</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2025-05-14 07:48:30</t>
+          <t>2025-05-13 13:23:39</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-05-14 08:23:30</t>
+          <t>2025-05-13 13:53:39</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>2025-05-14 08:23:30</t>
+          <t>2025-05-13 13:53:39</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>2025-05-14 10:49:29</t>
+          <t>2025-05-14 07:50:55</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -5510,7 +5510,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O77" t="n">
@@ -5522,41 +5522,41 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>251465</v>
+        <v>251557</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D78" t="n">
-        <v>90.23188405797102</v>
+        <v>109.9180327868852</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-05-14 08:08:55</t>
+          <t>2025-05-13 13:43:16</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-05-14 08:38:55</t>
+          <t>2025-05-13 14:23:16</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>2025-05-14 08:38:55</t>
+          <t>2025-05-13 14:23:16</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>2025-05-14 10:09:09</t>
+          <t>2025-05-14 08:13:11</t>
         </is>
       </c>
       <c r="I78" t="n">
-        <v>6226</v>
+        <v>6705</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -5576,7 +5576,7 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O78" t="n">
@@ -5588,41 +5588,41 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>251987</v>
+        <v>251562</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D79" t="n">
-        <v>2965.154929577465</v>
+        <v>118</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2025-05-14 08:30:52</t>
+          <t>2025-05-13 13:44:57</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-05-14 09:04:52</t>
+          <t>2025-05-13 14:09:57</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>2025-05-14 09:04:52</t>
+          <t>2025-05-13 14:09:57</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>2025-05-22 10:30:01</t>
+          <t>2025-05-14 08:07:57</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>210526</v>
+        <v>8142</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -5631,18 +5631,18 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L79" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M79" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O79" t="n">
@@ -5654,41 +5654,41 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>251462</v>
+        <v>251520</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D80" t="n">
-        <v>87.69014084507042</v>
+        <v>230.1408450704225</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2025-05-14 09:24:00</t>
+          <t>2025-05-13 13:53:32</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-05-14 09:43:00</t>
+          <t>2025-05-14 07:13:32</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>2025-05-14 09:43:00</t>
+          <t>2025-05-14 07:13:32</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>2025-05-14 11:10:41</t>
+          <t>2025-05-14 11:03:40</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>6226</v>
+        <v>16340</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -5697,18 +5697,18 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M80" t="n">
         <v>70</v>
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O80" t="n">
@@ -5720,41 +5720,41 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>251467</v>
+        <v>251260</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D81" t="n">
-        <v>90.23188405797102</v>
+        <v>146.390625</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2025-05-14 10:09:09</t>
+          <t>2025-05-14 07:12:16</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-05-14 10:34:09</t>
+          <t>2025-05-14 07:27:16</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2025-05-14 10:34:09</t>
+          <t>2025-05-14 07:27:16</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>2025-05-14 12:04:23</t>
+          <t>2025-05-14 09:53:40</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>6226</v>
+        <v>9369</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -5763,11 +5763,11 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M81" t="n">
         <v>70</v>
@@ -5786,41 +5786,41 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>251520</v>
+        <v>251062</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>80</v>
+        <v>38.5</v>
       </c>
       <c r="D82" t="n">
-        <v>230.1408450704225</v>
+        <v>411.3454545454546</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025-05-14 10:19:14</t>
+          <t>2025-05-14 07:25:24</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-05-14 11:39:14</t>
+          <t>2025-05-14 08:03:54</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>2025-05-14 11:39:14</t>
+          <t>2025-05-14 08:03:54</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>2025-05-15 07:29:22</t>
+          <t>2025-05-14 14:55:15</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>16340</v>
+        <v>22624</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -5829,18 +5829,18 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M82" t="n">
         <v>70</v>
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O82" t="n">
@@ -5852,41 +5852,41 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>251374</v>
+        <v>251750</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="D83" t="n">
-        <v>558.0204081632653</v>
+        <v>54.80281690140845</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-05-14 10:49:29</t>
+          <t>2025-05-14 07:43:14</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-05-14 11:39:29</t>
+          <t>2025-05-14 08:00:14</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>2025-05-14 11:39:29</t>
+          <t>2025-05-14 08:00:14</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>2025-05-15 12:57:30</t>
+          <t>2025-05-14 08:55:02</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>27343</v>
+        <v>3891</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -5895,14 +5895,14 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M83" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="N83" t="inlineStr">
         <is>
@@ -5918,41 +5918,41 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>251580</v>
+        <v>251252</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D84" t="n">
-        <v>100.7464788732394</v>
+        <v>247.2622950819672</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-05-14 11:10:41</t>
+          <t>2025-05-14 07:50:55</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-05-14 11:29:41</t>
+          <t>2025-05-14 08:20:55</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2025-05-14 11:29:41</t>
+          <t>2025-05-14 08:20:55</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>2025-05-14 13:10:26</t>
+          <t>2025-05-14 12:28:10</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>7153</v>
+        <v>15083</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -5961,18 +5961,18 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L84" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M84" t="n">
         <v>70</v>
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O84" t="n">
@@ -5984,41 +5984,41 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>251557</v>
+        <v>251251</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D85" t="n">
-        <v>109.9180327868852</v>
+        <v>229.8550724637681</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-05-14 11:25:38</t>
+          <t>2025-05-14 08:07:57</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-05-14 12:05:38</t>
+          <t>2025-05-14 08:52:57</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2025-05-14 12:05:38</t>
+          <t>2025-05-14 08:52:57</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>2025-05-14 13:55:33</t>
+          <t>2025-05-14 12:42:48</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>6705</v>
+        <v>15860</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -6027,18 +6027,18 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M85" t="n">
         <v>70</v>
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O85" t="n">
@@ -6050,41 +6050,41 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>251562</v>
+        <v>251249</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D86" t="n">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-05-14 12:04:23</t>
+          <t>2025-05-14 08:13:11</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-05-14 12:29:23</t>
+          <t>2025-05-14 08:46:11</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>2025-05-14 12:29:23</t>
+          <t>2025-05-14 08:46:11</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>2025-05-14 14:27:23</t>
+          <t>2025-05-14 10:04:11</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>8142</v>
+        <v>4758</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -6093,18 +6093,18 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L86" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M86" t="n">
         <v>70</v>
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O86" t="n">
@@ -6116,41 +6116,41 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>251062</v>
+        <v>251987</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>30.5</v>
+        <v>36</v>
       </c>
       <c r="D87" t="n">
-        <v>411.3454545454546</v>
+        <v>2965.154929577465</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2025-05-14 13:00:11</t>
+          <t>2025-05-14 08:55:02</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-05-14 13:30:41</t>
+          <t>2025-05-14 09:31:02</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>2025-05-14 13:30:41</t>
+          <t>2025-05-14 09:31:02</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>2025-05-15 12:22:02</t>
+          <t>2025-05-22 10:56:11</t>
         </is>
       </c>
       <c r="I87" t="n">
-        <v>22624</v>
+        <v>210526</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
@@ -6159,18 +6159,18 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L87" t="n">
         <v>6</v>
       </c>
       <c r="M87" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>NESSUN VEICOLO (interno)</t>
+          <t>NESSUN VEICOLO (esterno)</t>
         </is>
       </c>
       <c r="O87" t="n">
@@ -6182,41 +6182,41 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>251252</v>
+        <v>251795</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D88" t="n">
-        <v>212.4366197183099</v>
+        <v>292.796875</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2025-05-14 13:10:26</t>
+          <t>2025-05-14 09:53:40</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-05-14 13:29:26</t>
+          <t>2025-05-14 10:08:40</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>2025-05-14 13:29:26</t>
+          <t>2025-05-14 10:08:40</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>2025-05-15 09:01:52</t>
+          <t>2025-05-15 07:01:28</t>
         </is>
       </c>
       <c r="I88" t="n">
-        <v>15083</v>
+        <v>18739</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L88" t="n">
@@ -6248,41 +6248,41 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>251251</v>
+        <v>245090</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D89" t="n">
-        <v>260</v>
+        <v>8470.786885245901</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2025-05-14 13:55:33</t>
+          <t>2025-05-14 10:04:11</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2025-05-14 14:35:33</t>
+          <t>2025-05-14 10:46:11</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>2025-05-14 14:35:33</t>
+          <t>2025-05-14 10:46:11</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>2025-05-15 10:55:33</t>
+          <t>2025-06-09 07:56:59</t>
         </is>
       </c>
       <c r="I89" t="n">
-        <v>15860</v>
+        <v>516718</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
@@ -6291,14 +6291,14 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M89" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N89" t="inlineStr">
         <is>
@@ -6314,41 +6314,41 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>251249</v>
+        <v>245089</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D90" t="n">
-        <v>68.95652173913044</v>
+        <v>1727.676056338028</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2025-05-14 14:27:23</t>
+          <t>2025-05-14 11:52:41</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2025-05-15 07:12:23</t>
+          <t>2025-05-14 12:28:41</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>2025-05-15 07:12:23</t>
+          <t>2025-05-14 12:28:41</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>2025-05-15 08:21:20</t>
+          <t>2025-05-20 09:16:21</t>
         </is>
       </c>
       <c r="I90" t="n">
-        <v>4758</v>
+        <v>122665</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -6357,14 +6357,14 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L90" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M90" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N90" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Sistemate le ricerche locali per evitare che commesse con veicolo non nelle partenze (i.e. veicolo "tassativi" non nell'estrazione) fossero spostate anche molto in avanti rispetto alla due date
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,6 +575,11 @@
       <c r="P2" t="n">
         <v>39747</v>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>2025-03-13 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -641,6 +646,11 @@
       <c r="P3" t="n">
         <v>39749</v>
       </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2025-04-07 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -707,6 +717,11 @@
       <c r="P4" t="n">
         <v>39746</v>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>2025-05-05 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -773,6 +788,11 @@
       <c r="P5" t="n">
         <v>39747</v>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>2025-04-30 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -839,6 +859,11 @@
       <c r="P6" t="n">
         <v>39762</v>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>2025-05-08 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -905,6 +930,11 @@
       <c r="P7" t="n">
         <v>39666</v>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>2025-04-14 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -971,6 +1001,11 @@
       <c r="P8" t="n">
         <v>39666</v>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>2025-04-24 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1037,6 +1072,11 @@
       <c r="P9" t="n">
         <v>39754</v>
       </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2025-05-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1103,6 +1143,11 @@
       <c r="P10" t="n">
         <v>39760</v>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1169,6 +1214,11 @@
       <c r="P11" t="n">
         <v>39749</v>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>2025-05-02 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1235,6 +1285,11 @@
       <c r="P12" t="n">
         <v>39742</v>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1301,6 +1356,11 @@
       <c r="P13" t="n">
         <v>39749</v>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2025-04-15 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1367,6 +1427,11 @@
       <c r="P14" t="n">
         <v>39749</v>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>2025-04-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1433,6 +1498,11 @@
       <c r="P15" t="n">
         <v>39758</v>
       </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1499,6 +1569,11 @@
       <c r="P16" t="n">
         <v>39749</v>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>2025-05-06 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1565,6 +1640,11 @@
       <c r="P17" t="n">
         <v>39749</v>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>2025-05-06 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1631,6 +1711,11 @@
       <c r="P18" t="n">
         <v>39749</v>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>2025-05-15 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1697,6 +1782,11 @@
       <c r="P19" t="n">
         <v>39749</v>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>2025-04-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1763,6 +1853,11 @@
       <c r="P20" t="n">
         <v>39746</v>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1829,6 +1924,11 @@
       <c r="P21" t="n">
         <v>39749</v>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>2025-04-22 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1895,6 +1995,11 @@
       <c r="P22" t="n">
         <v>39723</v>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>2025-05-15 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1961,6 +2066,11 @@
       <c r="P23" t="n">
         <v>39747</v>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>2025-05-12 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2027,6 +2137,11 @@
       <c r="P24" t="n">
         <v>39747</v>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>2025-04-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2093,6 +2208,11 @@
       <c r="P25" t="n">
         <v>39750</v>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>2025-04-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2159,6 +2279,11 @@
       <c r="P26" t="n">
         <v>39747</v>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>2025-04-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2225,6 +2350,11 @@
       <c r="P27" t="n">
         <v>39764</v>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>2025-05-14 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2289,6 +2419,11 @@
       <c r="P28" t="n">
         <v>0</v>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>2025-05-05 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2353,6 +2488,11 @@
       <c r="P29" t="n">
         <v>0</v>
       </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>2025-05-12 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2417,6 +2557,11 @@
       <c r="P30" t="n">
         <v>0</v>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>2025-04-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2483,6 +2628,11 @@
       <c r="P31" t="n">
         <v>0</v>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>2025-05-07 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2549,6 +2699,11 @@
       <c r="P32" t="n">
         <v>0</v>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>2025-05-07 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2615,6 +2770,11 @@
       <c r="P33" t="n">
         <v>0</v>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>2025-05-07 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2681,6 +2841,11 @@
       <c r="P34" t="n">
         <v>0</v>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>2025-04-30 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2747,6 +2912,11 @@
       <c r="P35" t="n">
         <v>0</v>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>2025-04-30 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2813,6 +2983,11 @@
       <c r="P36" t="n">
         <v>0</v>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>2025-05-05 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2879,6 +3054,11 @@
       <c r="P37" t="n">
         <v>0</v>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>2025-05-30 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2945,6 +3125,11 @@
       <c r="P38" t="n">
         <v>0</v>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>2025-06-10 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -3011,6 +3196,11 @@
       <c r="P39" t="n">
         <v>0</v>
       </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>2025-12-31 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -3077,6 +3267,11 @@
       <c r="P40" t="n">
         <v>0</v>
       </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3143,6 +3338,11 @@
       <c r="P41" t="n">
         <v>0</v>
       </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>2025-12-31 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3209,6 +3409,11 @@
       <c r="P42" t="n">
         <v>0</v>
       </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>2023-11-06 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3275,6 +3480,11 @@
       <c r="P43" t="n">
         <v>0</v>
       </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3341,6 +3551,11 @@
       <c r="P44" t="n">
         <v>0</v>
       </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3407,6 +3622,11 @@
       <c r="P45" t="n">
         <v>0</v>
       </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3473,6 +3693,11 @@
       <c r="P46" t="n">
         <v>0</v>
       </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>2025-04-30 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3539,6 +3764,11 @@
       <c r="P47" t="n">
         <v>0</v>
       </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>2025-05-07 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -3605,6 +3835,11 @@
       <c r="P48" t="n">
         <v>0</v>
       </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>2025-05-08 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3671,6 +3906,11 @@
       <c r="P49" t="n">
         <v>0</v>
       </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>2025-05-08 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3737,6 +3977,11 @@
       <c r="P50" t="n">
         <v>0</v>
       </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>2025-05-08 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3803,6 +4048,11 @@
       <c r="P51" t="n">
         <v>0</v>
       </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>2025-05-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3869,6 +4119,11 @@
       <c r="P52" t="n">
         <v>0</v>
       </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>2025-05-22 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -3935,6 +4190,11 @@
       <c r="P53" t="n">
         <v>0</v>
       </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>2024-09-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -4001,6 +4261,11 @@
       <c r="P54" t="n">
         <v>0</v>
       </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>2025-04-18 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4067,6 +4332,11 @@
       <c r="P55" t="n">
         <v>0</v>
       </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>2025-01-25 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -4133,6 +4403,11 @@
       <c r="P56" t="n">
         <v>0</v>
       </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>2025-04-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -4199,6 +4474,11 @@
       <c r="P57" t="n">
         <v>0</v>
       </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -4265,6 +4545,11 @@
       <c r="P58" t="n">
         <v>0</v>
       </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -4331,6 +4616,11 @@
       <c r="P59" t="n">
         <v>0</v>
       </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>2025-05-05 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -4397,6 +4687,11 @@
       <c r="P60" t="n">
         <v>0</v>
       </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>2025-05-06 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4463,6 +4758,11 @@
       <c r="P61" t="n">
         <v>0</v>
       </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>2024-08-02 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4529,6 +4829,11 @@
       <c r="P62" t="n">
         <v>0</v>
       </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>2025-05-19 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -4595,6 +4900,11 @@
       <c r="P63" t="n">
         <v>0</v>
       </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>2025-04-18 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4661,6 +4971,11 @@
       <c r="P64" t="n">
         <v>0</v>
       </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>2024-09-30 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -4727,6 +5042,11 @@
       <c r="P65" t="n">
         <v>0</v>
       </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>2025-03-18 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4793,6 +5113,11 @@
       <c r="P66" t="n">
         <v>0</v>
       </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>2025-03-28 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -4859,6 +5184,11 @@
       <c r="P67" t="n">
         <v>0</v>
       </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>2025-05-05 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -4925,6 +5255,11 @@
       <c r="P68" t="n">
         <v>0</v>
       </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -4991,6 +5326,11 @@
       <c r="P69" t="n">
         <v>0</v>
       </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -5057,6 +5397,11 @@
       <c r="P70" t="n">
         <v>0</v>
       </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -5123,6 +5468,11 @@
       <c r="P71" t="n">
         <v>0</v>
       </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -5189,6 +5539,11 @@
       <c r="P72" t="n">
         <v>0</v>
       </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -5255,6 +5610,11 @@
       <c r="P73" t="n">
         <v>0</v>
       </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -5321,6 +5681,11 @@
       <c r="P74" t="n">
         <v>0</v>
       </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -5387,6 +5752,11 @@
       <c r="P75" t="n">
         <v>0</v>
       </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -5453,6 +5823,11 @@
       <c r="P76" t="n">
         <v>0</v>
       </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>2025-05-15 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -5519,6 +5894,11 @@
       <c r="P77" t="n">
         <v>0</v>
       </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>2025-05-15 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -5585,6 +5965,11 @@
       <c r="P78" t="n">
         <v>0</v>
       </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>2025-05-15 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -5651,6 +6036,11 @@
       <c r="P79" t="n">
         <v>0</v>
       </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>2025-05-15 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -5717,6 +6107,11 @@
       <c r="P80" t="n">
         <v>0</v>
       </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>2025-05-12 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -5783,6 +6178,11 @@
       <c r="P81" t="n">
         <v>0</v>
       </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>2025-05-22 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -5849,6 +6249,11 @@
       <c r="P82" t="n">
         <v>0</v>
       </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>2025-05-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -5915,6 +6320,11 @@
       <c r="P83" t="n">
         <v>0</v>
       </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>2025-05-26 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -5981,6 +6391,11 @@
       <c r="P84" t="n">
         <v>0</v>
       </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>2025-05-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -6047,6 +6462,11 @@
       <c r="P85" t="n">
         <v>0</v>
       </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>2025-05-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -6113,6 +6533,11 @@
       <c r="P86" t="n">
         <v>0</v>
       </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>2025-06-06 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -6179,6 +6604,11 @@
       <c r="P87" t="n">
         <v>0</v>
       </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>2025-09-01 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -6245,6 +6675,11 @@
       <c r="P88" t="n">
         <v>0</v>
       </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>2025-06-19 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -6311,6 +6746,11 @@
       <c r="P89" t="n">
         <v>0</v>
       </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>2025-12-31 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6376,6 +6816,11 @@
       </c>
       <c r="P90" t="n">
         <v>0</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>2025-12-31 00:00:00</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primo tentativo di implementazione
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[hh]:mm:ss"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,8 +48,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,7 +515,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>250759</v>
+        <v>251455</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -520,10 +523,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>131.21875</v>
+        <v>82.765625</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -532,21 +535,21 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-07 07:34:00</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-07 07:34:00</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-07 09:45:13</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>8398</v>
+        <v>5297</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -555,17 +558,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L2" t="n">
         <v>4</v>
       </c>
       <c r="M2" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N2" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -573,17 +576,20 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
-        </is>
+          <t>2025-04-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>-22.36233723958333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>250923</v>
+        <v>251391</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -594,30 +600,30 @@
         <v>17</v>
       </c>
       <c r="D3" t="n">
-        <v>109.46875</v>
+        <v>91.640625</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-07 09:45:13</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-07 10:02:13</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-07 10:02:13</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-07 11:51:41</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>7006</v>
+        <v>5865</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -626,14 +632,14 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L3" t="n">
         <v>5</v>
       </c>
       <c r="M3" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N3" t="n">
         <v>39749</v>
@@ -648,13 +654,16 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
-        </is>
+          <t>2025-04-23 00:00:00</t>
+        </is>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>-14.43778211805556</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251227</v>
+        <v>251395</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -665,30 +674,30 @@
         <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>35.34375</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-07 11:51:41</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-07 12:08:41</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-07 12:08:41</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-07 12:08:41</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>2262</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -697,17 +706,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M4" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N4" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -715,17 +724,20 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
-        </is>
+          <t>2025-04-23 00:00:00</t>
+        </is>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>-14.47413194444444</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251225</v>
+        <v>251371</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -733,29 +745,29 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-07 12:08:41</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-07 12:23:41</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-07 12:23:41</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-07 12:23:41</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -768,17 +780,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L5" t="n">
         <v>4</v>
       </c>
       <c r="M5" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N5" t="n">
-        <v>39747</v>
+        <v>39666</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -786,17 +798,20 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>39747</v>
+        <v>39666</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
-        </is>
+          <t>2025-04-24 00:00:00</t>
+        </is>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>-13.48732638888889</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251421</v>
+        <v>251453</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -807,30 +822,30 @@
         <v>17</v>
       </c>
       <c r="D6" t="n">
-        <v>81.9375</v>
+        <v>78.125</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-07 12:23:41</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-07 12:40:41</t>
+          <t>2025-05-07 11:58:45</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-07 12:40:41</t>
+          <t>2025-05-07 11:58:45</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-07 14:02:37</t>
+          <t>2025-05-07 13:16:52</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>5244</v>
+        <v>5000</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -839,17 +854,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
         <v>3</v>
       </c>
       <c r="M6" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N6" t="n">
-        <v>39762</v>
+        <v>39742</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -857,17 +872,20 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39762</v>
+        <v>39742</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-08 00:00:00</t>
-        </is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>-9.553385416666666</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251268</v>
+        <v>251396</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -875,33 +893,33 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>35.34375</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-07 14:02:37</t>
+          <t>2025-05-07 13:16:52</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-07 14:19:37</t>
+          <t>2025-05-07 13:37:52</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-07 14:19:37</t>
+          <t>2025-05-07 13:37:52</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-07 14:19:37</t>
+          <t>2025-05-07 14:13:13</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>2262</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -910,17 +928,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M7" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N7" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -928,17 +946,20 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-04-14 00:00:00</t>
-        </is>
+          <t>2025-05-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>-5.592513020833334</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251371</v>
+        <v>251548</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -946,33 +967,33 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>206.90625</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:19:37</t>
+          <t>2025-05-07 14:13:13</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:49:37</t>
+          <t>2025-05-07 14:32:13</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:49:37</t>
+          <t>2025-05-07 14:32:13</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-07 14:49:37</t>
+          <t>2025-05-08 09:59:07</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>13242</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -991,7 +1012,7 @@
         <v>70</v>
       </c>
       <c r="N8" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -999,51 +1020,54 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
-        </is>
+          <t>2025-05-06 00:00:00</t>
+        </is>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>-2.416059027777778</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251782</v>
+        <v>251547</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" t="n">
-        <v>188.640625</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-07 14:49:37</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:21:37</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:21:37</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 10:30:15</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>12073</v>
+        <v>13129</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1052,17 +1076,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N9" t="n">
-        <v>39754</v>
+        <v>39749</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1070,28 +1094,31 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39754</v>
+        <v>39749</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
-        </is>
+          <t>2025-05-06 00:00:00</t>
+        </is>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>-2.443691314548611</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251477</v>
+        <v>251742</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D10" t="n">
-        <v>422.5211267605634</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1100,21 +1127,21 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:17:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 07:17:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 14:19:31</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>29999</v>
+        <v>8226</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1123,17 +1150,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M10" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N10" t="n">
-        <v>39760</v>
+        <v>39749</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1141,28 +1168,31 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39760</v>
+        <v>39749</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
-        </is>
+          <t>2025-05-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251396</v>
+        <v>251268</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D11" t="n">
-        <v>37.08196721311475</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1171,21 +1201,21 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 08:17:04</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>2262</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1194,17 +1224,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M11" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N11" t="n">
-        <v>39749</v>
+        <v>39666</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1212,17 +1242,20 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39749</v>
+        <v>39666</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
-        </is>
+          <t>2025-04-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>-24.32430555555555</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251453</v>
+        <v>251164</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1230,33 +1263,33 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D12" t="n">
-        <v>102.0408163265306</v>
+        <v>204.0816326530612</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-08 07:47:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-08 08:34:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-08 08:34:00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-08 09:22:02</t>
+          <t>2025-05-08 11:58:04</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1269,13 +1302,13 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M12" t="n">
         <v>70</v>
       </c>
       <c r="N12" t="n">
-        <v>39742</v>
+        <v>39749</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1283,17 +1316,20 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39742</v>
+        <v>39749</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
-        </is>
+          <t>2025-04-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>-16.49866780045139</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251455</v>
+        <v>251840</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1301,33 +1337,33 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D13" t="n">
-        <v>86.8360655737705</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 08:17:04</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 08:47:04</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 08:47:04</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-08 10:13:55</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>5297</v>
+        <v>5714</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1340,13 +1376,13 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
       <c r="N13" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1354,51 +1390,54 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
-        </is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251391</v>
+        <v>250923</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D14" t="n">
-        <v>119.6938775510204</v>
+        <v>109.46875</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-08 09:22:02</t>
+          <t>2025-05-08 09:59:07</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-08 10:07:02</t>
+          <t>2025-05-08 10:31:07</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-08 10:07:02</t>
+          <t>2025-05-08 10:31:07</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:06:44</t>
+          <t>2025-05-08 12:20:35</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>5865</v>
+        <v>7006</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1407,14 +1446,14 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
         <v>5</v>
       </c>
       <c r="M14" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N14" t="n">
         <v>39749</v>
@@ -1429,47 +1468,50 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
-        </is>
+          <t>2025-04-07 00:00:00</t>
+        </is>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>-31.51430121527778</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251840</v>
+        <v>250759</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D15" t="n">
-        <v>93.67213114754098</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-08 10:13:55</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:55</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:55</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:12:35</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>5714</v>
+        <v>8398</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1478,17 +1520,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M15" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N15" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1496,51 +1538,54 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
-        </is>
+          <t>2025-03-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="R15" s="1" t="n">
+        <v>-56.54666471048611</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251548</v>
+        <v>251456</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" t="n">
-        <v>206.90625</v>
+        <v>147.5245901639344</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-08 10:30:15</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:15</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:15</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-08 14:29:10</t>
+          <t>2025-05-08 14:41:02</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>13242</v>
+        <v>8999</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1553,13 +1598,13 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
       <c r="N16" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1567,51 +1612,54 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
-        </is>
+          <t>2025-05-09 00:00:00</t>
+        </is>
+      </c>
+      <c r="R16" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251547</v>
+        <v>251477</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D17" t="n">
-        <v>267.9387755102041</v>
+        <v>422.5211267605634</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:06:44</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:46:44</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:46:44</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-09 09:14:40</t>
+          <t>2025-05-09 11:19:31</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>13129</v>
+        <v>29999</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1620,17 +1668,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M17" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N17" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1638,32 +1686,35 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
-        </is>
+          <t>2025-04-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="R17" s="1" t="n">
+        <v>-11.47188967136574</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251742</v>
+        <v>251225</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>134.8524590163935</v>
+        <v>0</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:12:35</t>
+          <t>2025-05-08 12:20:35</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1678,11 +1729,11 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-08 14:52:26</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>8226</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1691,17 +1742,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L18" t="n">
         <v>4</v>
       </c>
       <c r="M18" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N18" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1709,51 +1760,54 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
-        </is>
+          <t>2025-04-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="R18" s="1" t="n">
+        <v>-8.526106770833334</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251395</v>
+        <v>251227</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D19" t="n">
-        <v>31.85915492957746</v>
+        <v>0</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-08 14:19:31</t>
+          <t>2025-05-08 12:37:35</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-08 14:55:31</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-08 14:55:31</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-09 07:27:22</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>2262</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1762,17 +1816,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M19" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N19" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1780,17 +1834,20 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
-        </is>
+          <t>2025-05-05 00:00:00</t>
+        </is>
+      </c>
+      <c r="R19" s="1" t="n">
+        <v>-3.5365234375</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251456</v>
+        <v>251421</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1801,30 +1858,30 @@
         <v>17</v>
       </c>
       <c r="D20" t="n">
-        <v>140.609375</v>
+        <v>81.9375</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-08 14:29:10</t>
+          <t>2025-05-08 12:52:35</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:10</t>
+          <t>2025-05-08 13:09:35</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-08 14:46:10</t>
+          <t>2025-05-08 13:09:35</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-09 09:06:46</t>
+          <t>2025-05-08 14:31:31</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>8999</v>
+        <v>5244</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1833,17 +1890,17 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L20" t="n">
         <v>3</v>
       </c>
       <c r="M20" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N20" t="n">
-        <v>39746</v>
+        <v>39762</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1851,51 +1908,54 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>39746</v>
+        <v>39762</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
-        </is>
+          <t>2025-05-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="R20" s="1" t="n">
+        <v>-0.6052300347222223</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251164</v>
+        <v>251229</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D21" t="n">
-        <v>163.9344262295082</v>
+        <v>263.9295774647887</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-08 14:52:26</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-09 07:22:26</t>
+          <t>2025-05-08 13:41:11</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-09 07:22:26</t>
+          <t>2025-05-08 13:41:11</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-09 10:06:22</t>
+          <t>2025-05-09 10:05:07</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>10000</v>
+        <v>18739</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1904,7 +1964,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
@@ -1914,7 +1974,7 @@
         <v>70</v>
       </c>
       <c r="N21" t="n">
-        <v>39749</v>
+        <v>39723</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1922,51 +1982,54 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>39749</v>
+        <v>39723</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
-        </is>
+          <t>2025-05-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="R21" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251229</v>
+        <v>251782</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="D22" t="n">
-        <v>307.1967213114754</v>
+        <v>188.640625</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 14:31:31</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-09 07:46:00</t>
+          <t>2025-05-08 14:46:31</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-09 07:46:00</t>
+          <t>2025-05-08 14:46:31</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-09 12:53:11</t>
+          <t>2025-05-09 09:55:10</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>18739</v>
+        <v>12073</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1975,17 +2038,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M22" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N22" t="n">
-        <v>39723</v>
+        <v>39754</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -1993,12 +2056,15 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39723</v>
+        <v>39754</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
-        </is>
+          <t>2025-05-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="R22" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2071,6 +2137,9 @@
           <t>2025-05-12 00:00:00</t>
         </is>
       </c>
+      <c r="R23" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2142,10 +2211,13 @@
           <t>2025-04-16 00:00:00</t>
         </is>
       </c>
+      <c r="R24" s="1" t="n">
+        <v>-23.44236111111111</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251081</v>
+        <v>251054</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2153,10 +2225,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>125</v>
+        <v>35</v>
       </c>
       <c r="D25" t="n">
-        <v>42.42253521126761</v>
+        <v>0</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -2165,21 +2237,21 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-09 12:42:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-09 12:42:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-09 13:24:25</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>3012</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2192,13 +2264,13 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="M25" t="n">
         <v>70</v>
       </c>
       <c r="N25" t="n">
-        <v>39750</v>
+        <v>39747</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2206,17 +2278,20 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>39750</v>
+        <v>39747</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
-        </is>
+          <t>2025-04-16 00:00:00</t>
+        </is>
+      </c>
+      <c r="R25" s="1" t="n">
+        <v>-23.46666666666667</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251054</v>
+        <v>251081</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2227,30 +2302,30 @@
         <v>125</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:24:25</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-12 07:29:25</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-12 07:29:25</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-12 07:29:25</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>3012</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2263,13 +2338,13 @@
         </is>
       </c>
       <c r="L26" t="n">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M26" t="n">
         <v>70</v>
       </c>
       <c r="N26" t="n">
-        <v>39747</v>
+        <v>39750</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2277,12 +2352,15 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>39747</v>
+        <v>39750</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
-        </is>
+          <t>2025-04-23 00:00:00</t>
+        </is>
+      </c>
+      <c r="R26" s="1" t="n">
+        <v>-16.58293231612268</v>
       </c>
     </row>
     <row r="27">
@@ -2355,6 +2433,9 @@
           <t>2025-05-14 00:00:00</t>
         </is>
       </c>
+      <c r="R27" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2362,33 +2443,33 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D28" t="n">
-        <v>623.4084507042254</v>
+        <v>903.3061224489796</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 11:58:04</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:00</t>
+          <t>2025-05-08 12:40:04</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:00</t>
+          <t>2025-05-08 12:40:04</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-09 14:44:24</t>
+          <t>2025-05-12 11:43:23</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2424,44 +2505,47 @@
           <t>2025-05-05 00:00:00</t>
         </is>
       </c>
+      <c r="R28" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251651</v>
+        <v>251416</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D29" t="n">
-        <v>659.5774647887324</v>
+        <v>183.9672131147541</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:27:22</t>
+          <t>2025-05-08 14:41:02</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:59:22</t>
+          <t>2025-05-09 07:06:02</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-09 07:59:22</t>
+          <t>2025-05-09 07:06:02</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-12 10:58:57</t>
+          <t>2025-05-09 10:10:00</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>46830</v>
+        <v>11222</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2470,14 +2554,14 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M29" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N29" t="n">
         <v>39755</v>
@@ -2490,47 +2574,50 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
-        </is>
+          <t>2025-04-23 00:00:00</t>
+        </is>
+      </c>
+      <c r="R29" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251416</v>
+        <v>251651</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D30" t="n">
-        <v>175.34375</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-09 09:06:46</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-09 09:23:46</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-09 09:23:46</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-09 12:19:07</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>11222</v>
+        <v>46830</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2539,14 +2626,14 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L30" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M30" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N30" t="n">
         <v>39755</v>
@@ -2559,8 +2646,11 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
-        </is>
+          <t>2025-05-12 00:00:00</t>
+        </is>
+      </c>
+      <c r="R30" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rimane da sistemare la ricercal ocale; c'è qualche problema con il calcolo dei check per le ricerche locali che escludono casi di ovvia problematicità (i.e. aumentano il ritardo)
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-22.36233723958333</v>
+        <v>-0.3623372395833334</v>
       </c>
     </row>
     <row r="3">
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-14.43778211805556</v>
+        <v>-0.4377821180555556</v>
       </c>
     </row>
     <row r="4">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-14.47413194444444</v>
+        <v>-0.4741319444444445</v>
       </c>
     </row>
     <row r="5">
@@ -789,8 +789,10 @@
       <c r="M5" t="n">
         <v>70</v>
       </c>
-      <c r="N5" t="n">
-        <v>39666</v>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>39666 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -863,8 +865,10 @@
       <c r="M6" t="n">
         <v>70</v>
       </c>
-      <c r="N6" t="n">
-        <v>39742</v>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>39742 (esterno)</t>
+        </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -880,7 +884,7 @@
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-9.553385416666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -954,7 +958,7 @@
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-5.592513020833334</v>
+        <v>-0.5925130208333333</v>
       </c>
     </row>
     <row r="8">
@@ -1028,7 +1032,7 @@
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-2.416059027777778</v>
+        <v>-1.416059027777778</v>
       </c>
     </row>
     <row r="9">
@@ -1102,7 +1106,7 @@
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-2.443691314548611</v>
+        <v>-1.443691314548611</v>
       </c>
     </row>
     <row r="10">
@@ -1176,7 +1180,7 @@
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>0</v>
+        <v>-1.406147540983796</v>
       </c>
     </row>
     <row r="11">
@@ -1233,8 +1237,10 @@
       <c r="M11" t="n">
         <v>76</v>
       </c>
-      <c r="N11" t="n">
-        <v>39666</v>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1250,7 +1256,7 @@
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-24.32430555555555</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1324,7 +1330,7 @@
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-16.49866780045139</v>
+        <v>-1.498667800451389</v>
       </c>
     </row>
     <row r="13">
@@ -1398,7 +1404,7 @@
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>0</v>
+        <v>-0.4885587431712963</v>
       </c>
     </row>
     <row r="14">
@@ -1472,7 +1478,7 @@
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-31.51430121527778</v>
+        <v>-1.514301215277778</v>
       </c>
     </row>
     <row r="15">
@@ -1546,7 +1552,7 @@
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-56.54666471048611</v>
+        <v>-0.5466647104861111</v>
       </c>
     </row>
     <row r="16">
@@ -1620,7 +1626,7 @@
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>0</v>
+        <v>-2.611839708564815</v>
       </c>
     </row>
     <row r="17">
@@ -1694,7 +1700,7 @@
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-11.47188967136574</v>
+        <v>-2.471889671365741</v>
       </c>
     </row>
     <row r="18">
@@ -1768,7 +1774,7 @@
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-8.526106770833334</v>
+        <v>-0.5261067708333333</v>
       </c>
     </row>
     <row r="19">
@@ -1842,7 +1848,7 @@
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-3.5365234375</v>
+        <v>-2.5365234375</v>
       </c>
     </row>
     <row r="20">
@@ -1899,8 +1905,10 @@
       <c r="M20" t="n">
         <v>76</v>
       </c>
-      <c r="N20" t="n">
-        <v>39762</v>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>39762 (esterno)</t>
+        </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1916,7 +1924,7 @@
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-0.6052300347222223</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1973,8 +1981,10 @@
       <c r="M21" t="n">
         <v>70</v>
       </c>
-      <c r="N21" t="n">
-        <v>39723</v>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>39723 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2064,7 +2074,7 @@
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>0</v>
+        <v>-0.4133138020833333</v>
       </c>
     </row>
     <row r="23">
@@ -2138,7 +2148,7 @@
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>0</v>
+        <v>-1.526104797974537</v>
       </c>
     </row>
     <row r="24">
@@ -2212,7 +2222,7 @@
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-23.44236111111111</v>
+        <v>-1.442361111111111</v>
       </c>
     </row>
     <row r="25">
@@ -2286,7 +2296,7 @@
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-23.46666666666667</v>
+        <v>-1.466666666666667</v>
       </c>
     </row>
     <row r="26">
@@ -2343,8 +2353,10 @@
       <c r="M26" t="n">
         <v>70</v>
       </c>
-      <c r="N26" t="n">
-        <v>39750</v>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>39750 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2417,8 +2429,10 @@
       <c r="M27" t="n">
         <v>0</v>
       </c>
-      <c r="N27" t="n">
-        <v>39764</v>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>39764 (non in estrazione)</t>
+        </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Risolto (teoricamente) il problema delle ricerce locali: era posto check=True a inizio funzione quindi tutte le volte bastava che l'elemento di schedula finale fosse "True" e veniva validata la mossa nella sua interezza
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -791,7 +791,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>39666 (non in estrazione)</t>
+          <t>39666 (esterno)</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -867,7 +867,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>39742 (esterno)</t>
+          <t>39742 (non in estrazione)</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>39666 (esterno)</t>
+          <t>39666 (non in estrazione)</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>39762 (esterno)</t>
+          <t>39762 (non in estrazione)</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>39723 (non in estrazione)</t>
+          <t>39723 (esterno)</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>39750 (non in estrazione)</t>
+          <t>39750 (esterno)</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>39764 (non in estrazione)</t>
+          <t>39764 (esterno)</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">

</xml_diff>

<commit_message>
Cambiato come si gestiscono le commesse tassative interne a veicolo non in estrazione e la graficazione
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
+++ b/PS-VRP/OUTPUT_TEST/euristico_costruttivo.xlsx
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>0</v>
+        <v>-9.553385416666666</v>
       </c>
     </row>
     <row r="7">
@@ -1256,7 +1256,7 @@
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>0</v>
+        <v>-24.32430555555555</v>
       </c>
     </row>
     <row r="12">
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>0</v>
+        <v>-0.6052300347222223</v>
       </c>
     </row>
     <row r="21">

</xml_diff>